<commit_message>
New File PP Regression4
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_Inputs.xlsx
+++ b/UploadExcel/TD_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E339ED0C-4D26-470E-A14E-FFB08A78AC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF38F44-339B-4399-92F8-0DD0A259C22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alipay" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="326">
   <si>
     <t>CancellationFlag</t>
   </si>
@@ -508,40 +508,112 @@
     <t>\UploadExcel\JsonTemplates\CreditCardNewCustomer.json</t>
   </si>
   <si>
+    <t>20240702112604</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f41281569</t>
+  </si>
+  <si>
+    <t>20240702112604Test</t>
+  </si>
+  <si>
+    <t>20240702112604Auto</t>
+  </si>
+  <si>
+    <t>20240702112604@Wiley.com</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e111a</t>
+  </si>
+  <si>
+    <t>e0c5210c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213165 for AS order 20240702112604</t>
+  </si>
+  <si>
+    <t>3213165</t>
+  </si>
+  <si>
+    <t>0000000135548858</t>
+  </si>
+  <si>
+    <t>0000000135550648</t>
+  </si>
+  <si>
+    <t>0000000135545948</t>
+  </si>
+  <si>
+    <t>20240701164345</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f29527164</t>
+  </si>
+  <si>
+    <t>20240701162813Test</t>
+  </si>
+  <si>
+    <t>20240701162813Auto</t>
+  </si>
+  <si>
+    <t>20240701162813@Wiley.com</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e352a</t>
+  </si>
+  <si>
+    <t>e0c2155c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213146 for AS order 20240701164345</t>
+  </si>
+  <si>
+    <t>3213146</t>
+  </si>
+  <si>
+    <t>0000000135545558</t>
+  </si>
+  <si>
+    <t>0000000135548831</t>
+  </si>
+  <si>
+    <t>0000000135545561</t>
+  </si>
+  <si>
     <t>Alipay_CN</t>
   </si>
   <si>
-    <t>20240514120817</t>
-  </si>
-  <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f51469381</t>
-  </si>
-  <si>
-    <t>20240514120817Test</t>
-  </si>
-  <si>
-    <t>20240514120817Auto</t>
-  </si>
-  <si>
-    <t>20240514120817@Wiley.com</t>
-  </si>
-  <si>
-    <t>df1e950b-a1d7-45bf-acab-42f7ed3e282a</t>
-  </si>
-  <si>
-    <t>e0c6155c-ba2c-401d-b2a6-3fb3a59b3c00</t>
-  </si>
-  <si>
-    <t>Created Viax order 3211968 for AS order 20240514120817</t>
-  </si>
-  <si>
-    <t>3211968</t>
-  </si>
-  <si>
-    <t>0000000135364759</t>
-  </si>
-  <si>
-    <t>0000000135363232</t>
+    <t>20240701164842</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f37815148</t>
+  </si>
+  <si>
+    <t>20240701164842Test</t>
+  </si>
+  <si>
+    <t>20240701164842Auto</t>
+  </si>
+  <si>
+    <t>20240701164842@Wiley.com</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e874a</t>
+  </si>
+  <si>
+    <t>e0c1685c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213147 for AS order 20240701164842</t>
+  </si>
+  <si>
+    <t>3213147</t>
+  </si>
+  <si>
+    <t>0000000135552204</t>
+  </si>
+  <si>
+    <t>0000000135545565</t>
   </si>
   <si>
     <t>Issue In Idoc or No Idoc Found</t>
@@ -550,25 +622,79 @@
     <t>AlipayExisting_CN</t>
   </si>
   <si>
-    <t>20240514122419</t>
-  </si>
-  <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f72455517</t>
-  </si>
-  <si>
-    <t>df1e950b-a1d7-45bf-acab-42f7ed3e844a</t>
-  </si>
-  <si>
-    <t>e0c6325c-ba2c-401d-b2a6-3fb3a59b3c00</t>
-  </si>
-  <si>
-    <t>Created Viax order 3211969 for AS order 20240514122419</t>
-  </si>
-  <si>
-    <t>3211969</t>
-  </si>
-  <si>
-    <t>0000000135365558</t>
+    <t>20240701170549</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f40230129</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e599a</t>
+  </si>
+  <si>
+    <t>e0c2579c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213151 for AS order 20240701170549</t>
+  </si>
+  <si>
+    <t>0000000135550525</t>
+  </si>
+  <si>
+    <t>20240701171741</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f87863139</t>
+  </si>
+  <si>
+    <t>20240701171741Test</t>
+  </si>
+  <si>
+    <t>20240701171741Auto</t>
+  </si>
+  <si>
+    <t>20240701171741@Wiley.com</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e205a</t>
+  </si>
+  <si>
+    <t>e0c4172c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213152 for AS order 20240701171741</t>
+  </si>
+  <si>
+    <t>3213152</t>
+  </si>
+  <si>
+    <t>0000000135545585</t>
+  </si>
+  <si>
+    <t>0000000135545584</t>
+  </si>
+  <si>
+    <t>0000000135545586</t>
+  </si>
+  <si>
+    <t>20240701173354</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f11482632</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e140a</t>
+  </si>
+  <si>
+    <t>e0c6549c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213153 for AS order 20240701173354</t>
+  </si>
+  <si>
+    <t>3213153</t>
+  </si>
+  <si>
+    <t>0000000135552217</t>
   </si>
   <si>
     <t>VIAXEnvironment</t>
@@ -601,10 +727,7 @@
     <t>c597beef-e45f-4cc7-b34c-0df812e2ef25</t>
   </si>
   <si>
-    <t>Created Viax order 7231439 for PriceProposal 24ef5270-783b-4808-9127-af8e42410676</t>
-  </si>
-  <si>
-    <t>7231439</t>
+    <t>Created Viax order 7236048 for PriceProposal 24ef6375-783b-4808-9127-af8e42410759</t>
   </si>
   <si>
     <t>PriceDetermined</t>
@@ -618,7 +741,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef5270-783b-4808-9127-af8e42410676",
+      "submissionId": "24ef6375-783b-4808-9127-af8e42410759",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -674,7 +797,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231439 for PriceProposal 24ef5270-783b-4808-9127-af8e42410676\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231439\",\"priceProposal\":{\"uid\":\"66782ffb-78f0-4209-bf0c-6fa63a8fd7fe\",\"biId\":\"7231439\",\"wAsSubmissionId\":\"24ef5270-783b-4808-9127-af8e42410676\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:23:55.979Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d12-8c68-fe0b8c46172a\",\"submissionId\":\"24ef5270-783b-4808-9127-af8e42410676\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"Research Article\",\"displayArticleType\":\"Research Article (ABC)\",\"submissionDate\":\"2024-04-15\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[\"JCASP\"],\"promoCodes\":[],\"discountCodes\":[],\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"US\",\"country\":\"US\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[{\"discountCode\":\"JCASP\",\"discountType\":\"Society\",\"discountAmount\":10,\"discountPercentage\":5,\"discountDescription\":\"BULK LOAD EQ2 - QA ON 12/19/2023\",\"sapDiscountTableCode\":\"ZSP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":false,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"JCASP\",\"attribute\":\"wAsSelectedSocietyPercentageDiscountCode\"}]}],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:23:56.491Z\"}},\"wAsCountryCode\":\"US\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":800,\"price\":200,\"subtotal\":190,\"tax\":0,\"total\":190,\"discountAmount\":10,\"discountPercentage\":5,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"JCASP\",\"discountType\":\"Society\",\"discountAmount\":10,\"discountPercentage\":5,\"discountDescription\":\"BULK LOAD EQ2 - QA ON 12/19/2023\",\"sapDiscountTableCode\":\"ZSP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"JCASP\",\"attribute\":\"wAsSelectedSocietyPercentageDiscountCode\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]},{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"RESEARCH ARTICLE\",\"attribute\":\"wAsBaseArticleType\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]}],\"appliedDiscounts\":[{\"discountCode\":\"JCASP\",\"discountType\":\"Society\",\"discountAmount\":10,\"discountPercentage\":5,\"discountDescription\":\"BULK LOAD EQ2 - QA ON 12/19/2023\",\"sapDiscountTableCode\":\"ZSP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null},{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"US\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef5270-783b-4808-9127-af8e42410676\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef5270-783b-4808-9127-af8e42410676\",\"wAsSubmissionDate\":\"2024-04-15\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"Research Article\",\"wAsDisplayArticleType\":\"Research Article (ABC)\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236048 for PriceProposal 24ef6375-783b-4808-9127-af8e42410759","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236048","priceProposal":{"uid":"6683cf65-573c-43d8-8366-e7429cbbd385","biId":"7236048","wAsSubmissionId":"24ef6375-783b-4808-9127-af8e42410759","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:01.653Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6375-783b-4808-9127-af8e42410759","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:02.178Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6375-783b-4808-9127-af8e42410759","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef6375-783b-4808-9127-af8e42410759","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Promotional discount</t>
@@ -683,10 +806,10 @@
     <t>Promotional</t>
   </si>
   <si>
-    <t>Created Viax order 7231440 for PriceProposal 24ef4777-783b-4808-9127-af8e42410226</t>
-  </si>
-  <si>
-    <t>7231440</t>
+    <t>Created Viax order 7236049 for PriceProposal 24ef5688-783b-4808-9127-af8e42410761</t>
+  </si>
+  <si>
+    <t>7236049</t>
   </si>
   <si>
     <t>{
@@ -694,7 +817,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef4777-783b-4808-9127-af8e42410226",
+      "submissionId": "24ef5688-783b-4808-9127-af8e42410761",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -750,19 +873,19 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231440 for PriceProposal 24ef4777-783b-4808-9127-af8e42410226\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231440\",\"priceProposal\":{\"uid\":\"66782ffd-7a1f-4cc4-bf67-b493ca5a8027\",\"biId\":\"7231440\",\"wAsSubmissionId\":\"24ef4777-783b-4808-9127-af8e42410226\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:23:57.601Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d12-8c68-fe0b8c46172a\",\"submissionId\":\"24ef4777-783b-4808-9127-af8e42410226\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"Research Article\",\"displayArticleType\":\"Research Article (ABC)\",\"submissionDate\":\"2024-04-15\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[],\"promoCodes\":[\"PROMO50\"],\"discountCodes\":[],\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"US\",\"country\":\"US\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[{\"discountCode\":\"PROMO50\",\"discountType\":\"WileyPromoCode\",\"discountAmount\":40,\"discountPercentage\":20,\"discountDescription\":\"UPDATED VALID TO DATE\",\"sapDiscountTableCode\":\"ZPP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":false,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"PROMO50\",\"attribute\":\"wAsSelectedPromotionPercentageDiscountCode\"}]}],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:23:58.056Z\"}},\"wAsCountryCode\":\"US\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":800,\"price\":200,\"subtotal\":160,\"tax\":0,\"total\":160,\"discountAmount\":40,\"discountPercentage\":20,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"RESEARCH ARTICLE\",\"attribute\":\"wAsBaseArticleType\"}]},{\"discountCode\":\"PROMO50\",\"discountType\":\"WileyPromoCode\",\"discountAmount\":40,\"discountPercentage\":20,\"discountDescription\":\"UPDATED VALID TO DATE\",\"sapDiscountTableCode\":\"ZPP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"PROMO50\",\"attribute\":\"wAsSelectedPromotionPercentageDiscountCode\"}]}],\"appliedDiscounts\":[{\"discountCode\":\"PROMO50\",\"discountType\":\"WileyPromoCode\",\"discountAmount\":40,\"discountPercentage\":20,\"discountDescription\":\"UPDATED VALID TO DATE\",\"sapDiscountTableCode\":\"ZPP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null},{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"US\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef4777-783b-4808-9127-af8e42410226\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef4777-783b-4808-9127-af8e42410226\",\"wAsSubmissionDate\":\"2024-04-15\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"Research Article\",\"wAsDisplayArticleType\":\"Research Article (ABC)\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
-  </si>
-  <si>
-    <t>Create PP with Institutional  discount(%)</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236049 for PriceProposal 24ef5688-783b-4808-9127-af8e42410761","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236049","priceProposal":{"uid":"6683cf69-f057-44e3-b4ca-a517a48adb51","biId":"7236049","wAsSubmissionId":"24ef5688-783b-4808-9127-af8e42410761","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:05.710Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef5688-783b-4808-9127-af8e42410761","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:06.140Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5688-783b-4808-9127-af8e42410761","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef5688-783b-4808-9127-af8e42410761","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+  </si>
+  <si>
+    <t>Create PP with Institutional discount</t>
   </si>
   <si>
     <t>Institutional</t>
   </si>
   <si>
-    <t>Created Viax order 7231441 for PriceProposal 24ef2921-783b-4808-9127-af8e42410459</t>
-  </si>
-  <si>
-    <t>7231441</t>
+    <t>Created Viax order 7236050 for PriceProposal 24ef1093-783b-4808-9127-af8e42410467</t>
+  </si>
+  <si>
+    <t>7236050</t>
   </si>
   <si>
     <t>{
@@ -770,7 +893,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef2921-783b-4808-9127-af8e42410459",
+      "submissionId": "24ef1093-783b-4808-9127-af8e42410467",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -824,7 +947,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231441 for PriceProposal 24ef2921-783b-4808-9127-af8e42410459\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231441\",\"priceProposal\":{\"uid\":\"66782fff-c211-49f9-9e6c-fbbc77c4e502\",\"biId\":\"7231441\",\"wAsSubmissionId\":\"24ef2921-783b-4808-9127-af8e42410459\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:23:59.077Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d02-8c68-fe0b8c46172a\",\"submissionId\":\"24ef2921-783b-4808-9127-af8e42410459\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"Research Article\",\"displayArticleType\":\"Research Article (ABC)\",\"submissionDate\":\"2024-04-16\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[],\"promoCodes\":[],\"discountCodes\":[],\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"1666\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"US\",\"country\":\"US\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:23:59.733Z\"}},\"wAsCountryCode\":\"US\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":{\"institutionId\":\"1666\",\"institutionName\":\"E O LAWRENCE BERKELEY NATIONAL LABORATORY\",\"institutionIdType\":\"Ringgold\",\"woaCode\":null,\"consortiumCode\":\"CDL\"},\"prices\":[{\"basePrice\":800,\"price\":200,\"subtotal\":0,\"tax\":0,\"total\":0,\"discountAmount\":200,\"discountPercentage\":100,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"E O LAWRENCE BERKELEY NATIONAL LABORATORY\",\"discountType\":\"Institutional\",\"discountAmount\":200,\"discountPercentage\":100,\"discountDescription\":\"Institutional Discounts Group\",\"sapDiscountTableCode\":\"ZIV1\",\"isPercentageDiscount\":false,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[]},{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"RESEARCH ARTICLE\",\"attribute\":\"wAsBaseArticleType\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]}],\"appliedDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null},{\"discountCode\":\"E O LAWRENCE BERKELEY NATIONAL LABORATORY\",\"discountType\":\"Institutional\",\"discountAmount\":200,\"discountPercentage\":100,\"discountDescription\":\"Institutional Discounts Group\",\"sapDiscountTableCode\":\"ZIV1\",\"isPercentageDiscount\":false,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"1666\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"US\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef2921-783b-4808-9127-af8e42410459\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef2921-783b-4808-9127-af8e42410459\",\"wAsSubmissionDate\":\"2024-04-16\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"Research Article\",\"wAsDisplayArticleType\":\"Research Article (ABC)\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236050 for PriceProposal 24ef1093-783b-4808-9127-af8e42410467","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236050","priceProposal":{"uid":"6683cf73-b182-4a96-a00b-becc0dcb413f","biId":"7236050","wAsSubmissionId":"24ef1093-783b-4808-9127-af8e42410467","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:15.755Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef1093-783b-4808-9127-af8e42410467","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-16","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:16.318Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":800,"price":200,"subtotal":0,"tax":0,"total":0,"discountAmount":200,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef1093-783b-4808-9127-af8e42410467","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef1093-783b-4808-9127-af8e42410467","wAsSubmissionDate":"2024-04-16","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Editorial discount</t>
@@ -833,10 +956,10 @@
     <t>Editorial</t>
   </si>
   <si>
-    <t>Created Viax order 7231442 for PriceProposal 24ef6959-783b-4808-9127-af8e42410944</t>
-  </si>
-  <si>
-    <t>7231442</t>
+    <t>Created Viax order 7236051 for PriceProposal 24ef8267-783b-4808-9127-af8e42410133</t>
+  </si>
+  <si>
+    <t>7236051</t>
   </si>
   <si>
     <t>{
@@ -844,7 +967,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef6959-783b-4808-9127-af8e42410944",
+      "submissionId": "24ef8267-783b-4808-9127-af8e42410133",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -899,7 +1022,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231442 for PriceProposal 24ef6959-783b-4808-9127-af8e42410944\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231442\",\"priceProposal\":{\"uid\":\"66783000-d7a6-4404-b8b4-acb936e8866e\",\"biId\":\"7231442\",\"wAsSubmissionId\":\"24ef6959-783b-4808-9127-af8e42410944\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:24:00.759Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d02-8c68-fe0b8c46172a\",\"submissionId\":\"24ef6959-783b-4808-9127-af8e42410944\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"OPINION\",\"displayArticleType\":\"OPINION\",\"submissionDate\":\"2024-03-21\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[],\"promoCodes\":[],\"discountCodes\":[],\"editorialDiscountCode\":\"CCCAM424\",\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"MH\",\"country\":\"MH\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:01.229Z\"}},\"wAsCountryCode\":\"MH\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":800,\"price\":640,\"subtotal\":0,\"tax\":0,\"total\":0,\"discountAmount\":640,\"discountPercentage\":100,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":160,\"discountPercentage\":20,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"OPINION\",\"attribute\":\"wAsBaseArticleType\"}]},{\"discountCode\":\"CCCAM424\",\"discountType\":\"EditorialDiscount\",\"discountAmount\":576,\"discountPercentage\":90,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZEPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"CCCAM424\",\"attribute\":\"wAsEditorialDiscountCode\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]},{\"discountCode\":\"\",\"discountType\":\"GeographicalDiscount\",\"discountAmount\":640,\"discountPercentage\":100,\"discountDescription\":\"\",\"sapDiscountTableCode\":\"ZGPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"MH\",\"attribute\":\"wAsCountryCode\"}]}],\"appliedDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":160,\"discountPercentage\":20,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null},{\"discountCode\":\"\",\"discountType\":\"GeographicalDiscount\",\"discountAmount\":640,\"discountPercentage\":100,\"discountDescription\":\"\",\"sapDiscountTableCode\":\"ZGPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"MH\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":\"CCCAM424\",\"biiSalable\":{\"maId\":\"24ef6959-783b-4808-9127-af8e42410944\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef6959-783b-4808-9127-af8e42410944\",\"wAsSubmissionDate\":\"2024-03-21\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"OPINION\",\"wAsDisplayArticleType\":\"OPINION\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236051 for PriceProposal 24ef8267-783b-4808-9127-af8e42410133","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236051","priceProposal":{"uid":"6683cf79-051a-43f3-8398-c576c15bd46b","biId":"7236051","wAsSubmissionId":"24ef8267-783b-4808-9127-af8e42410133","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:21.179Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef8267-783b-4808-9127-af8e42410133","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"OPINION","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"CCCAM424","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"MH","country":"MH","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:22.352Z"}},"wAsCountryCode":"MH","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":640,"subtotal":0,"tax":0,"total":0,"discountAmount":640,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":576,"discountPercentage":90,"discountDescription":null,"sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":640,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"MH","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":640,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"MH","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef8267-783b-4808-9127-af8e42410133","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef8267-783b-4808-9127-af8e42410133","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"OPINION","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Referral discount</t>
@@ -911,10 +1034,10 @@
     <t>1b28a8b9-067b-4ce9-b981-e8eabe16e0a7</t>
   </si>
   <si>
-    <t>Created Viax order 7231443 for PriceProposal 24ef4438-783b-4808-9127-af8e42410900</t>
-  </si>
-  <si>
-    <t>7231443</t>
+    <t>Created Viax order 7236052 for PriceProposal 24ef1284-783b-4808-9127-af8e42410880</t>
+  </si>
+  <si>
+    <t>7236052</t>
   </si>
   <si>
     <t>{
@@ -922,7 +1045,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef4438-783b-4808-9127-af8e42410900",
+      "submissionId": "24ef1284-783b-4808-9127-af8e42410880",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "1b28a8b9-067b-4ce9-b981-e8eabe16e0a7",
@@ -977,7 +1100,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231443 for PriceProposal 24ef4438-783b-4808-9127-af8e42410900\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231443\",\"priceProposal\":{\"uid\":\"66783002-1638-4120-b341-baaee7538d3d\",\"biId\":\"7231443\",\"wAsSubmissionId\":\"24ef4438-783b-4808-9127-af8e42410900\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:24:02.314Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d02-8c68-fe0b8c46172a\",\"submissionId\":\"24ef4438-783b-4808-9127-af8e42410900\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"Research Article\",\"displayArticleType\":\"Research Article (ABC)\",\"submissionDate\":\"2024-04-15\",\"articleAcceptedDate\":\"2024-02-10\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"Have a goood day(*&amp;^%$#.\",\"societyCodes\":[],\"promoCodes\":[],\"discountCodes\":[],\"referringJournalId\":\"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\",\"authors\":[{\"role\":\"CorrespondingAuthor\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"anagarajan@wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"AixenProvence\",\"countryCode\":\"IN\",\"country\":\"IN\",\"institution\":\"GrantInstitute\",\"department\":\"SchoolofGeoSciences\",\"stateProvince\":\"AndhraPradesh\",\"postalCode\":\"500072\",\"streetAddress\":[\"1832ColvinAve\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:02.692Z\"}},\"wAsCountryCode\":\"IN\",\"wAsReferringJournal\":\"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\",\"wAsReferringJournalRef\":{\"maId\":\"AND\",\"maName\":\"Andrologia\",\"wAsJournalUuid\":\"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalStatus\":\"Yes\",\"wAsJournalTitle\":\"Andrologia\",\"wAsJournalGroupCode\":\"AND\",\"wAsJournalEISSN\":\"14390272\",\"wAsEditorialOfficeEmail\":null},\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":3450,\"price\":3450,\"subtotal\":3450,\"tax\":0,\"total\":3450,\"discountAmount\":0,\"discountPercentage\":0,\"currencyCode\":\"USD\",\"allDiscounts\":[],\"appliedDiscounts\":[]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"Have a goood day(*&amp;^%$#.\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"anagarajan@wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"GrantInstitute\",\"countryCode\":\"IN\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef4438-783b-4808-9127-af8e42410900\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef4438-783b-4808-9127-af8e42410900\",\"wAsSubmissionDate\":\"2024-04-15\",\"wAsAcceptedDate\":\"2024-02-10\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"Research Article\",\"wAsDisplayArticleType\":\"Research Article (ABC)\",\"ibrProduct\":{\"maId\":\"AND\",\"maName\":\"Andrologia\",\"wAsJournalUuid\":\"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"14390272\",\"wAsFlipDate\":\"2022-09-21\",\"wAsJournalTitle\":\"Andrologia\",\"wAsJournalGroupCode\":\"AND\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":null}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236052 for PriceProposal 24ef1284-783b-4808-9127-af8e42410880","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236052","priceProposal":{"uid":"6683cf7f-ba01-4774-961e-a86318934155","biId":"7236052","wAsSubmissionId":"24ef1284-783b-4808-9127-af8e42410880","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:27.208Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef1284-783b-4808-9127-af8e42410880","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2024-02-10","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"Have a goood day(*&amp;^%$#.","societyCodes":[],"promoCodes":[],"discountCodes":[],"referringJournalId":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"anagarajan@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"AixenProvence","countryCode":"IN","country":"IN","institution":"GrantInstitute","department":"SchoolofGeoSciences","stateProvince":"AndhraPradesh","postalCode":"500072","streetAddress":["1832ColvinAve"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:27.649Z"}},"wAsCountryCode":"IN","wAsReferringJournal":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","wAsReferringJournalRef":{"maId":"AND","maName":"Andrologia","wAsJournalUuid":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Andrologia","wAsJournalGroupCode":"AND","wAsJournalEISSN":"14390272","wAsEditorialOfficeEmail":null},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":3450,"price":3450,"subtotal":3450,"tax":0,"total":3450,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"Have a goood day(*&amp;^%$#.","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"anagarajan@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"GrantInstitute","countryCode":"IN","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef1284-783b-4808-9127-af8e42410880","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef1284-783b-4808-9127-af8e42410880","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2024-02-10","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"AND","maName":"Andrologia","wAsJournalUuid":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"14390272","wAsFlipDate":"2022-09-21","wAsJournalTitle":"Andrologia","wAsJournalGroupCode":"AND","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":null}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Geographical discount</t>
@@ -989,10 +1112,10 @@
     <t>b6d18dc5-3811-4b21-81f0-a01997c20001</t>
   </si>
   <si>
-    <t>Created Viax order 7231444 for PriceProposal 24ef1743-783b-4808-9127-af8e42410944</t>
-  </si>
-  <si>
-    <t>7231444</t>
+    <t>Created Viax order 7236053 for PriceProposal 24ef2470-783b-4808-9127-af8e42410841</t>
+  </si>
+  <si>
+    <t>7236053</t>
   </si>
   <si>
     <t>{
@@ -1000,7 +1123,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef1743-783b-4808-9127-af8e42410944",
+      "submissionId": "24ef2470-783b-4808-9127-af8e42410841",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "b6d18dc5-3811-4b21-81f0-a01997c20001",
@@ -1055,7 +1178,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231444 for PriceProposal 24ef1743-783b-4808-9127-af8e42410944\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231444\",\"priceProposal\":{\"uid\":\"66783003-150a-46ee-8226-8cc7afd09c1b\",\"biId\":\"7231444\",\"wAsSubmissionId\":\"24ef1743-783b-4808-9127-af8e42410944\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:24:03.755Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d02-8c68-fe0b8c46172a\",\"submissionId\":\"24ef1743-783b-4808-9127-af8e42410944\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"b6d18dc5-3811-4b21-81f0-a01997c20001\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"OPINION\",\"displayArticleType\":\"OPINION\",\"submissionDate\":\"2024-03-21\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[],\"promoCodes\":[],\"discountCodes\":[],\"editorialDiscountCode\":\"EMTW5R\",\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"MH\",\"country\":\"MH\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:04.206Z\"}},\"wAsCountryCode\":\"MH\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":300,\"price\":150,\"subtotal\":0,\"tax\":0,\"total\":0,\"discountAmount\":150,\"discountPercentage\":100,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":150,\"discountPercentage\":50,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"OPINION\",\"attribute\":\"wAsBaseArticleType\"},{\"value\":\"b6d18dc5-3811-4b21-81f0-a01997c20001\",\"attribute\":\"wAsJournalUuid\"}]},{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":60,\"discountPercentage\":20,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"OPINION\",\"attribute\":\"wAsBaseArticleType\"}]},{\"discountCode\":\"\",\"discountType\":\"GeographicalDiscount\",\"discountAmount\":150,\"discountPercentage\":100,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZGPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"MH\",\"attribute\":\"wAsCountryCode\"}]},{\"discountCode\":\"EMTW5R\",\"discountType\":\"EditorialDiscount\",\"discountAmount\":150,\"discountPercentage\":100,\"discountDescription\":\"EDITORIAL\",\"sapDiscountTableCode\":\"ZEPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"b6d18dc5-3811-4b21-81f0-a01997c20001\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"EMTW5R\",\"attribute\":\"wAsEditorialDiscountCode\"}]}],\"appliedDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":150,\"discountPercentage\":50,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null},{\"discountCode\":\"\",\"discountType\":\"GeographicalDiscount\",\"discountAmount\":150,\"discountPercentage\":100,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZGPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"MH\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":\"EMTW5R\",\"biiSalable\":{\"maId\":\"24ef1743-783b-4808-9127-af8e42410944\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef1743-783b-4808-9127-af8e42410944\",\"wAsSubmissionDate\":\"2024-03-21\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"OPINION\",\"wAsDisplayArticleType\":\"OPINION\",\"ibrProduct\":{\"maId\":\"CCR3\",\"maName\":\"Clinical Case Reports\",\"wAsJournalUuid\":\"b6d18dc5-3811-4b21-81f0-a01997c20001\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20500904\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Clinical Case Reports\",\"wAsJournalGroupCode\":\"CCR3\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"clinicalcases@wiley.com\"}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236053 for PriceProposal 24ef2470-783b-4808-9127-af8e42410841","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236053","priceProposal":{"uid":"6683cf83-efcf-4761-b4d1-b2b28a9a5c65","biId":"7236053","wAsSubmissionId":"24ef2470-783b-4808-9127-af8e42410841","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:31.910Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef2470-783b-4808-9127-af8e42410841","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"b6d18dc5-3811-4b21-81f0-a01997c20001","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"OPINION","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"EMTW5R","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"MH","country":"MH","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:32.359Z"}},"wAsCountryCode":"MH","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":300,"price":150,"subtotal":0,"tax":0,"total":0,"discountAmount":150,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"EMTW5R","discountType":"EditorialDiscount","discountAmount":150,"discountPercentage":100,"discountDescription":"EDITORIAL","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"b6d18dc5-3811-4b21-81f0-a01997c20001","attribute":"wAsJournalUuid"},{"value":"EMTW5R","attribute":"wAsEditorialDiscountCode"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":150,"discountPercentage":100,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"MH","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":150,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"b6d18dc5-3811-4b21-81f0-a01997c20001","attribute":"wAsJournalUuid"},{"value":"OPINION","attribute":"wAsBaseArticleType"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":60,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":150,"discountPercentage":100,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":150,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"MH","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"EMTW5R","biiSalable":{"maId":"24ef2470-783b-4808-9127-af8e42410841","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef2470-783b-4808-9127-af8e42410841","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"OPINION","ibrProduct":{"maId":"CCR3","maName":"Clinical Case Reports","wAsJournalUuid":"b6d18dc5-3811-4b21-81f0-a01997c20001","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20500904","wAsFlipDate":null,"wAsJournalTitle":"Clinical Case Reports","wAsJournalGroupCode":"CCR3","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"clinicalcases@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Article type discount</t>
@@ -1064,10 +1187,10 @@
     <t>ArticleType</t>
   </si>
   <si>
-    <t>Created Viax order 7231445 for PriceProposal 24ef1439-783b-4808-9127-af8e42410739</t>
-  </si>
-  <si>
-    <t>7231445</t>
+    <t>Created Viax order 7236054 for PriceProposal 24ef2890-783b-4808-9127-af8e42410382</t>
+  </si>
+  <si>
+    <t>7236054</t>
   </si>
   <si>
     <t>{
@@ -1075,7 +1198,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef1439-783b-4808-9127-af8e42410739",
+      "submissionId": "24ef2890-783b-4808-9127-af8e42410382",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1129,22 +1252,19 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231445 for PriceProposal 24ef1439-783b-4808-9127-af8e42410739\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231445\",\"priceProposal\":{\"uid\":\"66783005-c523-4ea5-8067-c2502baf34aa\",\"biId\":\"7231445\",\"wAsSubmissionId\":\"24ef1439-783b-4808-9127-af8e42410739\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:24:05.313Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d02-8c68-fe0b8c46172a\",\"submissionId\":\"24ef1439-783b-4808-9127-af8e42410739\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"RESEARCH ARTICLE\",\"displayArticleType\":\"RESEARCH ARTICLE\",\"submissionDate\":\"2024-04-03\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[],\"promoCodes\":[],\"discountCodes\":[],\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"US\",\"country\":\"US\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:05.787Z\"}},\"wAsCountryCode\":\"US\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":800,\"price\":200,\"subtotal\":200,\"tax\":0,\"total\":200,\"discountAmount\":0,\"discountPercentage\":0,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"RESEARCH ARTICLE\",\"attribute\":\"wAsBaseArticleType\"}]}],\"appliedDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"US\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef1439-783b-4808-9127-af8e42410739\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef1439-783b-4808-9127-af8e42410739\",\"wAsSubmissionDate\":\"2024-04-03\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"RESEARCH ARTICLE\",\"wAsDisplayArticleType\":\"RESEARCH ARTICLE\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
-  </si>
-  <si>
-    <t>Create PP with Stacked Institutional discount($ &amp; %)</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236054 for PriceProposal 24ef2890-783b-4808-9127-af8e42410382","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236054","priceProposal":{"uid":"6683cf89-af29-4923-b59a-423f8149493b","biId":"7236054","wAsSubmissionId":"24ef2890-783b-4808-9127-af8e42410382","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:37.032Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef2890-783b-4808-9127-af8e42410382","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-04-03","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:37.482Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2890-783b-4808-9127-af8e42410382","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef2890-783b-4808-9127-af8e42410382","wAsSubmissionDate":"2024-04-03","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+  </si>
+  <si>
+    <t>Create PP with Stacked Institutional discount</t>
   </si>
   <si>
     <t>Stacked</t>
   </si>
   <si>
-    <t>Created Viax order 7231446 for PriceProposal 24ef4825-783b-4808-9127-af8e42410858</t>
-  </si>
-  <si>
-    <t>7231446</t>
-  </si>
-  <si>
-    <t>DataCorrectionRequired</t>
+    <t>Created Viax order 7236055 for PriceProposal 24ef8508-783b-4808-9127-af8e42410878</t>
+  </si>
+  <si>
+    <t>7236055</t>
   </si>
   <si>
     <t>{
@@ -1152,10 +1272,10 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef4825-783b-4808-9127-af8e42410858",
+      "submissionId": "24ef8508-783b-4808-9127-af8e42410878",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
-      "journalId": "1b28a8b9-067b-4ce9-b981-e8eabe16e0a7",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
@@ -1206,7 +1326,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231446 for PriceProposal 24ef4825-783b-4808-9127-af8e42410858\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231446\",\"priceProposal\":{\"uid\":\"66783006-00fa-41a2-9b27-ce309e2be8dd\",\"biId\":\"7231446\",\"wAsSubmissionId\":\"24ef4825-783b-4808-9127-af8e42410858\",\"bpStatus\":{\"code\":\"DataCorrectionRequired\"},\"biCreatedAt\":\"2024-06-23T14:24:06.865Z\",\"wAsPaymentType\":\"Undefined\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d02-8c68-fe0b8c46172a\",\"submissionId\":\"24ef4825-783b-4808-9127-af8e42410858\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"Research Article\",\"displayArticleType\":\"Research Article (ABC)\",\"submissionDate\":\"2024-03-21\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[],\"promoCodes\":[],\"discountCodes\":[],\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"1666\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"GB\",\"country\":\"UK\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:07.427Z\"}},\"wAsCountryCode\":\"GB\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[{\"errorCode\":\"500\",\"errorMessage\":\"Price calculation error. {}\",\"fieldPath\":\"\",\"fieldValue\":\"\"}],\"wAsPricing\":null,\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"1666\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"GB\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef4825-783b-4808-9127-af8e42410858\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef4825-783b-4808-9127-af8e42410858\",\"wAsSubmissionDate\":\"2024-03-21\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"Research Article\",\"wAsDisplayArticleType\":\"Research Article (ABC)\",\"ibrProduct\":{\"maId\":\"AND\",\"maName\":\"Andrologia\",\"wAsJournalUuid\":\"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"14390272\",\"wAsFlipDate\":\"2022-09-21\",\"wAsJournalTitle\":\"Andrologia\",\"wAsJournalGroupCode\":\"AND\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":null}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236055 for PriceProposal 24ef8508-783b-4808-9127-af8e42410878","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236055","priceProposal":{"uid":"6683cf8d-4bec-43e0-9933-a9fd65e2b505","biId":"7236055","wAsSubmissionId":"24ef8508-783b-4808-9127-af8e42410878","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:41.183Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef8508-783b-4808-9127-af8e42410878","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"GB","country":"UK","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:41.799Z"}},"wAsCountryCode":"GB","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":2471,"price":617.75,"subtotal":0,"tax":0,"total":0,"discountAmount":617.75,"discountPercentage":100,"currencyCode":"GBP","allDiscounts":[{"discountCode":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","discountType":"Institutional","discountAmount":617.75,"discountPercentage":39.76851477134763,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":1853.25,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1853.25,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","discountType":"Institutional","discountAmount":617.75,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"GB","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8508-783b-4808-9127-af8e42410878","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef8508-783b-4808-9127-af8e42410878","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with multiple Society and Promotional discounts</t>
@@ -1215,10 +1335,10 @@
     <t>SocietyPromo</t>
   </si>
   <si>
-    <t>Created Viax order 7231447 for PriceProposal 24ef1041-783b-4808-9127-af8e42410696</t>
-  </si>
-  <si>
-    <t>7231447</t>
+    <t>Created Viax order 7236056 for PriceProposal 24ef6804-783b-4808-9127-af8e42410110</t>
+  </si>
+  <si>
+    <t>7236056</t>
   </si>
   <si>
     <t>{
@@ -1226,7 +1346,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef1041-783b-4808-9127-af8e42410696",
+      "submissionId": "24ef6804-783b-4808-9127-af8e42410110",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1284,42 +1404,44 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231447 for PriceProposal 24ef1041-783b-4808-9127-af8e42410696\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231447\",\"priceProposal\":{\"uid\":\"66783008-e754-4e33-90b1-ec3a29c3041e\",\"biId\":\"7231447\",\"wAsSubmissionId\":\"24ef1041-783b-4808-9127-af8e42410696\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:24:08.475Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d12-8c68-fe0b8c46172a\",\"submissionId\":\"24ef1041-783b-4808-9127-af8e42410696\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"Research Article\",\"displayArticleType\":\"Research Article (ABC)\",\"submissionDate\":\"2024-04-17\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[\"JCASP\"],\"promoCodes\":[\"PROMO50\"],\"discountCodes\":[],\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"US\",\"country\":\"US\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[{\"discountCode\":\"PROMO50\",\"discountType\":\"WileyPromoCode\",\"discountAmount\":40,\"discountPercentage\":20,\"discountDescription\":\"UPDATED VALID TO DATE\",\"sapDiscountTableCode\":\"ZPP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":false,\"discountContext\":[{\"value\":\"PROMO50\",\"attribute\":\"wAsSelectedPromotionPercentageDiscountCode\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]},{\"discountCode\":\"JCASP\",\"discountType\":\"Society\",\"discountAmount\":10,\"discountPercentage\":5,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZSP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":false,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"JCASP\",\"attribute\":\"wAsSelectedSocietyPercentageDiscountCode\"}]}],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:08.920Z\"}},\"wAsCountryCode\":\"US\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":800,\"price\":200,\"subtotal\":160,\"tax\":0,\"total\":160,\"discountAmount\":40,\"discountPercentage\":20,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"JCASP\",\"discountType\":\"Society\",\"discountAmount\":10,\"discountPercentage\":5,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZSP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"JCASP\",\"attribute\":\"wAsSelectedSocietyPercentageDiscountCode\"}]},{\"discountCode\":\"PROMO50\",\"discountType\":\"WileyPromoCode\",\"discountAmount\":40,\"discountPercentage\":20,\"discountDescription\":\"UPDATED VALID TO DATE\",\"sapDiscountTableCode\":\"ZPP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"PROMO50\",\"attribute\":\"wAsSelectedPromotionPercentageDiscountCode\"}]},{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"RESEARCH ARTICLE\",\"attribute\":\"wAsBaseArticleType\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]}],\"appliedDiscounts\":[{\"discountCode\":\"PROMO50\",\"discountType\":\"WileyPromoCode\",\"discountAmount\":40,\"discountPercentage\":20,\"discountDescription\":\"UPDATED VALID TO DATE\",\"sapDiscountTableCode\":\"ZPP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null},{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"US\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef1041-783b-4808-9127-af8e42410696\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef1041-783b-4808-9127-af8e42410696\",\"wAsSubmissionDate\":\"2024-04-17\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"Research Article\",\"wAsDisplayArticleType\":\"Research Article (ABC)\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
-  </si>
-  <si>
-    <t>Create PP with same discount % (Geographical, Editorial and Society discounts)</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236056 for PriceProposal 24ef6804-783b-4808-9127-af8e42410110","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236056","priceProposal":{"uid":"6683cf91-da42-4e15-80c0-c0d121be7217","biId":"7236056","wAsSubmissionId":"24ef6804-783b-4808-9127-af8e42410110","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:45.584Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6804-783b-4808-9127-af8e42410110","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-17","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:46.112Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6804-783b-4808-9127-af8e42410110","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef6804-783b-4808-9127-af8e42410110","wAsSubmissionDate":"2024-04-17","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+  </si>
+  <si>
+    <t>Create PP with same discount Geographical Editorial and Society discounts</t>
   </si>
   <si>
     <t>GeoEditSociety</t>
   </si>
   <si>
-    <t>['Price proposal already created.']</t>
+    <t>Created Viax order 7236057 for PriceProposal 24ef1931-783b-4808-9127-af8e42410691</t>
+  </si>
+  <si>
+    <t>7236057</t>
   </si>
   <si>
     <t>{
   "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
   "variables": {
     "data": {
-      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "5168a602-3307-4503-8576-aa709dd0d368",
+      "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
+      "submissionId": "24ef1931-783b-4808-9127-af8e42410691",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
-      "journalId": "3a634d93-aea6-4ba1-9cd2-08ec458c273b",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
-      "baseArticleType": "OPINION",
-      "displayArticleType": "OPINION",
-      "submissionDate": "2024-04-23",
+      "baseArticleType": "EDUCATION",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-04-17",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
       "isManualOverrideRequired": false,
       "manualOverrideInstructions": "string",
       "societyCodes": [
-        "MAU25"
+        "EANM9"
       ],
       "promoCodes": [],
       "discountCodes": [],
-      "editorialDiscountCode": "BES25",
       "authors": [
         {
           "role": "Corresponding Author",
@@ -1340,8 +1462,8 @@
                 }
               ],
               "addressLocality": "Aix en Provence",
-              "countryCode": "PE",
-              "country": "PE",
+              "countryCode": "BO",
+              "country": "BO",
               "institution": "Grant Institute",
               "department": "School of GeoSciences",
               "stateProvince": "New Jersey",
@@ -1358,19 +1480,19 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"FAILURE\",\"errors\":[\"Price proposal already created.\"],\"errorCode\":\"P040\",\"errorValue\":\"5168a602-3307-4503-8576-aa709dd0d368\"}"}}}</t>
-  </si>
-  <si>
-    <t>Create PP with Society, Promotional, Geographical, Editorial, Article type &amp; Referral discounts</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236057 for PriceProposal 24ef1931-783b-4808-9127-af8e42410691","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236057","priceProposal":{"uid":"6683cf95-047f-4903-a1eb-be436fa537fb","biId":"7236057","wAsSubmissionId":"24ef1931-783b-4808-9127-af8e42410691","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:49.814Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef1931-783b-4808-9127-af8e42410691","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-17","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM9"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"BO","country":"BO","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"EANM9","discountType":"Society","discountAmount":400,"discountPercentage":50,"discountDescription":"SOCIETY","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"EANM9","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:50.183Z"}},"wAsCountryCode":"BO","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":400,"tax":0,"total":400,"discountAmount":400,"discountPercentage":50,"currencyCode":"USD","allDiscounts":[{"discountCode":"EANM9","discountType":"Society","discountAmount":400,"discountPercentage":50,"discountDescription":"SOCIETY","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"EANM9","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":400,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"BO","attribute":"wAsCountryCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":400,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"BO","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef1931-783b-4808-9127-af8e42410691","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef1931-783b-4808-9127-af8e42410691","wAsSubmissionDate":"2024-04-17","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+  </si>
+  <si>
+    <t>Create PP with Society Promotional Geographical Editorial Article type and Referral discounts</t>
   </si>
   <si>
     <t>All</t>
   </si>
   <si>
-    <t>Created Viax order 7231448 for PriceProposal 24ef3295-783b-4808-9127-af8e42410770</t>
-  </si>
-  <si>
-    <t>7231448</t>
+    <t>Created Viax order 7236058 for PriceProposal 24ef4032-783b-4808-9127-af8e42410900</t>
+  </si>
+  <si>
+    <t>7236058</t>
   </si>
   <si>
     <t>{
@@ -1378,7 +1500,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef3295-783b-4808-9127-af8e42410770",
+      "submissionId": "24ef4032-783b-4808-9127-af8e42410900",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1438,7 +1560,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231448 for PriceProposal 24ef3295-783b-4808-9127-af8e42410770\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231448\",\"priceProposal\":{\"uid\":\"6678300a-d8c2-4d35-9871-986fefd8897d\",\"biId\":\"7231448\",\"wAsSubmissionId\":\"24ef3295-783b-4808-9127-af8e42410770\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:24:10.546Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d02-8c68-fe0b8c46172a\",\"submissionId\":\"24ef3295-783b-4808-9127-af8e42410770\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"RESEARCH ARTICLE\",\"displayArticleType\":\"RESEARCH ARTICLE\",\"submissionDate\":\"2024-04-03\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[\"JCASP\"],\"promoCodes\":[\"PROMO50\"],\"discountCodes\":[],\"editorialDiscountCode\":\"CCCAM424\",\"referringJournalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"PE\",\"country\":\"PE\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[{\"discountCode\":\"JCASP\",\"discountType\":\"Society\",\"discountAmount\":10,\"discountPercentage\":5,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZSP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":false,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"JCASP\",\"attribute\":\"wAsSelectedSocietyPercentageDiscountCode\"}]},{\"discountCode\":\"PROMO50\",\"discountType\":\"WileyPromoCode\",\"discountAmount\":40,\"discountPercentage\":20,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZPP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":false,\"discountContext\":[{\"value\":\"PROMO50\",\"attribute\":\"wAsSelectedPromotionPercentageDiscountCode\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]}],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:10.986Z\"}},\"wAsCountryCode\":\"PE\",\"wAsReferringJournal\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsReferringJournalRef\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalStatus\":\"Yes\",\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalEISSN\":\"20457634\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"},\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":800,\"price\":200,\"subtotal\":20,\"tax\":0,\"total\":20,\"discountAmount\":180,\"discountPercentage\":90,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ReferralDiscount\",\"discountAmount\":100,\"discountPercentage\":50,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZRPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsReferringJournal\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]},{\"discountCode\":\"JCASP\",\"discountType\":\"Society\",\"discountAmount\":10,\"discountPercentage\":5,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZSP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"JCASP\",\"attribute\":\"wAsSelectedSocietyPercentageDiscountCode\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]},{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"RESEARCH ARTICLE\",\"attribute\":\"wAsBaseArticleType\"}]},{\"discountCode\":\"CCCAM424\",\"discountType\":\"EditorialDiscount\",\"discountAmount\":180,\"discountPercentage\":90,\"discountDescription\":\"\",\"sapDiscountTableCode\":\"ZEPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"CCCAM424\",\"attribute\":\"wAsEditorialDiscountCode\"}]},{\"discountCode\":\"PROMO50\",\"discountType\":\"WileyPromoCode\",\"discountAmount\":40,\"discountPercentage\":20,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZPP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"PROMO50\",\"attribute\":\"wAsSelectedPromotionPercentageDiscountCode\"}]},{\"discountCode\":\"\",\"discountType\":\"GeographicalDiscount\",\"discountAmount\":100,\"discountPercentage\":50,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZGPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"PE\",\"attribute\":\"wAsCountryCode\"}]}],\"appliedDiscounts\":[{\"discountCode\":\"CCCAM424\",\"discountType\":\"EditorialDiscount\",\"discountAmount\":180,\"discountPercentage\":90,\"discountDescription\":\"\",\"sapDiscountTableCode\":\"ZEPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null},{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"PE\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":\"CCCAM424\",\"biiSalable\":{\"maId\":\"24ef3295-783b-4808-9127-af8e42410770\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef3295-783b-4808-9127-af8e42410770\",\"wAsSubmissionDate\":\"2024-04-03\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"RESEARCH ARTICLE\",\"wAsDisplayArticleType\":\"RESEARCH ARTICLE\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236058 for PriceProposal 24ef4032-783b-4808-9127-af8e42410900","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236058","priceProposal":{"uid":"6683cf99-7481-4ed4-a663-49b344350c10","biId":"7236058","wAsSubmissionId":"24ef4032-783b-4808-9127-af8e42410900","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:53.476Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef4032-783b-4808-9127-af8e42410900","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-04-03","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"editorialDiscountCode":"CCCAM424","referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"PE","country":"PE","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:54.050Z"}},"wAsCountryCode":"PE","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsReferringJournalRef":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalEISSN":"20457634","wAsEditorialOfficeEmail":"cancermed@wiley.com"},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":20,"tax":0,"total":20,"discountAmount":180,"discountPercentage":90,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":100,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PE","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ReferralDiscount","discountAmount":100,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsReferringJournal"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":180,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":180,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"PE","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef4032-783b-4808-9127-af8e42410900","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef4032-783b-4808-9127-af8e42410900","wAsSubmissionDate":"2024-04-03","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Multiple Insitutional discounts</t>
@@ -1447,10 +1569,10 @@
     <t>MultiInsti</t>
   </si>
   <si>
-    <t>Created Viax order 7231449 for PriceProposal 24ef9761-783b-4808-9127-af8e42410283</t>
-  </si>
-  <si>
-    <t>7231449</t>
+    <t>Created Viax order 7236059 for PriceProposal 24ef5056-783b-4808-9127-af8e42410812</t>
+  </si>
+  <si>
+    <t>7236059</t>
   </si>
   <si>
     <t>{
@@ -1458,7 +1580,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef9761-783b-4808-9127-af8e42410283",
+      "submissionId": "24ef5056-783b-4808-9127-af8e42410812",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1514,7 +1636,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231449 for PriceProposal 24ef9761-783b-4808-9127-af8e42410283\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231449\",\"priceProposal\":{\"uid\":\"6678300c-ecea-419e-afee-d23317200e13\",\"biId\":\"7231449\",\"wAsSubmissionId\":\"24ef9761-783b-4808-9127-af8e42410283\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:24:12.070Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d02-8c68-fe0b8c46172a\",\"submissionId\":\"24ef9761-783b-4808-9127-af8e42410283\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"Research Article\",\"displayArticleType\":\"Research Article (ABC)\",\"submissionDate\":\"2024-04-10\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[],\"promoCodes\":[],\"discountCodes\":[],\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"PhD\",\"orcId\":\"0000-0003-4043-3196\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"131661\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Stavnger\",\"countryCode\":\"US\",\"country\":\"France\",\"institution\":\"Ardrossan Area School\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"Rogaland Fylke\",\"postalCode\":\"4036\",\"streetAddress\":[\"Po Box 2554\"]}]}],\"funders\":[]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:12.572Z\"}},\"wAsCountryCode\":\"US\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":800,\"price\":200,\"subtotal\":200,\"tax\":0,\"total\":200,\"discountAmount\":0,\"discountPercentage\":0,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"RESEARCH ARTICLE\",\"attribute\":\"wAsBaseArticleType\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]}],\"appliedDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":\"0000-0003-4043-3196\",\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"PhD\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"131661\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Ardrossan Area School\",\"countryCode\":\"US\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef9761-783b-4808-9127-af8e42410283\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef9761-783b-4808-9127-af8e42410283\",\"wAsSubmissionDate\":\"2024-04-10\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"Research Article\",\"wAsDisplayArticleType\":\"Research Article (ABC)\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236059 for PriceProposal 24ef5056-783b-4808-9127-af8e42410812","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236059","priceProposal":{"uid":"6683cf9d-2dd8-469a-92c6-7568ca3b3e0d","biId":"7236059","wAsSubmissionId":"24ef5056-783b-4808-9127-af8e42410812","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:57.034Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef5056-783b-4808-9127-af8e42410812","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-10","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"PhD","orcId":"0000-0003-4043-3196","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"addressLocality":"Stavnger","countryCode":"US","country":"France","institution":"Ardrossan Area School","department":"School of GeoSciences","stateProvince":"Rogaland Fylke","postalCode":"4036","streetAddress":["Po Box 2554"]}]}],"funders":[]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:57.411Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":"0000-0003-4043-3196","firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"PhD","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"affiliationName":"Ardrossan Area School","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5056-783b-4808-9127-af8e42410812","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef5056-783b-4808-9127-af8e42410812","wAsSubmissionDate":"2024-04-10","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Funder details</t>
@@ -1523,10 +1645,10 @@
     <t>FunderPaid</t>
   </si>
   <si>
-    <t>Created Viax order 7231450 for PriceProposal 24ef2145-783b-4808-9127-af8e42410972</t>
-  </si>
-  <si>
-    <t>7231450</t>
+    <t>Created Viax order 7236060 for PriceProposal 24ef2720-783b-4808-9127-af8e42410157</t>
+  </si>
+  <si>
+    <t>7236060</t>
   </si>
   <si>
     <t>{
@@ -1534,7 +1656,7 @@
   "variables": {
     "data": {
       "requestId": "4a48d9c8-6b6d-4583-b9ac-1836890cb988",
-      "submissionId": "24ef2145-783b-4808-9127-af8e42410972",
+      "submissionId": "24ef2720-783b-4808-9127-af8e42410157",
       "edRefCode": "CAM4-2024-04-1853",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1621,7 +1743,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231450 for PriceProposal 24ef2145-783b-4808-9127-af8e42410972\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231450\",\"priceProposal\":{\"uid\":\"6678300d-1f8d-44ac-be2e-56edb7ee408b\",\"biId\":\"7231450\",\"wAsSubmissionId\":\"24ef2145-783b-4808-9127-af8e42410972\",\"bpStatus\":{\"code\":\"PriceDetermined\"},\"biCreatedAt\":\"2024-06-23T14:24:13.557Z\",\"wAsPaymentType\":\"AuthorPaid\",\"wAsPriceProposalPayload\":{\"requestId\":\"4a48d9c8-6b6d-4583-b9ac-1836890cb988\",\"submissionId\":\"24ef2145-783b-4808-9127-af8e42410972\",\"edRefCode\":\"CAM4-2024-04-1853\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"Data Article\",\"displayArticleType\":\"Research Article (ABC)\",\"submissionDate\":\"2024-03-21\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[],\"promoCodes\":[],\"discountCodes\":[],\"wAsManualDiscountAmount\":0,\"authors\":[{\"role\":\"CorrespondingAuthor\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"email\":\"TestAuto@wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"131661\",\"institutionIdType\":\"Ringgold\"}],\"orcId\":\"0000-0003-0888-1984\",\"addressLocality\":\"Stavnger\",\"countryCode\":\"US\",\"country\":\"USA\",\"institution\":\"Universidad Nacional De Ingenieria\",\"department\":\"SchoolofGeoSciences\",\"stateProvince\":\"RogalandFylke\",\"postalCode\":\"4036\",\"streetAddress\":[\"PoBox2554\"]},{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"orcId\":\"0000-0003-0888-1984\",\"addressLocality\":\"Stavnger\",\"countryCode\":\"US\",\"country\":\"USA\",\"institution\":\"Universidad Nacional De Ingenieria\",\"department\":\"SchoolofGeoSciences\",\"stateProvince\":\"RogalandFylke\",\"postalCode\":\"4036\",\"streetAddress\":[\"PoBox2554\"]}]}],\"funders\":[{\"name\":\"ARC of the Piedmont (The Arc)\",\"funderId\":\"10.13039/100006467\",\"grants\":[{\"grantNumber\":\"124566AA\",\"grantRecipient\":[\"PhilipJ.Cameron-Smith\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:13.909Z\"}},\"wAsCountryCode\":\"US\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":800,\"price\":800,\"subtotal\":800,\"tax\":0,\"total\":800,\"discountAmount\":0,\"discountPercentage\":0,\"currencyCode\":\"USD\",\"allDiscounts\":[],\"appliedDiscounts\":[]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAuto@wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":null,\"honorificSuffix\":null,\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"131661\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Universidad Nacional De Ingenieria\",\"countryCode\":\"US\",\"isPrimary\":null},{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Universidad Nacional De Ingenieria\",\"countryCode\":\"US\",\"isPrimary\":null}]},\"wAsResearchFunders\":[{\"funderId\":\"10.13039/100006467\",\"name\":\"ARC of the Piedmont (The Arc)\",\"researchGrants\":[{\"grantNumber\":\"124566AA\",\"grantRecipients\":[\"PhilipJ.Cameron-Smith\"]}]}],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef2145-783b-4808-9127-af8e42410972\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"CAM4-2024-04-1853\",\"wAsSubmissionId\":\"24ef2145-783b-4808-9127-af8e42410972\",\"wAsSubmissionDate\":\"2024-03-21\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"Data Article\",\"wAsDisplayArticleType\":\"Research Article (ABC)\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236060 for PriceProposal 24ef2720-783b-4808-9127-af8e42410157","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236060","priceProposal":{"uid":"6683cfa0-2b4a-4ab0-a74d-f5c4b120f9a7","biId":"7236060","wAsSubmissionId":"24ef2720-783b-4808-9127-af8e42410157","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T10:00:00.727Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"4a48d9c8-6b6d-4583-b9ac-1836890cb988","submissionId":"24ef2720-783b-4808-9127-af8e42410157","edRefCode":"CAM4-2024-04-1853","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Data Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"wAsManualDiscountAmount":0,"authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","email":"TestAuto@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"orcId":"0000-0003-0888-1984","addressLocality":"Stavnger","countryCode":"US","country":"USA","institution":"Universidad Nacional De Ingenieria","department":"SchoolofGeoSciences","stateProvince":"RogalandFylke","postalCode":"4036","streetAddress":["PoBox2554"]},{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"orcId":"0000-0003-0888-1984","addressLocality":"Stavnger","countryCode":"US","country":"USA","institution":"Universidad Nacional De Ingenieria","department":"SchoolofGeoSciences","stateProvince":"RogalandFylke","postalCode":"4036","streetAddress":["PoBox2554"]}]}],"funders":[{"name":"ARC of the Piedmont (The Arc)","funderId":"10.13039/100006467","grants":[{"grantNumber":"124566AA","grantRecipient":["PhilipJ.Cameron-Smith"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T10:00:01.661Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":800,"tax":0,"total":800,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAuto@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":null,"honorificSuffix":null,"affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Universidad Nacional De Ingenieria","countryCode":"US","isPrimary":null},{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"affiliationName":"Universidad Nacional De Ingenieria","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[{"funderId":"10.13039/100006467","name":"ARC of the Piedmont (The Arc)","researchGrants":[{"grantNumber":"124566AA","grantRecipients":["PhilipJ.Cameron-Smith"]}]}],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2720-783b-4808-9127-af8e42410157","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"CAM4-2024-04-1853","wAsSubmissionId":"24ef2720-783b-4808-9127-af8e42410157","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Data Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Invalid Promotional discount code</t>
@@ -1630,10 +1752,13 @@
     <t>InvalidPromo</t>
   </si>
   <si>
-    <t>Created Viax order 7231451 for PriceProposal 24ef7783-783b-4808-9127-af8e42410291</t>
-  </si>
-  <si>
-    <t>7231451</t>
+    <t>Created Viax order 7236061 for PriceProposal 24ef9151-783b-4808-9127-af8e42410275</t>
+  </si>
+  <si>
+    <t>7236061</t>
+  </si>
+  <si>
+    <t>DataCorrectionRequired</t>
   </si>
   <si>
     <t>{
@@ -1641,7 +1766,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef7783-783b-4808-9127-af8e42410291",
+      "submissionId": "24ef9151-783b-4808-9127-af8e42410275",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1697,7 +1822,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231451 for PriceProposal 24ef7783-783b-4808-9127-af8e42410291\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231451\",\"priceProposal\":{\"uid\":\"6678300e-4a9b-4df6-8858-183a38a09dcf\",\"biId\":\"7231451\",\"wAsSubmissionId\":\"24ef7783-783b-4808-9127-af8e42410291\",\"bpStatus\":{\"code\":\"DataCorrectionRequired\"},\"biCreatedAt\":\"2024-06-23T14:24:14.851Z\",\"wAsPaymentType\":\"Undefined\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d12-8c68-fe0b8c46172a\",\"submissionId\":\"24ef7783-783b-4808-9127-af8e42410291\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"Research Article\",\"displayArticleType\":\"Research Article (ABC)\",\"submissionDate\":\"2024-04-15\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":false,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[],\"promoCodes\":[\"PRKMO50\"],\"discountCodes\":[],\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"US\",\"country\":\"US\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[{\"discountCode\":\"PRKMO50\",\"discountType\":\"WileyPromoCode\",\"discountAmount\":null,\"discountPercentage\":null,\"discountDescription\":null,\"sapDiscountTableCode\":null,\"isPercentageDiscount\":null,\"isStackedDiscount\":null,\"discountContext\":[]}],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:15.264Z\"}},\"wAsCountryCode\":\"US\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[{\"errorCode\":\"P030\",\"errorMessage\":\"The discount code 'PRKMO50' does not exist.\",\"fieldPath\":\"wAsDiscountCodes[0].discountCode\",\"fieldValue\":\"PRKMO50\"}],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":800,\"price\":200,\"subtotal\":200,\"tax\":0,\"total\":200,\"discountAmount\":0,\"discountPercentage\":0,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"RESEARCH ARTICLE\",\"attribute\":\"wAsBaseArticleType\"}]},{\"discountCode\":\"PRKMO50\",\"discountType\":\"WileyPromoCode\",\"discountAmount\":null,\"discountPercentage\":null,\"discountDescription\":null,\"sapDiscountTableCode\":null,\"isPercentageDiscount\":null,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[]}],\"appliedDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":false,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"US\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef7783-783b-4808-9127-af8e42410291\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef7783-783b-4808-9127-af8e42410291\",\"wAsSubmissionDate\":\"2024-04-15\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"Research Article\",\"wAsDisplayArticleType\":\"Research Article (ABC)\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236061 for PriceProposal 24ef9151-783b-4808-9127-af8e42410275","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236061","priceProposal":{"uid":"6683cfae-af87-4170-bb8b-4558efc43967","biId":"7236061","wAsSubmissionId":"24ef9151-783b-4808-9127-af8e42410275","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-07-02T10:00:14.406Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef9151-783b-4808-9127-af8e42410275","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PRKMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T10:00:14.908Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'PRKMO50\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"PRKMO50"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef9151-783b-4808-9127-af8e42410275","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef9151-783b-4808-9127-af8e42410275","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Manual override required value as Yes</t>
@@ -1706,10 +1831,10 @@
     <t>ManualOverride</t>
   </si>
   <si>
-    <t>Created Viax order 7231452 for PriceProposal 24ef9402-783b-4808-9127-af8e42410312</t>
-  </si>
-  <si>
-    <t>7231452</t>
+    <t>Created Viax order 7236065 for PriceProposal 24ef8820-783b-4808-9127-af8e42410282</t>
+  </si>
+  <si>
+    <t>7236065</t>
   </si>
   <si>
     <t>ManualOverrideRequired</t>
@@ -1720,7 +1845,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef9402-783b-4808-9127-af8e42410312",
+      "submissionId": "24ef8820-783b-4808-9127-af8e42410282",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1776,7 +1901,7 @@
 }</t>
   </si>
   <si>
-    <t>{"data":{"testFunction":{"status":200,"data":"{\"status\":\"SUCCESS\",\"message\":\"Created Viax order 7231452 for PriceProposal 24ef9402-783b-4808-9127-af8e42410312\",\"version\":\"1.4.0-qa2.36\",\"viaxPriceProposalId\":\"7231452\",\"priceProposal\":{\"uid\":\"66783010-14a7-45eb-afbf-7262bbe28b5d\",\"biId\":\"7231452\",\"wAsSubmissionId\":\"24ef9402-783b-4808-9127-af8e42410312\",\"bpStatus\":{\"code\":\"ManualOverrideRequired\"},\"biCreatedAt\":\"2024-06-23T14:24:16.299Z\",\"wAsPaymentType\":\"Undefined\",\"wAsPriceProposalPayload\":{\"requestId\":\"e5a1358c-2f36-4d12-8c68-fe0b8c46172a\",\"submissionId\":\"24ef9402-783b-4808-9127-af8e42410312\",\"edRefCode\":\"ACN3-2023-06-0432\",\"articleDOI\":\"\",\"journalId\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"sourceSystem\":\"EM\",\"baseArticleType\":\"Research Article\",\"displayArticleType\":\"Research Article (ABC)\",\"submissionDate\":\"2024-04-15\",\"articleAcceptedDate\":\"2015-09-29\",\"editorialStatus\":\"TBC\",\"articleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"isManualOverrideRequired\":true,\"manualOverrideInstructions\":\"string\",\"societyCodes\":[\"JCASP\"],\"promoCodes\":[],\"discountCodes\":[],\"authors\":[{\"role\":\"Corresponding Author\",\"authorSequenceNumber\":1,\"firstName\":\"Jim\",\"middleName\":\"M.\",\"lastName\":\"TESSON\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"email\":\"TestAutomation@Wiley.com\",\"affiliationIdType\":\"Ringgold\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"addressLocality\":\"Aix en Provence\",\"countryCode\":\"US\",\"country\":\"US\",\"institution\":\"Grant Institute\",\"department\":\"School of GeoSciences\",\"stateProvince\":\"New Jersey\",\"postalCode\":\"90210\",\"streetAddress\":[\"1832 Colvin Ave\"]}]}]},\"wAsOrderUniqueId\":null,\"wAsOrderStatus\":null,\"wAsLastEmailDate\":null,\"wAsSuppressEmail\":null,\"wAsDiscountCodes\":[{\"discountCode\":\"JCASP\",\"discountType\":\"Society\",\"discountAmount\":10,\"discountPercentage\":5,\"discountDescription\":\"BULK LOAD EQ2 - QA ON 12/19/2023\",\"sapDiscountTableCode\":\"ZSP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":false,\"discountContext\":[{\"value\":\"JCASP\",\"attribute\":\"wAsSelectedSocietyPercentageDiscountCode\"},{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"}]}],\"auAudit\":{\"updatedAt\":{\"dateTime\":\"2024-06-23T14:24:16.736Z\"}},\"wAsCountryCode\":\"US\",\"wAsReferringJournal\":null,\"wAsReferringJournalRef\":null,\"wAsValidationErrors\":[],\"wAsPricing\":{\"isFunded\":false,\"woadInstitution\":null,\"prices\":[{\"basePrice\":800,\"price\":200,\"subtotal\":190,\"tax\":0,\"total\":190,\"discountAmount\":10,\"discountPercentage\":5,\"currencyCode\":\"USD\",\"allDiscounts\":[{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"RESEARCH ARTICLE\",\"attribute\":\"wAsBaseArticleType\"}]},{\"discountCode\":\"JCASP\",\"discountType\":\"Society\",\"discountAmount\":10,\"discountPercentage\":5,\"discountDescription\":\"BULK LOAD EQ2 - QA ON 12/19/2023\",\"sapDiscountTableCode\":\"ZSP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null,\"discountContext\":[{\"value\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"attribute\":\"wAsJournalUuid\"},{\"value\":\"JCASP\",\"attribute\":\"wAsSelectedSocietyPercentageDiscountCode\"}]}],\"appliedDiscounts\":[{\"discountCode\":\"JCASP\",\"discountType\":\"Society\",\"discountAmount\":10,\"discountPercentage\":5,\"discountDescription\":\"BULK LOAD EQ2 - QA ON 12/19/2023\",\"sapDiscountTableCode\":\"ZSP1\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null},{\"discountCode\":\"\",\"discountType\":\"ArticleType\",\"discountAmount\":600,\"discountPercentage\":75,\"discountDescription\":null,\"sapDiscountTableCode\":\"ZAPA\",\"isPercentageDiscount\":true,\"isStackedDiscount\":null,\"institutionId\":null,\"institutionName\":null,\"institutionIdType\":null,\"woaCode\":null,\"consortiumCode\":null}]}]},\"wAsBillingDetails\":[],\"wAsManualDiscountAmount\":null,\"wAsManualOverrideRequired\":true,\"wAsManualDiscountPercentage\":null,\"wAsManualOverrideInstructions\":\"string\",\"wAsManualOverrideAppliedTime\":null,\"wAsCorrespondingAuthor\":{\"orcId\":null,\"firstName\":\"Jim\",\"lastName\":\"TESSON\",\"email\":\"TestAutomation@Wiley.com\",\"isResponsible\":false,\"affiliationIdType\":\"Ringgold\",\"honorificPrefix\":\"Mr.\",\"honorificSuffix\":\"\",\"affiliations\":[{\"affiliationIds\":[{\"institutionId\":\"\",\"institutionIdType\":\"Ringgold\"}],\"affiliationName\":\"Grant Institute\",\"countryCode\":\"US\",\"isPrimary\":null}]},\"wAsResearchFunders\":[],\"hiConsistsOf\":[{\"wAsEditorialDiscountCode\":null,\"biiSalable\":{\"maId\":\"24ef9402-783b-4808-9127-af8e42410312\",\"wAsArticleId\":null,\"wAsArticleDoi\":\"\",\"wAsArticleTitle\":\"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.\",\"wAsManuscriptId\":\"ACN3-2023-06-0432\",\"wAsSubmissionId\":\"24ef9402-783b-4808-9127-af8e42410312\",\"wAsSubmissionDate\":\"2024-04-15\",\"wAsAcceptedDate\":\"2015-09-29\",\"wAsEditorialStatus\":\"TBC\",\"wAsBaseArticleType\":\"Research Article\",\"wAsDisplayArticleType\":\"Research Article (ABC)\",\"ibrProduct\":{\"maId\":\"CAM4\",\"maName\":\"Cancer Medicine\",\"wAsJournalUuid\":\"c597beef-e45f-4cc7-b34c-0df812e2ef25\",\"wAsNewJournalRevenueModel\":\"OA\",\"wAsJournalEISSN\":\"20457634\",\"wAsFlipDate\":null,\"wAsJournalTitle\":\"Cancer Medicine\",\"wAsJournalGroupCode\":\"CAM4\",\"wAsJournalOwnership\":null,\"wAsJournalStatus\":\"Yes\",\"wAsEditorialOfficeEmail\":\"cancermed@wiley.com\"}}}]}}"}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236065 for PriceProposal 24ef8820-783b-4808-9127-af8e42410282","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236065","priceProposal":{"uid":"6683cfb2-23d1-4598-80ff-c6baeacc9e26","biId":"7236065","wAsSubmissionId":"24ef8820-783b-4808-9127-af8e42410282","bpStatus":{"code":"ManualOverrideRequired"},"biCreatedAt":"2024-07-02T10:00:18.794Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef8820-783b-4808-9127-af8e42410282","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":true,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T10:00:19.315Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":true,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8820-783b-4808-9127-af8e42410282","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef8820-783b-4808-9127-af8e42410282","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
 </sst>
 </file>
@@ -1851,8 +1976,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -3113,8 +3238,8 @@
   </sheetPr>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3124,7 +3249,7 @@
     <col min="3" max="3" width="27.90625" customWidth="1"/>
     <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="102.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.26953125" customWidth="1"/>
     <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1"/>
@@ -3343,10 +3468,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3477,34 +3602,34 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
         <v>160</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>161</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>162</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>163</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>164</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>165</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>166</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>167</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>168</v>
-      </c>
-      <c r="K2" t="s">
-        <v>169</v>
       </c>
       <c r="L2" t="s">
         <v>42</v>
@@ -3515,14 +3640,32 @@
       <c r="N2" t="s">
         <v>43</v>
       </c>
+      <c r="O2" t="s">
+        <v>44</v>
+      </c>
       <c r="P2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q2" t="s">
         <v>170</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>171</v>
       </c>
-      <c r="R2" t="s">
-        <v>172</v>
+      <c r="W2" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -3530,52 +3673,273 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" t="s">
         <v>173</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>174</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>175</v>
       </c>
-      <c r="E3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F3" t="s">
-        <v>164</v>
-      </c>
       <c r="G3" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="H3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L3" t="s">
         <v>42</v>
       </c>
       <c r="M3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>182</v>
+      </c>
+      <c r="R3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J4" t="s">
+        <v>192</v>
+      </c>
+      <c r="K4" t="s">
+        <v>193</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>195</v>
+      </c>
+      <c r="R4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" t="s">
+        <v>200</v>
+      </c>
+      <c r="I5" t="s">
+        <v>201</v>
+      </c>
+      <c r="J5" t="s">
+        <v>202</v>
+      </c>
+      <c r="K5">
+        <v>3213151</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" t="s">
         <v>55</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N5" t="s">
         <v>56</v>
       </c>
-      <c r="P3" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>171</v>
-      </c>
-      <c r="R3" t="s">
-        <v>172</v>
+      <c r="P5" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>195</v>
+      </c>
+      <c r="R5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" t="s">
+        <v>206</v>
+      </c>
+      <c r="F6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6" t="s">
+        <v>208</v>
+      </c>
+      <c r="H6" t="s">
+        <v>209</v>
+      </c>
+      <c r="I6" t="s">
+        <v>210</v>
+      </c>
+      <c r="J6" t="s">
+        <v>211</v>
+      </c>
+      <c r="K6" t="s">
+        <v>212</v>
+      </c>
+      <c r="L6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>214</v>
+      </c>
+      <c r="R6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" t="s">
+        <v>208</v>
+      </c>
+      <c r="H7" t="s">
+        <v>218</v>
+      </c>
+      <c r="I7" t="s">
+        <v>219</v>
+      </c>
+      <c r="J7" t="s">
+        <v>220</v>
+      </c>
+      <c r="K7" t="s">
+        <v>221</v>
+      </c>
+      <c r="L7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P7" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>214</v>
+      </c>
+      <c r="R7" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3591,8 +3955,8 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3614,31 +3978,31 @@
         <v>79</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>181</v>
+        <v>223</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>183</v>
+        <v>225</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>185</v>
+        <v>227</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>186</v>
+        <v>228</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>187</v>
+        <v>229</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>30</v>
@@ -3652,31 +4016,31 @@
         <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>189</v>
+        <v>231</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G2" t="s">
-        <v>192</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>194</v>
+        <v>233</v>
+      </c>
+      <c r="G2">
+        <v>7236048</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J2" t="s">
-        <v>195</v>
+        <v>236</v>
       </c>
       <c r="K2" t="s">
-        <v>196</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -3687,31 +4051,31 @@
         <v>154</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>197</v>
+        <v>238</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>198</v>
+        <v>239</v>
       </c>
       <c r="E3" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F3" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="G3" t="s">
-        <v>200</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>194</v>
+        <v>241</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J3" t="s">
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="K3" t="s">
-        <v>202</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -3722,31 +4086,31 @@
         <v>154</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>203</v>
+        <v>244</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>204</v>
+        <v>245</v>
       </c>
       <c r="E4" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F4" t="s">
-        <v>205</v>
+        <v>246</v>
       </c>
       <c r="G4" t="s">
-        <v>206</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>194</v>
+        <v>247</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J4" t="s">
-        <v>207</v>
+        <v>248</v>
       </c>
       <c r="K4" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -3757,31 +4121,31 @@
         <v>154</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>210</v>
+        <v>251</v>
       </c>
       <c r="E5" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F5" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="G5" t="s">
-        <v>212</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>194</v>
+        <v>253</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J5" t="s">
-        <v>213</v>
+        <v>254</v>
       </c>
       <c r="K5" t="s">
-        <v>214</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -3792,31 +4156,31 @@
         <v>154</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>215</v>
+        <v>256</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>216</v>
+        <v>257</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>258</v>
       </c>
       <c r="F6" t="s">
-        <v>218</v>
+        <v>259</v>
       </c>
       <c r="G6" t="s">
-        <v>219</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>194</v>
+        <v>260</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J6" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="K6" t="s">
-        <v>221</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -3827,31 +4191,31 @@
         <v>154</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>222</v>
+        <v>263</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="E7" t="s">
-        <v>224</v>
+        <v>265</v>
       </c>
       <c r="F7" t="s">
-        <v>225</v>
+        <v>266</v>
       </c>
       <c r="G7" t="s">
-        <v>226</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>194</v>
+        <v>267</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J7" t="s">
-        <v>227</v>
+        <v>268</v>
       </c>
       <c r="K7" t="s">
-        <v>228</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -3862,31 +4226,31 @@
         <v>154</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>229</v>
+        <v>270</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>230</v>
+        <v>271</v>
       </c>
       <c r="E8" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F8" t="s">
-        <v>231</v>
+        <v>272</v>
       </c>
       <c r="G8" t="s">
-        <v>232</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>194</v>
+        <v>273</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J8" t="s">
-        <v>233</v>
+        <v>274</v>
       </c>
       <c r="K8" t="s">
-        <v>234</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -3897,31 +4261,31 @@
         <v>154</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="F9" t="s">
+        <v>278</v>
+      </c>
+      <c r="G9" t="s">
+        <v>279</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="F9" t="s">
-        <v>237</v>
-      </c>
-      <c r="G9" t="s">
-        <v>238</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>194</v>
-      </c>
       <c r="J9" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="K9" t="s">
-        <v>241</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -3932,31 +4296,31 @@
         <v>154</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>243</v>
+        <v>283</v>
       </c>
       <c r="E10" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F10" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
       <c r="G10" t="s">
-        <v>245</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>194</v>
+        <v>285</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J10" t="s">
-        <v>246</v>
+        <v>286</v>
       </c>
       <c r="K10" t="s">
-        <v>247</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -3967,25 +4331,31 @@
         <v>154</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>248</v>
+        <v>288</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>249</v>
+        <v>289</v>
       </c>
       <c r="E11" t="s">
-        <v>190</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>194</v>
+        <v>232</v>
+      </c>
+      <c r="F11" t="s">
+        <v>290</v>
+      </c>
+      <c r="G11" t="s">
+        <v>291</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J11" t="s">
-        <v>251</v>
+        <v>292</v>
       </c>
       <c r="K11" t="s">
-        <v>252</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -3996,31 +4366,31 @@
         <v>154</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>253</v>
+        <v>294</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>254</v>
+        <v>295</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F12" t="s">
-        <v>255</v>
+        <v>296</v>
       </c>
       <c r="G12" t="s">
-        <v>256</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>194</v>
+        <v>297</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J12" t="s">
-        <v>257</v>
+        <v>298</v>
       </c>
       <c r="K12" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -4031,31 +4401,31 @@
         <v>154</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>259</v>
+        <v>300</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>260</v>
+        <v>301</v>
       </c>
       <c r="E13" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F13" t="s">
-        <v>261</v>
+        <v>302</v>
       </c>
       <c r="G13" t="s">
-        <v>262</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>194</v>
+        <v>303</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J13" t="s">
-        <v>263</v>
+        <v>304</v>
       </c>
       <c r="K13" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -4066,31 +4436,31 @@
         <v>154</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>265</v>
+        <v>306</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>266</v>
+        <v>307</v>
       </c>
       <c r="E14" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F14" t="s">
-        <v>267</v>
+        <v>308</v>
       </c>
       <c r="G14" t="s">
-        <v>268</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>194</v>
+        <v>309</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J14" t="s">
-        <v>269</v>
+        <v>310</v>
       </c>
       <c r="K14" t="s">
-        <v>270</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -4101,31 +4471,31 @@
         <v>154</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>271</v>
+        <v>312</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>272</v>
+        <v>313</v>
       </c>
       <c r="E15" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F15" t="s">
-        <v>273</v>
+        <v>314</v>
       </c>
       <c r="G15" t="s">
-        <v>274</v>
+        <v>315</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>194</v>
+        <v>316</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J15" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
       <c r="K15" t="s">
-        <v>276</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -4136,31 +4506,31 @@
         <v>154</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
       <c r="E16" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F16" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
       <c r="G16" t="s">
-        <v>280</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>194</v>
+        <v>322</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J16" t="s">
-        <v>282</v>
+        <v>324</v>
       </c>
       <c r="K16" t="s">
-        <v>283</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI Validations added V.10
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_Inputs.xlsx
+++ b/UploadExcel/TD_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00C771F-1EFE-4BCA-9E53-F5F7A2966FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08776715-6573-4995-9E22-8952FB98289B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HappyFlowData" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="326">
   <si>
     <t>ExecutionEnvironment</t>
   </si>
@@ -454,22 +454,22 @@
     <t>OrderID</t>
   </si>
   <si>
-    <t>7240387</t>
-  </si>
-  <si>
-    <t>7240397</t>
-  </si>
-  <si>
-    <t>7240403</t>
-  </si>
-  <si>
-    <t>Created Viax order 7240387 for PriceProposal 24ef6643-215b-4808-9127-af8e42410573</t>
-  </si>
-  <si>
-    <t>Created Viax order 7240397 for PriceProposal 24ef1880-885b-4808-9127-af8e42410529</t>
-  </si>
-  <si>
-    <t>Created Viax order 7240403 for PriceProposal 24ef9636-578b-4808-9127-af8e42410753</t>
+    <t>7242085</t>
+  </si>
+  <si>
+    <t>7242086</t>
+  </si>
+  <si>
+    <t>7242087</t>
+  </si>
+  <si>
+    <t>Created Viax order 7242085 for PriceProposal 24ef2384-235b-4808-9127-af8e42410930</t>
+  </si>
+  <si>
+    <t>Created Viax order 7242086 for PriceProposal 24ef7710-983b-4808-9127-af8e42410367</t>
+  </si>
+  <si>
+    <t>Created Viax order 7242087 for PriceProposal 24ef2007-947b-4808-9127-af8e42410687</t>
   </si>
   <si>
     <t>ResponseCode</t>
@@ -811,12 +811,155 @@
     <t>NA</t>
   </si>
   <si>
+    <t>Created Viax order 7242082 for PriceProposal 24ef6668-620b-4808-9127-af8e42410466</t>
+  </si>
+  <si>
+    <t>7242082</t>
+  </si>
+  <si>
+    <t>PriceDetermined</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn($data: Object) { testFunction(input: {name: \"receive-price-proposal-from-kafka\", data: {apiversion: \"1.0.1\", tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", id: \"51014872-8dfd-11ed-a1eb-0242ac120002\", type: \"priceproposal.requested\", source: \"urn:appcat:cmh-eeolink\", specversion: \"1.0\", subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", time: \"2019-08-24T14:15:22Z\", datacontenttype: \"application/json\", data: $data}}) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef6668-620b-4808-9127-af8e42410466",
+      "edRefCode": "ACN3-2023-06-0432",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-04-15",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [
+        "JCASP"
+      ],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7242082 for PriceProposal 24ef6668-620b-4808-9127-af8e42410466","version":"1.4.2-qa2.46","viaxPriceProposalId":"7242082","priceProposal":{"uid":"669493c1-499c-471f-b9d4-56dbf9039ae0","biId":"7242082","wAsSubmissionId":"24ef6668-620b-4808-9127-af8e42410466","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-15T03:13:05.538Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6668-620b-4808-9127-af8e42410466","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-15T03:13:06.116Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6668-620b-4808-9127-af8e42410466","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef6668-620b-4808-9127-af8e42410466","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Promotional discount</t>
   </si>
   <si>
     <t>Promotional</t>
   </si>
   <si>
+    <t>Created Viax order 7242083 for PriceProposal 24ef7692-465b-4808-9127-af8e42410586</t>
+  </si>
+  <si>
+    <t>7242083</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn($data: Object) { testFunction(input: {name: \"receive-price-proposal-from-kafka\", data: {apiversion: \"1.0.1\", tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", id: \"51014872-8dfd-11ed-a1eb-0242ac120002\", type: \"priceproposal.requested\", source: \"urn:appcat:cmh-eeolink\", specversion: \"1.0\", subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", time: \"2019-08-24T14:15:22Z\", datacontenttype: \"application/json\", data: $data}}) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef7692-465b-4808-9127-af8e42410586",
+      "edRefCode": "ACN3-2023-06-0432",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-04-15",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [
+		"PROMO50"
+	  ],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7242083 for PriceProposal 24ef7692-465b-4808-9127-af8e42410586","version":"1.4.2-qa2.46","viaxPriceProposalId":"7242083","priceProposal":{"uid":"66949436-0a47-42b1-853e-57add7bcee60","biId":"7242083","wAsSubmissionId":"24ef7692-465b-4808-9127-af8e42410586","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-15T03:15:02.703Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef7692-465b-4808-9127-af8e42410586","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-15T03:15:03.258Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]}],"appliedDiscounts":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef7692-465b-4808-9127-af8e42410586","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef7692-465b-4808-9127-af8e42410586","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Institutional discount</t>
   </si>
   <si>
@@ -824,6 +967,74 @@
   </si>
   <si>
     <t>E O Lawrence Berkeley National Laboratory</t>
+  </si>
+  <si>
+    <t>Created Viax order 7242084 for PriceProposal 24ef9485-611b-4808-9127-af8e42410371</t>
+  </si>
+  <si>
+    <t>7242084</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
+      "submissionId": "24ef9485-611b-4808-9127-af8e42410371",
+      "edRefCode": "ACN3-2023-06-0432",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-04-16",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "1666",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7242084 for PriceProposal 24ef9485-611b-4808-9127-af8e42410371","version":"1.4.2-qa2.46","viaxPriceProposalId":"7242084","priceProposal":{"uid":"669494ac-d0db-4a5e-be7c-94119dcf54a2","biId":"7242084","wAsSubmissionId":"24ef9485-611b-4808-9127-af8e42410371","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-15T03:17:00.183Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef9485-611b-4808-9127-af8e42410371","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-16","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-15T03:17:01.179Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O Lawrence Berkeley National Laboratory","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":800,"price":200,"subtotal":0,"tax":0,"total":0,"discountAmount":200,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef9485-611b-4808-9127-af8e42410371","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef9485-611b-4808-9127-af8e42410371","wAsSubmissionDate":"2024-04-16","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Editorial discount</t>
@@ -1011,7 +1222,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1072,6 +1283,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1111,7 +1328,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1133,19 +1350,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2170,10 +2400,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2188,13 +2418,13 @@
       <c r="A1" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2202,13 +2432,13 @@
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="19" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2216,13 +2446,13 @@
       <c r="A3" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="19" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2230,13 +2460,13 @@
       <c r="A4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="19" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2244,13 +2474,13 @@
       <c r="A5" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="19" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2258,13 +2488,13 @@
       <c r="A6" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="20" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2272,13 +2502,13 @@
       <c r="A7" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="20" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2286,13 +2516,13 @@
       <c r="A8" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="20" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2300,13 +2530,13 @@
       <c r="A9" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="21" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2314,13 +2544,13 @@
       <c r="A10" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="19" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2328,13 +2558,13 @@
       <c r="A11" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="24" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2342,13 +2572,13 @@
       <c r="A12" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="19" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2356,13 +2586,13 @@
       <c r="A13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="19" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2370,13 +2600,13 @@
       <c r="A14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="19" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2384,13 +2614,13 @@
       <c r="A15" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="19" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2398,13 +2628,13 @@
       <c r="A16" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="25" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2412,13 +2642,13 @@
       <c r="A17" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="19" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2426,13 +2656,13 @@
       <c r="A18" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="21">
         <v>2221</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="21" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2440,13 +2670,13 @@
       <c r="A19" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="21" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2454,13 +2684,13 @@
       <c r="A20" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="21" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2468,13 +2698,13 @@
       <c r="A21" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="19" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2482,13 +2712,13 @@
       <c r="A22" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="21" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2496,13 +2726,13 @@
       <c r="A23" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="19" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2510,13 +2740,13 @@
       <c r="A24" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="21" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2524,13 +2754,13 @@
       <c r="A25" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="19" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2538,13 +2768,13 @@
       <c r="A26" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="21" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2552,13 +2782,13 @@
       <c r="A27" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="21" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2566,13 +2796,13 @@
       <c r="A28" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="21" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2580,13 +2810,13 @@
       <c r="A29" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="21" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2594,13 +2824,13 @@
       <c r="A30" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="21" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2608,13 +2838,13 @@
       <c r="A31" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="21" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2622,13 +2852,13 @@
       <c r="A32" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="21" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2636,13 +2866,13 @@
       <c r="A33" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="21" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2650,13 +2880,13 @@
       <c r="A34" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="21" t="s">
         <v>212</v>
       </c>
     </row>
@@ -2664,13 +2894,13 @@
       <c r="A35" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="21" t="s">
         <v>214</v>
       </c>
     </row>
@@ -2678,13 +2908,13 @@
       <c r="A36" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="21" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2692,13 +2922,13 @@
       <c r="A37" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="21" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2706,13 +2936,13 @@
       <c r="A38" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="26" t="s">
         <v>220</v>
       </c>
     </row>
@@ -2720,13 +2950,13 @@
       <c r="A39" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="21" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2734,13 +2964,13 @@
       <c r="A40" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="21" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2748,13 +2978,13 @@
       <c r="A41" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="21" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2762,13 +2992,13 @@
       <c r="A42" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="26" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2776,13 +3006,13 @@
       <c r="A43" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="21" t="s">
         <v>230</v>
       </c>
     </row>
@@ -2790,13 +3020,13 @@
       <c r="A44" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="21" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2804,13 +3034,13 @@
       <c r="A45" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="21" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2818,13 +3048,13 @@
       <c r="A46" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="26" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2832,13 +3062,13 @@
       <c r="A47" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="21" t="s">
         <v>235</v>
       </c>
     </row>
@@ -2846,15 +3076,20 @@
       <c r="A48" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="21" t="s">
         <v>229</v>
       </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="19"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2870,9 +3105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AI5" sqref="AI5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
@@ -2999,10 +3232,10 @@
       <c r="E2" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="17" t="s">
         <v>23</v>
       </c>
       <c r="H2" t="s">
@@ -3034,6 +3267,24 @@
       </c>
       <c r="Z2" t="s">
         <v>261</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>263</v>
+      </c>
+      <c r="AF2" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="AG2" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:35">
@@ -3044,27 +3295,27 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="E3" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="15" t="s">
         <v>214</v>
       </c>
       <c r="H3" t="s">
         <v>261</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="15" t="s">
         <v>218</v>
       </c>
       <c r="N3" t="s">
@@ -3079,14 +3330,32 @@
       <c r="T3" t="s">
         <v>261</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="X3" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y3" s="18" t="s">
+      <c r="Y3" s="15" t="s">
         <v>223</v>
       </c>
       <c r="Z3" t="s">
         <v>261</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>270</v>
+      </c>
+      <c r="AF3" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="AG3" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:35">
@@ -3097,28 +3366,28 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="E4" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>265</v>
+      <c r="G4" s="15" t="s">
+        <v>274</v>
       </c>
       <c r="H4" t="s">
         <v>261</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="M4" s="18" t="s">
-        <v>266</v>
+      <c r="M4" s="15" t="s">
+        <v>275</v>
       </c>
       <c r="N4" t="s">
         <v>261</v>
@@ -3126,20 +3395,38 @@
       <c r="R4">
         <v>75</v>
       </c>
-      <c r="S4" s="18" t="s">
+      <c r="S4" s="15" t="s">
         <v>261</v>
       </c>
       <c r="T4" t="s">
         <v>261</v>
       </c>
-      <c r="X4" s="18" t="s">
+      <c r="X4" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="18" t="s">
+      <c r="Y4" s="15" t="s">
         <v>223</v>
       </c>
       <c r="Z4" t="s">
         <v>261</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>276</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>277</v>
+      </c>
+      <c r="AF4" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="AG4" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:35">
@@ -3150,28 +3437,28 @@
         <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="E5" t="s">
         <v>156</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>269</v>
+      <c r="G5" s="15" t="s">
+        <v>282</v>
       </c>
       <c r="H5" t="s">
         <v>261</v>
       </c>
-      <c r="L5" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>271</v>
+      <c r="L5" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>284</v>
       </c>
       <c r="N5" t="s">
         <v>261</v>
@@ -3185,10 +3472,10 @@
       <c r="T5" t="s">
         <v>261</v>
       </c>
-      <c r="X5" s="18" t="s">
+      <c r="X5" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y5" s="18" t="s">
+      <c r="Y5" s="15" t="s">
         <v>223</v>
       </c>
       <c r="Z5" t="s">
@@ -3203,27 +3490,27 @@
         <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="E6" t="s">
-        <v>274</v>
-      </c>
-      <c r="F6" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>275</v>
+      <c r="G6" s="15" t="s">
+        <v>288</v>
       </c>
       <c r="H6" t="s">
         <v>261</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="15" t="s">
         <v>261</v>
       </c>
       <c r="N6" t="s">
@@ -3238,10 +3525,10 @@
       <c r="T6" t="s">
         <v>261</v>
       </c>
-      <c r="X6" s="18" t="s">
+      <c r="X6" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y6" s="18" t="s">
+      <c r="Y6" s="15" t="s">
         <v>223</v>
       </c>
       <c r="Z6" t="s">
@@ -3256,28 +3543,28 @@
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="E7" t="s">
-        <v>278</v>
-      </c>
-      <c r="F7" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>279</v>
+      <c r="G7" s="15" t="s">
+        <v>292</v>
       </c>
       <c r="H7" t="s">
         <v>261</v>
       </c>
-      <c r="L7" s="18" t="s">
+      <c r="L7" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="M7" s="18" t="s">
-        <v>280</v>
+      <c r="M7" s="15" t="s">
+        <v>293</v>
       </c>
       <c r="N7" t="s">
         <v>261</v>
@@ -3291,10 +3578,10 @@
       <c r="T7" t="s">
         <v>261</v>
       </c>
-      <c r="X7" s="18" t="s">
+      <c r="X7" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y7" s="18" t="s">
+      <c r="Y7" s="15" t="s">
         <v>223</v>
       </c>
       <c r="Z7" t="s">
@@ -3309,7 +3596,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>212</v>
@@ -3317,19 +3604,19 @@
       <c r="E8" t="s">
         <v>156</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="15" t="s">
         <v>261</v>
       </c>
       <c r="H8" t="s">
         <v>261</v>
       </c>
-      <c r="L8" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="M8" s="18" t="s">
+      <c r="L8" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="M8" s="15" t="s">
         <v>261</v>
       </c>
       <c r="N8" t="s">
@@ -3338,16 +3625,16 @@
       <c r="R8">
         <v>75</v>
       </c>
-      <c r="S8" s="18" t="s">
+      <c r="S8" s="15" t="s">
         <v>261</v>
       </c>
       <c r="T8" t="s">
         <v>261</v>
       </c>
-      <c r="X8" s="18" t="s">
+      <c r="X8" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y8" s="18" t="s">
+      <c r="Y8" s="15" t="s">
         <v>261</v>
       </c>
       <c r="Z8" t="s">
@@ -3362,19 +3649,19 @@
         <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G9" s="18" t="s">
-        <v>265</v>
+      <c r="G9" s="15" t="s">
+        <v>274</v>
       </c>
       <c r="H9" t="s">
         <v>261</v>
@@ -3382,11 +3669,11 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="M9" s="18" t="s">
-        <v>266</v>
+      <c r="M9" s="15" t="s">
+        <v>275</v>
       </c>
       <c r="N9" t="s">
         <v>261</v>
@@ -3397,7 +3684,7 @@
       <c r="R9" s="7">
         <v>75</v>
       </c>
-      <c r="S9" s="18" t="s">
+      <c r="S9" s="15" t="s">
         <v>261</v>
       </c>
       <c r="T9" t="s">
@@ -3435,30 +3722,30 @@
       <c r="E10" t="s">
         <v>156</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18" t="s">
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="N10" s="18" t="s">
+      <c r="N10" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
       <c r="R10">
         <v>75</v>
       </c>
@@ -3468,10 +3755,10 @@
       <c r="T10">
         <v>5</v>
       </c>
-      <c r="X10" s="18" t="s">
+      <c r="X10" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y10" s="18" t="s">
+      <c r="Y10" s="15" t="s">
         <v>223</v>
       </c>
       <c r="Z10" t="s">
@@ -3486,59 +3773,59 @@
         <v>18</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="E11" t="s">
         <v>156</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="G11" s="18" t="s">
+      <c r="F11" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H11" t="s">
         <v>261</v>
       </c>
-      <c r="L11" s="18" t="s">
-        <v>287</v>
-      </c>
-      <c r="M11" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="N11" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
+      <c r="L11" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
       <c r="R11">
         <v>50</v>
       </c>
       <c r="S11">
         <v>50</v>
       </c>
-      <c r="T11" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18" t="s">
+      <c r="T11" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y11" s="18" t="s">
+      <c r="Y11" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Z11" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
+      <c r="Z11" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
     </row>
     <row r="12" spans="1:35">
       <c r="A12" t="s">
@@ -3548,81 +3835,81 @@
         <v>18</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="E12" t="s">
         <v>156</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G12" s="18" t="s">
-        <v>269</v>
+      <c r="G12" s="15" t="s">
+        <v>282</v>
       </c>
       <c r="H12" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="I12" t="s">
-        <v>291</v>
-      </c>
-      <c r="J12" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="J12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="L12" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="N12" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="P12" s="18" t="s">
+      <c r="L12" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="P12" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="Q12" s="18" t="s">
+      <c r="Q12" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="R12" s="18">
+      <c r="R12" s="15">
         <v>75</v>
       </c>
       <c r="S12">
         <v>90</v>
       </c>
-      <c r="T12" s="18">
+      <c r="T12" s="15">
         <v>50</v>
       </c>
-      <c r="U12" s="18">
+      <c r="U12" s="15">
         <v>50</v>
       </c>
-      <c r="V12" s="18">
+      <c r="V12" s="15">
         <v>5</v>
       </c>
-      <c r="W12" s="18">
+      <c r="W12" s="15">
         <v>20</v>
       </c>
-      <c r="X12" s="18" t="s">
+      <c r="X12" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y12" s="18" t="s">
+      <c r="Y12" s="15" t="s">
         <v>223</v>
       </c>
       <c r="Z12" t="s">
         <v>235</v>
       </c>
-      <c r="AA12" s="18" t="s">
+      <c r="AA12" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="AB12" s="18" t="s">
+      <c r="AB12" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="AC12" s="18" t="s">
+      <c r="AC12" s="15" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3634,59 +3921,59 @@
         <v>18</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="E13" t="s">
         <v>156</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="G13" s="18" t="s">
+      <c r="F13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>261</v>
       </c>
       <c r="H13" t="s">
         <v>261</v>
       </c>
-      <c r="L13" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="M13" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="N13" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="S13" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="T13" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="Y13" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="Z13" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
+      <c r="L13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="S13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="T13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
     </row>
     <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1">
       <c r="A14" t="s">
@@ -3704,113 +3991,113 @@
       <c r="E14" t="s">
         <v>156</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="M14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="N14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="S14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="T14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="Y14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="Z14" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
+      <c r="F14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="T14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
     </row>
     <row r="15" spans="1:35">
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="E15" t="s">
         <v>156</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H15" t="s">
         <v>261</v>
       </c>
-      <c r="L15" s="18" t="s">
+      <c r="L15" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="M15" s="19" t="s">
+      <c r="M15" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="N15" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
+      <c r="N15" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
       <c r="R15">
         <v>75</v>
       </c>
       <c r="S15">
         <v>5</v>
       </c>
-      <c r="T15" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18" t="s">
+      <c r="T15" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y15" s="18" t="s">
+      <c r="Y15" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Z15" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA15" s="18"/>
-      <c r="AB15" s="18"/>
-      <c r="AC15" s="18"/>
+      <c r="Z15" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
     </row>
     <row r="16" spans="1:35">
       <c r="A16" t="s">
@@ -3820,131 +4107,131 @@
         <v>18</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="E16" t="s">
         <v>156</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="15" t="s">
         <v>214</v>
       </c>
       <c r="H16" t="s">
         <v>261</v>
       </c>
-      <c r="L16" s="18" t="s">
+      <c r="L16" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="M16" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="N16" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
+      <c r="M16" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
       <c r="R16">
         <v>75</v>
       </c>
       <c r="S16" t="s">
         <v>261</v>
       </c>
-      <c r="T16" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18" t="s">
+      <c r="T16" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y16" s="18" t="s">
+      <c r="Y16" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="Z16" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
-      <c r="AC16" s="18"/>
+      <c r="Z16" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="E17" t="s">
         <v>156</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18" t="s">
+      <c r="H17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="M17" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="N17" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
+      <c r="M17" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
       <c r="R17">
         <v>75</v>
       </c>
-      <c r="S17" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="T17" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18" t="s">
+      <c r="S17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="T17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="Y17" s="18" t="s">
+      <c r="Y17" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="Z17" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
+      <c r="Z17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="E18" t="s">
         <v>156</v>
@@ -3955,10 +4242,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="E19" t="s">
         <v>156</v>
@@ -3969,10 +4256,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="D20" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="E20" t="s">
         <v>156</v>
@@ -3983,10 +4270,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="D21" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="E21" t="s">
         <v>156</v>
@@ -3997,10 +4284,10 @@
         <v>18</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="D22" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="E22" t="s">
         <v>156</v>

</xml_diff>

<commit_message>
UI Validations added V.27
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_Inputs.xlsx
+++ b/UploadExcel/TD_Inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21523A06-435C-4196-AA9E-8480B1233238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34EAAB5-2723-446E-94E7-3DE45627DDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HappyFlowData" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="325">
   <si>
     <t>ExecutionEnvironment</t>
   </si>
@@ -986,68 +986,16 @@
     <t>UnPaidNewCustomer</t>
   </si>
   <si>
-    <t>3213528</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213528 for AS order 20240724115240</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 0d523810-099a-4e82-bd65-0a0c16c03cb8","Using soldTo : 0d523810-099a-4e82-bd65-0a0c16c03cb8","Using billTo: 0d523810-099a-4e82-bd65-0a0c16c03cb8","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213528 for AS order 20240724115240","version":"1.3.3-qa2.92","biId":"3213528"}}'}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e754a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240724115240 submittedDate: \"2024-07-24T15:00:14-05\" createdDate: \"2024-07-24T15:00:14-05\" cancelDate: \"2024-07-24T15:00:14-05\" paymentDate: \"2024-07-24T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-07-24T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-24\" vatIdNumber: \"\" countryCode: \"IS\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f32600759\" title: \"Secrets of nature\" dhId: \"e0c7047c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/ibi.38363\" } soldToDetails: { firstName: \"20240724115240Test\" lastName: \"20240724115240Auto\" email: \"20240724115240@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1080.00, billingAddress: { firstName: \"20240724115240Test\" lastName: \"20240724115240Auto\" streetAddress: [\"Lindarbraut 5\"] addressLocality: \"Laugarvatn\" addressRegion: \"8\" countryCode: \"IS\" postalCode: \"840\" phoneNumber: \"003545254000\" email: \"20240724115240@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e754a\" } } ] } }\t) { status data\t}}"
-}
-</t>
-  </si>
-  <si>
-    <t>2024-07-24 11:52:40.035</t>
-  </si>
-  <si>
     <t>Trigger CreditCard Order with New Customer</t>
   </si>
   <si>
     <t>CreditCardNewCustomer</t>
   </si>
   <si>
-    <t>3213529</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213529 for AS order 20240724115242</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP cb12cb1e-fba2-49b9-970f-ba42ff2cc8af","Using soldTo : cb12cb1e-fba2-49b9-970f-ba42ff2cc8af","Using billTo: cb12cb1e-fba2-49b9-970f-ba42ff2cc8af","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213529 for AS order 20240724115242","version":"1.3.3-qa2.92","biId":"3213529"}}'}}}</t>
-  </si>
-  <si>
-    <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e823a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-10-10T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240724115242 submittedDate: \"2024-07-24T15:00:14-05\" createdDate: \"2024-07-24T15:00:14-05\" cancelDate: \"2024-07-24T15:00:14-05\" paymentDate: \"2024-07-24T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2024-07-24T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CC order &lt;&lt;CURRENCY&gt;&gt; form validation\" apc: 1100.00 appliedDiscount: 200.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"GB564291137\" countryCode: \"GB\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f23495525\" title: \"Secrets of volcano\" dhId: \"e0c2068c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240724115242Test\" lastName: \"20240724115242Auto\" email: \"20240724115242@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 1080.00 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2024-07-24T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240724115242Test\" lastName: \"20240724115242Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"260 Edison Park\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"+44 1793 528342\" email: \"20240724115242@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e823a\" } } ] } }\t) { status data\t}}"
-}</t>
-  </si>
-  <si>
-    <t>2024-07-24 11:52:42.471</t>
-  </si>
-  <si>
     <t>Trigger Alipay Order with New Customer</t>
   </si>
   <si>
     <t>AlipayNewCustomer</t>
-  </si>
-  <si>
-    <t>3213530</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213530 for AS order 20240724115245</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP cfbd48fd-2e75-4ab1-a222-18a20241e8f3","Using soldTo : cfbd48fd-2e75-4ab1-a222-18a20241e8f3","Using billTo: cfbd48fd-2e75-4ab1-a222-18a20241e8f3","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213530 for AS order 20240724115245","version":"1.3.3-qa2.92","biId":"3213530"}}'}}}</t>
-  </si>
-  <si>
-    <t>{
-	"query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240724115245 submittedDate: \"2024-07-24T15:00:14-05\" createdDate: \"2024-07-24T15:00:14-05\" cancelDate: \"2024-07-24T15:00:14-05\" paymentDate: \"2024-07-24T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2024-07-24T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 0 discountType: \"Society\" estimatedTax: 0 totalChargedAmount: 1080.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f73332373\" title: \"Secrets of nature\" dhId: \"e0c2581c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240724115245Test\" lastName: \"20240724115245Auto\" email: \"20240724115245@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 1080.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2039-06-29 08:00:00\" } billingAddress: { firstName: \"20240724115245Test\" lastName: \"20240724115245Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"257 Sanxiang Road\"] addressLocality: \"SHenchou - Futian District\" addressRegion: \"GD\" countryCode: \"CN\" postalCode: \"1234435\" phoneNumber: \"0703503263\" email: \"20240724115245@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" } } ] } }\t) { status data\t}}"
-}</t>
-  </si>
-  <si>
-    <t>2024-07-24 11:52:45.100</t>
   </si>
   <si>
     <t>Verify UI Change Data Correction to Price Determined</t>
@@ -1099,7 +1047,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1160,12 +1108,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor rgb="FF00FF00"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1205,7 +1147,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1241,7 +1183,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2268,7 +2209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -3515,17 +3456,17 @@
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="23" t="s">
-        <v>339</v>
-      </c>
-      <c r="D25" s="23" t="s">
+      <c r="C25" s="22" t="s">
+        <v>324</v>
+      </c>
+      <c r="D25" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="21" t="s">
         <v>172</v>
       </c>
       <c r="F25" t="s">
@@ -3552,7 +3493,7 @@
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
-      <c r="R25" s="22">
+      <c r="R25" s="21">
         <v>75</v>
       </c>
       <c r="S25" s="15" t="s">
@@ -4287,8 +4228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4347,55 +4288,19 @@
       <c r="D2" t="s">
         <v>319</v>
       </c>
-      <c r="E2" t="s">
-        <v>320</v>
-      </c>
-      <c r="F2" t="s">
-        <v>321</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="H2" t="s">
-        <v>322</v>
-      </c>
-      <c r="I2" t="s">
-        <v>323</v>
-      </c>
-      <c r="J2" t="s">
-        <v>324</v>
-      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>326</v>
-      </c>
-      <c r="E3" t="s">
-        <v>327</v>
-      </c>
-      <c r="F3" t="s">
-        <v>328</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="H3" t="s">
-        <v>329</v>
-      </c>
-      <c r="I3" t="s">
-        <v>330</v>
-      </c>
-      <c r="J3" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -4403,31 +4308,13 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E4" t="s">
-        <v>334</v>
-      </c>
-      <c r="F4" t="s">
-        <v>335</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="H4" t="s">
-        <v>336</v>
-      </c>
-      <c r="I4" t="s">
-        <v>337</v>
-      </c>
-      <c r="J4" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI Validations added V.36
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_Inputs.xlsx
+++ b/UploadExcel/TD_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFC71A5-1417-42A0-B27F-2A4781E83300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F709D191-E3ED-4496-9D1A-8393BDC1E0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="380">
   <si>
     <t>ExecutionEnvironment</t>
   </si>
@@ -532,6 +532,9 @@
     <t>PriceProposalStatus</t>
   </si>
   <si>
+    <t>SubmissionID</t>
+  </si>
+  <si>
     <t>ResponseStatusCode</t>
   </si>
   <si>
@@ -559,6 +562,82 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>Created Viax order 7256059 for PriceProposal 24ef7029-691b-4808-9127-af8e42410263</t>
+  </si>
+  <si>
+    <t>24ef7029-691b-4808-9127-af8e42410263</t>
+  </si>
+  <si>
+    <t>PriceDetermined</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn($data: Object) { testFunction(input: {name: \"receive-price-proposal-from-kafka\", data: {apiversion: \"1.0.1\", tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", id: \"51014872-8dfd-11ed-a1eb-0242ac120002\", type: \"priceproposal.requested\", source: \"urn:appcat:cmh-eeolink\", specversion: \"1.0\", subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", time: \"2019-08-24T14:15:22Z\", datacontenttype: \"application/json\", data: $data}}) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef7029-691b-4808-9127-af8e42410263",
+      "edRefCode": "ACN3-2023-06-7029",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [
+        "JCASP"
+      ],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256059 for PriceProposal 24ef7029-691b-4808-9127-af8e42410263","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256059","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef7029-691b-4808-9127-af8e42410263","version":"1.6.6-qa2.75","submissionId":"24ef7029-691b-4808-9127-af8e42410263","priceProposal":{"uid":"66ac3eb2-3a46-4e41-9d58-3e8da76eb4ec","biId":"7256059","wAsSubmissionId":"24ef7029-691b-4808-9127-af8e42410263","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:04:34.613Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef7029-691b-4808-9127-af8e42410263","edRefCode":"ACN3-2023-06-7029","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:04:35.965Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef7029-691b-4808-9127-af8e42410263","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-7029","wAsSubmissionId":"24ef7029-691b-4808-9127-af8e42410263","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Promotional discount</t>
   </si>
   <si>
@@ -571,6 +650,76 @@
     <t>PROMO50</t>
   </si>
   <si>
+    <t>Created Viax order 7256064 for PriceProposal 24ef3531-304b-4808-9127-af8e42410422</t>
+  </si>
+  <si>
+    <t>7256064</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn($data: Object) { testFunction(input: {name: \"receive-price-proposal-from-kafka\", data: {apiversion: \"1.0.1\", tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", id: \"51014872-8dfd-11ed-a1eb-0242ac120002\", type: \"priceproposal.requested\", source: \"urn:appcat:cmh-eeolink\", specversion: \"1.0\", subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", time: \"2019-08-24T14:15:22Z\", datacontenttype: \"application/json\", data: $data}}) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef3531-304b-4808-9127-af8e42410422",
+      "edRefCode": "ACN3-2023-06-3531",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [
+		"PROMO50"
+	  ],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256064 for PriceProposal 24ef3531-304b-4808-9127-af8e42410422","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256064","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef3531-304b-4808-9127-af8e42410422","version":"1.6.6-qa2.75","submissionId":"24ef3531-304b-4808-9127-af8e42410422","priceProposal":{"uid":"66ac3f4c-0655-4e45-a427-cc11f656672d","biId":"7256064","wAsSubmissionId":"24ef3531-304b-4808-9127-af8e42410422","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:07:08.820Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef3531-304b-4808-9127-af8e42410422","edRefCode":"ACN3-2023-06-3531","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:07:09.452Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef3531-304b-4808-9127-af8e42410422","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-3531","wAsSubmissionId":"24ef3531-304b-4808-9127-af8e42410422","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Institutional discount</t>
   </si>
   <si>
@@ -580,6 +729,74 @@
     <t>E O Lawrence Berkeley National Laboratory</t>
   </si>
   <si>
+    <t>Created Viax order 7256065 for PriceProposal 24ef5609-371b-4808-9127-af8e42410508</t>
+  </si>
+  <si>
+    <t>7256065</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
+      "submissionId": "24ef5609-371b-4808-9127-af8e42410508",
+      "edRefCode": "ACN3-2023-06-5609",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "1666",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256065 for PriceProposal 24ef5609-371b-4808-9127-af8e42410508","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256065","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5609-371b-4808-9127-af8e42410508","version":"1.6.6-qa2.75","submissionId":"24ef5609-371b-4808-9127-af8e42410508","priceProposal":{"uid":"66ac3fc0-40d1-4ff5-ac8c-3187a8427aaf","biId":"7256065","wAsSubmissionId":"24ef5609-371b-4808-9127-af8e42410508","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:09:04.593Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef5609-371b-4808-9127-af8e42410508","edRefCode":"ACN3-2023-06-5609","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:09:05.628Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O Lawrence Berkeley National Laboratory","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":800,"price":200,"subtotal":0,"tax":0,"total":0,"discountAmount":200,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5609-371b-4808-9127-af8e42410508","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5609","wAsSubmissionId":"24ef5609-371b-4808-9127-af8e42410508","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Editorial discount</t>
   </si>
   <si>
@@ -595,6 +812,75 @@
     <t>CCCAM424</t>
   </si>
   <si>
+    <t>Created Viax order 7256066 for PriceProposal 24ef8753-169b-4808-9127-af8e42410833</t>
+  </si>
+  <si>
+    <t>7256066</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
+      "submissionId": "24ef8753-169b-4808-9127-af8e42410833",
+      "edRefCode": "ACN3-2023-06-8753",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "OPINION",
+      "displayArticleType": "OPINION",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "editorialDiscountCode": "CCCAM424",
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256066 for PriceProposal 24ef8753-169b-4808-9127-af8e42410833","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256066","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef8753-169b-4808-9127-af8e42410833","version":"1.6.6-qa2.75","submissionId":"24ef8753-169b-4808-9127-af8e42410833","priceProposal":{"uid":"66ac4033-2374-4754-b2b4-bada0bdf8570","biId":"7256066","wAsSubmissionId":"24ef8753-169b-4808-9127-af8e42410833","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:10:59.905Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef8753-169b-4808-9127-af8e42410833","edRefCode":"ACN3-2023-06-8753","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"OPINION","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"CCCAM424","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:11:00.635Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":640,"subtotal":64,"tax":0,"total":64,"discountAmount":576,"discountPercentage":90,"currencyCode":"USD","allDiscounts":[{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":576,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":576,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef8753-169b-4808-9127-af8e42410833","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-8753","wAsSubmissionId":"24ef8753-169b-4808-9127-af8e42410833","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"OPINION","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Referral discount</t>
   </si>
   <si>
@@ -607,6 +893,75 @@
     <t xml:space="preserve"> ReferralDiscount</t>
   </si>
   <si>
+    <t>Created Viax order 7256067 for PriceProposal 24ef6431-765b-4808-9127-af8e42410118</t>
+  </si>
+  <si>
+    <t>7256067</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
+      "submissionId": "24ef6431-765b-4808-9127-af8e42410118",
+      "edRefCode": "ACN3-2023-06-6431",
+      "articleDOI": "",
+      "journalId": "e1bbb7b4-5369-4c40-a53a-aa3dc55390a6",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2024-02-10",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "Hi",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "referringJournalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "authors": [
+        {
+          "role": "CorrespondingAuthor",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "anagarajan@wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "AixenProvence",
+              "countryCode": "IN",
+              "country": "IN",
+              "institution": "GrantInstitute",
+              "department": "SchoolofGeoSciences",
+              "stateProvince": "AndhraPradesh",
+              "postalCode": "500072",
+              "streetAddress": [
+                "1832ColvinAve"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256067 for PriceProposal 24ef6431-765b-4808-9127-af8e42410118","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256067","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef6431-765b-4808-9127-af8e42410118","version":"1.6.6-qa2.75","submissionId":"24ef6431-765b-4808-9127-af8e42410118","priceProposal":{"uid":"66ac40a9-caee-4ba5-a2c3-a10b6c265687","biId":"7256067","wAsSubmissionId":"24ef6431-765b-4808-9127-af8e42410118","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:12:57.417Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef6431-765b-4808-9127-af8e42410118","edRefCode":"ACN3-2023-06-6431","articleDOI":"","journalId":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2024-02-10","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"Hi","societyCodes":[],"promoCodes":[],"discountCodes":[],"referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"anagarajan@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"AixenProvence","countryCode":"IN","country":"IN","institution":"GrantInstitute","department":"SchoolofGeoSciences","stateProvince":"AndhraPradesh","postalCode":"500072","streetAddress":["1832ColvinAve"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:12:57.960Z"}},"wAsCountryCode":"IN","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsReferringJournalRef":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalEISSN":"20457634","wAsEditorialOfficeEmail":"cancermed@wiley.com"},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":1000,"price":900,"subtotal":762.75,"tax":0,"total":762.75,"discountAmount":137.25,"discountPercentage":15.25,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":100,"discountPercentage":10,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"","discountType":"ReferralDiscount","discountAmount":137.25,"discountPercentage":15.25,"discountDescription":"","sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","attribute":"wAsJournalUuid"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsReferringJournal"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ReferralDiscount","discountAmount":137.25,"discountPercentage":15.25,"discountDescription":"","sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":100,"discountPercentage":10,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"Hi","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"anagarajan@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"GrantInstitute","countryCode":"IN","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6431-765b-4808-9127-af8e42410118","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6431","wAsSubmissionId":"24ef6431-765b-4808-9127-af8e42410118","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2024-02-10","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"JCSM","maName":"Journal of Cachexia, Sarcopenia and Muscle","wAsJournalUuid":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"21906009x","wAsFlipDate":null,"wAsJournalTitle":"Journal of Cachexia, Sarcopenia and Muscle","wAsJournalGroupCode":"JCSM","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"JCSM1@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Geographical discount</t>
   </si>
   <si>
@@ -622,18 +977,222 @@
     <t>MH - Marshall Islands</t>
   </si>
   <si>
+    <t>Created Viax order 7256068 for PriceProposal 24ef4678-427b-4808-9127-af8e42410478</t>
+  </si>
+  <si>
+    <t>7256068</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
+      "submissionId": "24ef4678-427b-4808-9127-af8e42410478",
+      "edRefCode": "ACN3-2023-06-4678",
+      "articleDOI": "",
+      "journalId": "b6d18dc5-3811-4b21-81f0-a01997c20001",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "MH",
+              "country": "MH",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256068 for PriceProposal 24ef4678-427b-4808-9127-af8e42410478","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256068","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef4678-427b-4808-9127-af8e42410478","version":"1.6.6-qa2.75","submissionId":"24ef4678-427b-4808-9127-af8e42410478","priceProposal":{"uid":"66ac4117-e784-4aac-b77e-f34fd981e4ab","biId":"7256068","wAsSubmissionId":"24ef4678-427b-4808-9127-af8e42410478","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:14:47.699Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef4678-427b-4808-9127-af8e42410478","edRefCode":"ACN3-2023-06-4678","articleDOI":"","journalId":"b6d18dc5-3811-4b21-81f0-a01997c20001","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"MH","country":"MH","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:14:48.943Z"}},"wAsCountryCode":"MH","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":300,"price":210,"subtotal":0,"tax":0,"total":0,"discountAmount":210,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":210,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"MH","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":90,"discountPercentage":30,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"b6d18dc5-3811-4b21-81f0-a01997c20001","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":210,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":90,"discountPercentage":30,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"MH","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4678-427b-4808-9127-af8e42410478","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4678","wAsSubmissionId":"24ef4678-427b-4808-9127-af8e42410478","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article","ibrProduct":{"maId":"CCR3","maName":"Clinical Case Reports","wAsJournalUuid":"b6d18dc5-3811-4b21-81f0-a01997c20001","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20500904","wAsFlipDate":null,"wAsJournalTitle":"Clinical Case Reports","wAsJournalGroupCode":"CCR3","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"clinicalcases@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Article type discount</t>
   </si>
   <si>
     <t>RESEARCH ARTICLE</t>
   </si>
   <si>
+    <t>Created Viax order 7256069 for PriceProposal 24ef5134-691b-4808-9127-af8e42410536</t>
+  </si>
+  <si>
+    <t>7256069</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
+      "submissionId": "24ef5134-691b-4808-9127-af8e42410536",
+      "edRefCode": "ACN3-2023-06-5134",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "RESEARCH ARTICLE",
+      "displayArticleType": "RESEARCH ARTICLE",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256069 for PriceProposal 24ef5134-691b-4808-9127-af8e42410536","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256069","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5134-691b-4808-9127-af8e42410536","version":"1.6.6-qa2.75","submissionId":"24ef5134-691b-4808-9127-af8e42410536","priceProposal":{"uid":"66ac418c-22ca-4269-97a2-d9b302041348","biId":"7256069","wAsSubmissionId":"24ef5134-691b-4808-9127-af8e42410536","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:16:44.642Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef5134-691b-4808-9127-af8e42410536","edRefCode":"ACN3-2023-06-5134","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:16:45.302Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5134-691b-4808-9127-af8e42410536","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5134","wAsSubmissionId":"24ef5134-691b-4808-9127-af8e42410536","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Stacked Institutional discount</t>
   </si>
   <si>
     <t>Stacked</t>
   </si>
   <si>
+    <t>Created Viax order 7256070 for PriceProposal 24ef3341-758b-4808-9127-af8e42410499</t>
+  </si>
+  <si>
+    <t>7256070</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
+      "submissionId": "24ef3341-758b-4808-9127-af8e42410499",
+      "edRefCode": "ACN3-2023-06-3341",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "1666",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "GB",
+              "country": "UK",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256070 for PriceProposal 24ef3341-758b-4808-9127-af8e42410499","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256070","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef3341-758b-4808-9127-af8e42410499","version":"1.6.6-qa2.75","submissionId":"24ef3341-758b-4808-9127-af8e42410499","priceProposal":{"uid":"66ac41dc-69e1-410c-99aa-607728c1558d","biId":"7256070","wAsSubmissionId":"24ef3341-758b-4808-9127-af8e42410499","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:18:04.508Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef3341-758b-4808-9127-af8e42410499","edRefCode":"ACN3-2023-06-3341","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"GB","country":"UK","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:18:05.323Z"}},"wAsCountryCode":"GB","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O Lawrence Berkeley National Laboratory","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":2471,"price":617.75,"subtotal":0,"tax":0,"total":0,"discountAmount":617.75,"discountPercentage":100,"currencyCode":"GBP","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1853.25,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":617.75,"discountPercentage":33.535511938486444,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1853.25,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":617.75,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"GB","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef3341-758b-4808-9127-af8e42410499","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-3341","wAsSubmissionId":"24ef3341-758b-4808-9127-af8e42410499","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with multiple Society and Promotional discounts</t>
   </si>
   <si>
@@ -643,6 +1202,78 @@
     <t>No</t>
   </si>
   <si>
+    <t>Created Viax order 7256071 for PriceProposal 24ef9346-203b-4808-9127-af8e42410605</t>
+  </si>
+  <si>
+    <t>7256071</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef9346-203b-4808-9127-af8e42410605",
+      "edRefCode": "ACN3-2023-06-9346",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [
+        "JCASP"
+      ],
+      "promoCodes": [
+        "PROMO50"
+      ],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256071 for PriceProposal 24ef9346-203b-4808-9127-af8e42410605","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256071","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef9346-203b-4808-9127-af8e42410605","version":"1.6.6-qa2.75","submissionId":"24ef9346-203b-4808-9127-af8e42410605","priceProposal":{"uid":"66ac4251-5dab-4f92-a264-7d164d3c3f78","biId":"7256071","wAsSubmissionId":"24ef9346-203b-4808-9127-af8e42410605","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:20:01.494Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef9346-203b-4808-9127-af8e42410605","edRefCode":"ACN3-2023-06-9346","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:20:02.035Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef9346-203b-4808-9127-af8e42410605","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-9346","wAsSubmissionId":"24ef9346-203b-4808-9127-af8e42410605","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with same discount Geographical Editorial and Society discounts</t>
   </si>
   <si>
@@ -655,6 +1286,76 @@
     <t>EANM9</t>
   </si>
   <si>
+    <t>Created Viax order 7256072 for PriceProposal 24ef5278-339b-4808-9127-af8e42410612</t>
+  </si>
+  <si>
+    <t>7256072</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
+      "submissionId": "24ef5278-339b-4808-9127-af8e42410612",
+      "edRefCode": "ACN3-2023-06-5278",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "EDUCATION",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [
+        "EANM9"
+      ],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "rbenny@wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "BO",
+              "country": "BO",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256072 for PriceProposal 24ef5278-339b-4808-9127-af8e42410612","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256072","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5278-339b-4808-9127-af8e42410612","version":"1.6.6-qa2.75","submissionId":"24ef5278-339b-4808-9127-af8e42410612","priceProposal":{"uid":"66ac42de-bb66-48b9-9016-2fde7c04d7d6","biId":"7256072","wAsSubmissionId":"24ef5278-339b-4808-9127-af8e42410612","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:22:22.172Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef5278-339b-4808-9127-af8e42410612","edRefCode":"ACN3-2023-06-5278","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM9"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"BO","country":"BO","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"EANM9","discountType":"Society","discountAmount":400,"discountPercentage":50,"discountDescription":"SOCIETY","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"EANM9","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:22:22.725Z"}},"wAsCountryCode":"BO","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":400,"tax":0,"total":400,"discountAmount":400,"discountPercentage":50,"currencyCode":"USD","allDiscounts":[{"discountCode":"EANM9","discountType":"Society","discountAmount":400,"discountPercentage":50,"discountDescription":"SOCIETY","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"EANM9","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":400,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"BO","attribute":"wAsCountryCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":400,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"BO","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5278-339b-4808-9127-af8e42410612","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5278","wAsSubmissionId":"24ef5278-339b-4808-9127-af8e42410612","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Society Promotional Geographical Editorial Article type and Referral discounts</t>
   </si>
   <si>
@@ -667,24 +1368,323 @@
     <t>PE - Peru</t>
   </si>
   <si>
+    <t>Created Viax order 7256081 for PriceProposal 24ef6602-438b-4808-9127-af8e42410743</t>
+  </si>
+  <si>
+    <t>7256081</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
+      "submissionId": "24ef6602-438b-4808-9127-af8e42410743",
+      "edRefCode": "ACN3-2023-06-6602",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "RESEARCH ARTICLE",
+      "displayArticleType": "RESEARCH ARTICLE",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [
+        "JCASP"
+      ],
+      "promoCodes": [
+        "PROMO50"
+      ],
+      "discountCodes": [],
+      "editorialDiscountCode": "CCCAM424",
+      "referringJournalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "PE",
+              "country": "PE",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256081 for PriceProposal 24ef6602-438b-4808-9127-af8e42410743","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256081","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef6602-438b-4808-9127-af8e42410743","version":"1.6.6-qa2.75","submissionId":"24ef6602-438b-4808-9127-af8e42410743","priceProposal":{"uid":"66ac4897-22b2-4cb6-89a8-7074970f6b57","biId":"7256081","wAsSubmissionId":"24ef6602-438b-4808-9127-af8e42410743","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:46:47.195Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef6602-438b-4808-9127-af8e42410743","edRefCode":"ACN3-2023-06-6602","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"editorialDiscountCode":"CCCAM424","referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"PE","country":"PE","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:46:48.589Z"}},"wAsCountryCode":"PE","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsReferringJournalRef":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalEISSN":"20457634","wAsEditorialOfficeEmail":"cancermed@wiley.com"},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":20,"tax":0,"total":20,"discountAmount":180,"discountPercentage":90,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":100,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PE","attribute":"wAsCountryCode"}]},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":180,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"}]},{"discountCode":"","discountType":"ReferralDiscount","discountAmount":100,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsReferringJournal"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":180,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"PE","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef6602-438b-4808-9127-af8e42410743","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6602","wAsSubmissionId":"24ef6602-438b-4808-9127-af8e42410743","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Multiple Insitutional discounts</t>
   </si>
   <si>
     <t>MultiInsti</t>
   </si>
   <si>
+    <t>Created Viax order 7256082 for PriceProposal 24ef5088-168b-4808-9127-af8e42410890</t>
+  </si>
+  <si>
+    <t>7256082</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
+      "submissionId": "24ef5088-168b-4808-9127-af8e42410890",
+      "edRefCode": "ACN3-2023-06-5088",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "PhD",
+          "orcId": "0000-0003-4043-3196",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "131661",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Stavnger",
+              "countryCode": "US",
+              "country": "France",
+              "institution": "Ardrossan Area School",
+              "department": "School of GeoSciences",
+              "stateProvince": "Rogaland Fylke",
+              "postalCode": "4036",
+              "streetAddress": [
+                "Po Box 2554"
+              ]
+            }
+          ]
+        }
+      ],
+      "funders": []
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256082 for PriceProposal 24ef5088-168b-4808-9127-af8e42410890","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256082","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5088-168b-4808-9127-af8e42410890","version":"1.6.6-qa2.75","submissionId":"24ef5088-168b-4808-9127-af8e42410890","priceProposal":{"uid":"66ac4967-edaa-4f83-940e-380229b4cc07","biId":"7256082","wAsSubmissionId":"24ef5088-168b-4808-9127-af8e42410890","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:50:15.638Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef5088-168b-4808-9127-af8e42410890","edRefCode":"ACN3-2023-06-5088","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"PhD","orcId":"0000-0003-4043-3196","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"addressLocality":"Stavnger","countryCode":"US","country":"France","institution":"Ardrossan Area School","department":"School of GeoSciences","stateProvince":"Rogaland Fylke","postalCode":"4036","streetAddress":["Po Box 2554"]}]}],"funders":[]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:50:16.393Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":"0000-0003-4043-3196","firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"PhD","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"affiliationName":"Ardrossan Area School","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5088-168b-4808-9127-af8e42410890","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5088","wAsSubmissionId":"24ef5088-168b-4808-9127-af8e42410890","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Funder details</t>
   </si>
   <si>
     <t>FunderPaid</t>
   </si>
   <si>
+    <t>Created Viax order 7256083 for PriceProposal 24ef5554-787b-4808-9127-af8e42410953</t>
+  </si>
+  <si>
+    <t>7256083</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "4a48d9c8-6b6d-4583-b9ac-1836890cb988",
+      "submissionId": "24ef5554-787b-4808-9127-af8e42410953",
+      "edRefCode": "CAM4-2024-04-5554",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Data Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "wAsManualDiscountAmount": 0,
+      "authors": [
+        {
+          "role": "CorrespondingAuthor",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "email": "TestAuto@wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "2221",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "orcId": "0000-0003-0888-1984",
+              "addressLocality": "Stavnger",
+              "countryCode": "US",
+              "country": "USA",
+              "institution": "Universidad Nacional De Ingenieria",
+              "department": "SchoolofGeoSciences",
+              "stateProvince": "RogalandFylke",
+              "postalCode": "4036",
+              "streetAddress": [
+                "PoBox2554"
+              ]
+            }
+          ]
+        }
+      ],
+      "funders": [
+        {
+          "name": "ARC of the Piedmont (The Arc)",
+          "funderId": "10.13039/100006467",
+          "grants": [
+            {
+              "grantNumber": "124566AA",
+              "grantRecipient": [
+                "PhilipJ.Cameron-Smith"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256083 for PriceProposal 24ef5554-787b-4808-9127-af8e42410953","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256083","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5554-787b-4808-9127-af8e42410953","version":"1.6.6-qa2.75","submissionId":"24ef5554-787b-4808-9127-af8e42410953","priceProposal":{"uid":"66ac499f-a4d0-4065-8cae-14fadece6c21","biId":"7256083","wAsSubmissionId":"24ef5554-787b-4808-9127-af8e42410953","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:51:11.552Z","wAsPaymentType":"FunderPaid","wAsPriceProposalPayload":{"requestId":"4a48d9c8-6b6d-4583-b9ac-1836890cb988","submissionId":"24ef5554-787b-4808-9127-af8e42410953","edRefCode":"CAM4-2024-04-5554","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Data Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"wAsManualDiscountAmount":0,"authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","email":"TestAuto@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"2221","institutionIdType":"Ringgold"}],"orcId":"0000-0003-0888-1984","addressLocality":"Stavnger","countryCode":"US","country":"USA","institution":"Universidad Nacional De Ingenieria","department":"SchoolofGeoSciences","stateProvince":"RogalandFylke","postalCode":"4036","streetAddress":["PoBox2554"]}]}],"funders":[{"name":"ARC of the Piedmont (The Arc)","funderId":"10.13039/100006467","grants":[{"grantNumber":"124566AA","grantRecipient":["PhilipJ.Cameron-Smith"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:51:12.598Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":true,"woadInstitution":{"institutionId":"2221","institutionName":"Commonwealth Scientific and Industrial Research Organisation","institutionIdType":"Ringgold","woaCode":"CSIR","consortiumCode":""},"prices":[{"basePrice":800,"price":800,"subtotal":800,"tax":0,"total":800,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAuto@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":null,"honorificSuffix":null,"affiliations":[{"affiliationIds":[{"institutionId":"2221","institutionIdType":"Ringgold"}],"affiliationName":"Universidad Nacional De Ingenieria","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[{"funderId":"10.13039/100006467","name":"ARC of the Piedmont (The Arc)","researchGrants":[{"grantNumber":"124566AA","grantRecipients":["PhilipJ.Cameron-Smith"]}]}],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5554-787b-4808-9127-af8e42410953","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"CAM4-2024-04-5554","wAsSubmissionId":"24ef5554-787b-4808-9127-af8e42410953","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Data Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Manual override required value as Yes</t>
   </si>
   <si>
     <t>ManualOverride</t>
   </si>
   <si>
+    <t>Created Viax order 7256085 for PriceProposal 24ef8559-588b-4808-9127-af8e42410290</t>
+  </si>
+  <si>
+    <t>7256085</t>
+  </si>
+  <si>
+    <t>ManualOverrideRequired</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn($data: Object) { testFunction(input: {name: \"receive-price-proposal-from-kafka\", data: {apiversion: \"1.0.1\", tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", id: \"51014872-8dfd-11ed-a1eb-0242ac120002\", type: \"priceproposal.requested\", source: \"urn:appcat:cmh-eeolink\", specversion: \"1.0\", subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", time: \"2019-08-24T14:15:22Z\", datacontenttype: \"application/json\", data: $data}}) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef8559-588b-4808-9127-af8e42410290",
+      "edRefCode": "ACN3-2023-06-8559",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": true,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [
+        "JCASP"
+      ],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256085 for PriceProposal 24ef8559-588b-4808-9127-af8e42410290","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256085","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef8559-588b-4808-9127-af8e42410290","version":"1.6.6-qa2.75","submissionId":"24ef8559-588b-4808-9127-af8e42410290","priceProposal":{"uid":"66ac4a4c-0e3f-4d90-9349-e892ad2945df","biId":"7256085","wAsSubmissionId":"24ef8559-588b-4808-9127-af8e42410290","bpStatus":{"code":"ManualOverrideRequired"},"biCreatedAt":"2024-08-02T02:54:04.137Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef8559-588b-4808-9127-af8e42410290","edRefCode":"ACN3-2023-06-8559","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":true,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:54:04.706Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":true,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8559-588b-4808-9127-af8e42410290","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-8559","wAsSubmissionId":"24ef8559-588b-4808-9127-af8e42410290","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Invalid Promotional discount code</t>
   </si>
   <si>
@@ -694,6 +1694,79 @@
     <t>PRKMO50</t>
   </si>
   <si>
+    <t>Created Viax order 7256084 for PriceProposal 24ef7677-712b-4808-9127-af8e42410611</t>
+  </si>
+  <si>
+    <t>7256084</t>
+  </si>
+  <si>
+    <t>DataCorrectionRequired</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn($data: Object) { testFunction(input: {name: \"receive-price-proposal-from-kafka\", data: {apiversion: \"1.0.1\", tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", id: \"51014872-8dfd-11ed-a1eb-0242ac120002\", type: \"priceproposal.requested\", source: \"urn:appcat:cmh-eeolink\", specversion: \"1.0\", subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", time: \"2019-08-24T14:15:22Z\", datacontenttype: \"application/json\", data: $data}}) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef7677-712b-4808-9127-af8e42410611",
+      "edRefCode": "ACN3-2023-06-7677",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [
+		"PRKMO50"
+	  ],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256084 for PriceProposal 24ef7677-712b-4808-9127-af8e42410611","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256084","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef7677-712b-4808-9127-af8e42410611","version":"1.6.6-qa2.75","submissionId":"24ef7677-712b-4808-9127-af8e42410611","priceProposal":{"uid":"66ac49d8-dcd7-4328-9e15-794550032924","biId":"7256084","wAsSubmissionId":"24ef7677-712b-4808-9127-af8e42410611","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-02T02:52:07.986Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef7677-712b-4808-9127-af8e42410611","edRefCode":"ACN3-2023-06-7677","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PRKMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:52:08.571Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'PRKMO50\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"PRKMO50"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef7677-712b-4808-9127-af8e42410611","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-7677","wAsSubmissionId":"24ef7677-712b-4808-9127-af8e42410611","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Invalid Society</t>
   </si>
   <si>
@@ -703,115 +1776,785 @@
     <t>EANM</t>
   </si>
   <si>
+    <t>Created Viax order 7256086 for PriceProposal 24ef6216-261b-4808-9127-af8e42410557</t>
+  </si>
+  <si>
+    <t>7256086</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn($data: Object) { testFunction(input: {name: \"receive-price-proposal-from-kafka\", data: {apiversion: \"1.0.1\", tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", id: \"51014872-8dfd-11ed-a1eb-0242ac120002\", type: \"priceproposal.requested\", source: \"urn:appcat:cmh-eeolink\", specversion: \"1.0\", subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", time: \"2019-08-24T14:15:22Z\", datacontenttype: \"application/json\", data: $data}}) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef6216-261b-4808-9127-af8e42410557",
+      "edRefCode": "ACN3-2023-06-6216",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [
+        "EANM"
+      ],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256086 for PriceProposal 24ef6216-261b-4808-9127-af8e42410557","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256086","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef6216-261b-4808-9127-af8e42410557","version":"1.6.6-qa2.75","submissionId":"24ef6216-261b-4808-9127-af8e42410557","priceProposal":{"uid":"66ac4aae-0b1d-4144-b5f0-a802f3222584","biId":"7256086","wAsSubmissionId":"24ef6216-261b-4808-9127-af8e42410557","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-02T02:55:42.292Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6216-261b-4808-9127-af8e42410557","edRefCode":"ACN3-2023-06-6216","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:55:42.852Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'EANM\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"EANM"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6216-261b-4808-9127-af8e42410557","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6216","wAsSubmissionId":"24ef6216-261b-4808-9127-af8e42410557","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Invalid Article Type</t>
   </si>
   <si>
     <t>InvalidArticleType</t>
   </si>
   <si>
+    <t>Created Viax order 7256087 for PriceProposal 24ef4466-307b-4808-9127-af8e42410713</t>
+  </si>
+  <si>
+    <t>7256087</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
+      "submissionId": "24ef4466-307b-4808-9127-af8e42410713",
+      "edRefCode": "ACN3-2023-06-4466",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "EDUCATIO",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "rbenny@wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256087 for PriceProposal 24ef4466-307b-4808-9127-af8e42410713","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256087","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef4466-307b-4808-9127-af8e42410713","version":"1.6.6-qa2.75","submissionId":"24ef4466-307b-4808-9127-af8e42410713","priceProposal":{"uid":"66ac4af5-0a0b-476f-967d-876367f5cbe5","biId":"7256087","wAsSubmissionId":"24ef4466-307b-4808-9127-af8e42410713","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-02T02:56:52.995Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef4466-307b-4808-9127-af8e42410713","edRefCode":"ACN3-2023-06-4466","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATIO","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:56:54.429Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P005","errorMessage":"Base Article Type not defined.","fieldPath":"priceProposal.hiConsistsOf[0].biiSalable.wAsBaseArticleType","fieldValue":"EDUCATIO"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":800,"tax":0,"total":800,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4466-307b-4808-9127-af8e42410713","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4466","wAsSubmissionId":"24ef4466-307b-4808-9127-af8e42410713","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATIO","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Invalid Editorial</t>
   </si>
   <si>
     <t>InvalidEditorial</t>
   </si>
   <si>
+    <t>Created Viax order 7256088 for PriceProposal 24ef6320-470b-4808-9127-af8e42410858</t>
+  </si>
+  <si>
+    <t>7256088</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
+      "submissionId": "24ef6320-470b-4808-9127-af8e42410858",
+      "edRefCode": "ACN3-2023-06-6320",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "EDUCATION",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "editorialDiscountCode": "CWECE3",
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "rbenny@wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256088 for PriceProposal 24ef6320-470b-4808-9127-af8e42410858","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256088","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef6320-470b-4808-9127-af8e42410858","version":"1.6.6-qa2.75","submissionId":"24ef6320-470b-4808-9127-af8e42410858","priceProposal":{"uid":"66ac4b2f-8684-4409-9b28-52c6e74c297f","biId":"7256088","wAsSubmissionId":"24ef6320-470b-4808-9127-af8e42410858","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-02T02:57:51.040Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef6320-470b-4808-9127-af8e42410858","edRefCode":"ACN3-2023-06-6320","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"CWECE3","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:57:51.652Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P007","errorMessage":"Editorial code \'CWECE3\' does not exist for the journal","fieldPath":"hiConsistsOf[0].wAsEditorialDiscountCode","fieldValue":"CWECE3"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":800,"tax":0,"total":800,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"CWECE3","discountType":"EditorialDiscount","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CWECE3","biiSalable":{"maId":"24ef6320-470b-4808-9127-af8e42410858","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6320","wAsSubmissionId":"24ef6320-470b-4808-9127-af8e42410858","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Invalid Referal</t>
   </si>
   <si>
     <t>InvalidReferal</t>
   </si>
   <si>
+    <t>Created Viax order 7256089 for PriceProposal 24ef5372-595b-4808-9127-af8e42410195</t>
+  </si>
+  <si>
+    <t>7256089</t>
+  </si>
+  <si>
+    <t>ReSend</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
+      "submissionId": "24ef5372-595b-4808-9127-af8e42410195",
+      "edRefCode": "ACN3-2023-06-5372",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "OPINION",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "referringJournalId": "c597beef-e45f-4cc7-b34c-0df812e2ef21",
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "rbenny@wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256089 for PriceProposal 24ef5372-595b-4808-9127-af8e42410195","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256089","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5372-595b-4808-9127-af8e42410195","version":"1.6.6-qa2.75","submissionId":"24ef5372-595b-4808-9127-af8e42410195","priceProposal":{"uid":"66ac4b66-7a54-46f1-8506-9d7a2930d7fc","biId":"7256089","wAsSubmissionId":"24ef5372-595b-4808-9127-af8e42410195","bpStatus":{"code":"ReSend"},"biCreatedAt":"2024-08-02T02:58:46.980Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef5372-595b-4808-9127-af8e42410195","edRefCode":"ACN3-2023-06-5372","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef21","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:58:47.527Z"}},"wAsCountryCode":"US","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef21","wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P004","errorMessage":"Unable to locate the referring journal from STIBO.","fieldPath":"priceProposal.wAsReferringJournalRef.wAsJournalUuid","fieldValue":""}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":640,"subtotal":640,"tax":0,"total":640,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5372-595b-4808-9127-af8e42410195","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5372","wAsSubmissionId":"24ef5372-595b-4808-9127-af8e42410195","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Invalid CountryCode</t>
   </si>
   <si>
     <t>InvalidCountryCode</t>
   </si>
   <si>
+    <t>Created Viax order 7256090 for PriceProposal 24ef7904-293b-4808-9127-af8e42410597</t>
+  </si>
+  <si>
+    <t>7256090</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
+      "submissionId": "24ef7904-293b-4808-9127-af8e42410597",
+      "edRefCode": "ACN3-2023-06-7904",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "OPINION",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "rbenny@wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "ZZ",
+              "country": "ZZ",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256090 for PriceProposal 24ef7904-293b-4808-9127-af8e42410597","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256090","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef7904-293b-4808-9127-af8e42410597","version":"1.6.6-qa2.75","submissionId":"24ef7904-293b-4808-9127-af8e42410597","priceProposal":{"uid":"66ac4b9f-1480-4739-b5b1-77405a83bcd1","biId":"7256090","wAsSubmissionId":"24ef7904-293b-4808-9127-af8e42410597","bpStatus":{"code":"ReSend"},"biCreatedAt":"2024-08-02T02:59:43.598Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef7904-293b-4808-9127-af8e42410597","edRefCode":"ACN3-2023-06-7904","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"ZZ","country":"ZZ","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:59:44.129Z"}},"wAsCountryCode":"ZZ","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"500","errorMessage":"Price calculation error. {}","fieldPath":"","fieldValue":""},{"errorCode":"P006","errorMessage":"Country Code Not Defined","fieldPath":"priceProposal.wAsCorrespondingAuthor.affiliations?.[0].countryCode","fieldValue":"ZZ"}],"wAsPricing":null,"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"ZZ","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef7904-293b-4808-9127-af8e42410597","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-7904","wAsSubmissionId":"24ef7904-293b-4808-9127-af8e42410597","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP with Invalid MailId</t>
   </si>
   <si>
     <t>InvalidMailId</t>
   </si>
   <si>
+    <t>Created Viax order 7256091 for PriceProposal 24ef4190-617b-4808-9127-af8e42410397</t>
+  </si>
+  <si>
+    <t>7256091</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
+      "submissionId": "24ef4190-617b-4808-9127-af8e42410397",
+      "edRefCode": "ACN3-2023-06-4190",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "OPINION",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "rbenny.wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256091 for PriceProposal 24ef4190-617b-4808-9127-af8e42410397","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256091","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef4190-617b-4808-9127-af8e42410397","version":"1.6.6-qa2.75","submissionId":"24ef4190-617b-4808-9127-af8e42410397","priceProposal":{"uid":"66ac4bda-af04-4c02-996d-4d90bf2155c4","biId":"7256091","wAsSubmissionId":"24ef4190-617b-4808-9127-af8e42410397","bpStatus":{"code":"ReSend"},"biCreatedAt":"2024-08-02T03:00:42.565Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef4190-617b-4808-9127-af8e42410397","edRefCode":"ACN3-2023-06-4190","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny.wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T03:00:43.046Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P021","errorMessage":"Email address has invalid format","fieldPath":"priceProposal.wAsCorrespondingAuthor.email","fieldValue":"rbenny.wiley.com"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":640,"subtotal":640,"tax":0,"total":640,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny.wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4190-617b-4808-9127-af8e42410397","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4190","wAsSubmissionId":"24ef4190-617b-4808-9127-af8e42410397","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP Society discount with Rejected</t>
   </si>
   <si>
+    <t>Created Viax order 7256092 for PriceProposal 24ef6993-663b-4808-9127-af8e42410585</t>
+  </si>
+  <si>
+    <t>7256092</t>
+  </si>
+  <si>
+    <t>REJECTED</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn($data: Object) { testFunction(input: {name: \"receive-price-proposal-from-kafka\", data: {apiversion: \"1.0.1\", tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", id: \"51014872-8dfd-11ed-a1eb-0242ac120002\", type: \"priceproposal.requested\", source: \"urn:appcat:cmh-eeolink\", specversion: \"1.0\", subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", time: \"2019-08-24T14:15:22Z\", datacontenttype: \"application/json\", data: $data}}) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef6993-663b-4808-9127-af8e42410585",
+      "edRefCode": "ACN3-2023-06-6993",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [
+        "JCASP"
+      ],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256092 for PriceProposal 24ef6993-663b-4808-9127-af8e42410585","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256092","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef6993-663b-4808-9127-af8e42410585","version":"1.6.6-qa2.75","submissionId":"24ef6993-663b-4808-9127-af8e42410585","priceProposal":{"uid":"66ac4c14-81fc-4c71-a08b-3a5608bc9e3d","biId":"7256092","wAsSubmissionId":"24ef6993-663b-4808-9127-af8e42410585","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T03:01:39.984Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6993-663b-4808-9127-af8e42410585","edRefCode":"ACN3-2023-06-6993","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T03:01:40.627Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6993-663b-4808-9127-af8e42410585","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6993","wAsSubmissionId":"24ef6993-663b-4808-9127-af8e42410585","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Create PP Society discount with Withdrawn</t>
   </si>
   <si>
+    <t>Created Viax order 7256093 for PriceProposal 24ef9397-207b-4808-9127-af8e42410272</t>
+  </si>
+  <si>
+    <t>7256093</t>
+  </si>
+  <si>
+    <t>WITHDRAWN</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn($data: Object) { testFunction(input: {name: \"receive-price-proposal-from-kafka\", data: {apiversion: \"1.0.1\", tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", id: \"51014872-8dfd-11ed-a1eb-0242ac120002\", type: \"priceproposal.requested\", source: \"urn:appcat:cmh-eeolink\", specversion: \"1.0\", subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", time: \"2019-08-24T14:15:22Z\", datacontenttype: \"application/json\", data: $data}}) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef9397-207b-4808-9127-af8e42410272",
+      "edRefCode": "ACN3-2023-06-9397",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [
+        "JCASP"
+      ],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256093 for PriceProposal 24ef9397-207b-4808-9127-af8e42410272","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256093","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef9397-207b-4808-9127-af8e42410272","version":"1.6.6-qa2.75","submissionId":"24ef9397-207b-4808-9127-af8e42410272","priceProposal":{"uid":"66ac4c7a-59b5-42a8-8389-8d785f1736a5","biId":"7256093","wAsSubmissionId":"24ef9397-207b-4808-9127-af8e42410272","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T03:03:22.407Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef9397-207b-4808-9127-af8e42410272","edRefCode":"ACN3-2023-06-9397","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T03:03:22.986Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef9397-207b-4808-9127-af8e42410272","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-9397","wAsSubmissionId":"24ef9397-207b-4808-9127-af8e42410272","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>Verify UI Change Data Correction to Price Determined</t>
   </si>
   <si>
+    <t>Created Viax order 7256094 for PriceProposal 24ef2328-240b-4808-9127-af8e42410877</t>
+  </si>
+  <si>
+    <t>7256094</t>
+  </si>
+  <si>
+    <t>DATA CORRECTION REQUIRED::PRICE DETERMINED</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation testFn($data: Object) { testFunction(input: {name: \"receive-price-proposal-from-kafka\", data: {apiversion: \"1.0.1\", tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", id: \"51014872-8dfd-11ed-a1eb-0242ac120002\", type: \"priceproposal.requested\", source: \"urn:appcat:cmh-eeolink\", specversion: \"1.0\", subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\", time: \"2019-08-24T14:15:22Z\", datacontenttype: \"application/json\", data: $data}}) { status data }}",
+  "variables": {
+    "data": {
+      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
+      "submissionId": "24ef2328-240b-4808-9127-af8e42410877",
+      "edRefCode": "ACN3-2023-06-2328",
+      "articleDOI": "",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
+      "sourceSystem": "EM",
+      "baseArticleType": "Research Article",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-08-02",
+      "articleAcceptedDate": "2015-09-29",
+      "editorialStatus": "TBC",
+      "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
+      "isManualOverrideRequired": false,
+      "manualOverrideInstructions": "string",
+      "societyCodes": [
+        "EANM"
+      ],
+      "promoCodes": [],
+      "discountCodes": [],
+      "authors": [
+        {
+          "role": "Corresponding Author",
+          "authorSequenceNumber": 1,
+          "firstName": "Jim",
+          "middleName": "M.",
+          "lastName": "TESSON",
+          "honorificPrefix": "Mr.",
+          "honorificSuffix": "",
+          "email": "TestAutomation@Wiley.com",
+          "affiliationIdType": "Ringgold",
+          "affiliations": [
+            {
+              "affiliationIds": [
+                {
+                  "institutionId": "",
+                  "institutionIdType": "Ringgold"
+                }
+              ],
+              "addressLocality": "Aix en Provence",
+              "countryCode": "US",
+              "country": "US",
+              "institution": "Grant Institute",
+              "department": "School of GeoSciences",
+              "stateProvince": "New Jersey",
+              "postalCode": "90210",
+              "streetAddress": [
+                "1832 Colvin Ave"
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256094 for PriceProposal 24ef2328-240b-4808-9127-af8e42410877","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256094","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef2328-240b-4808-9127-af8e42410877","version":"1.6.6-qa2.75","submissionId":"24ef2328-240b-4808-9127-af8e42410877","priceProposal":{"uid":"66ac4ce0-bd45-4a41-8c14-05bf7eefe876","biId":"7256094","wAsSubmissionId":"24ef2328-240b-4808-9127-af8e42410877","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-02T03:05:04.971Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef2328-240b-4808-9127-af8e42410877","edRefCode":"ACN3-2023-06-2328","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T03:05:05.586Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'EANM\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"EANM"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2328-240b-4808-9127-af8e42410877","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-2328","wAsSubmissionId":"24ef2328-240b-4808-9127-af8e42410877","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+  </si>
+  <si>
     <t>TesctCaseName</t>
   </si>
   <si>
     <t>Country</t>
   </si>
   <si>
+    <t>Discount</t>
+  </si>
+  <si>
     <t>ExecutionDate</t>
   </si>
   <si>
     <t>Trigger Invoice Order with New Customer</t>
   </si>
   <si>
-    <t>UnPaidNewCustomer</t>
-  </si>
-  <si>
-    <t>20240725122330Test</t>
-  </si>
-  <si>
-    <t>20240725122330Auto</t>
-  </si>
-  <si>
-    <t>20240725122330@Wiley.com</t>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>1180.00</t>
+  </si>
+  <si>
+    <t>1416.00</t>
+  </si>
+  <si>
+    <t>236.00</t>
   </si>
   <si>
     <t>Trigger CreditCard Order with New Customer</t>
   </si>
   <si>
-    <t>CreditCardNewCustomer</t>
-  </si>
-  <si>
-    <t>20240725122331Test</t>
-  </si>
-  <si>
-    <t>20240725122331Auto</t>
-  </si>
-  <si>
-    <t>20240725122331@Wiley.com</t>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d</t>
+  </si>
+  <si>
+    <t>2300.25</t>
+  </si>
+  <si>
+    <t>N.A</t>
+  </si>
+  <si>
+    <t>0.00</t>
   </si>
   <si>
     <t>Trigger Alipay Order with New Customer</t>
   </si>
   <si>
-    <t>AlipayNewCustomer</t>
-  </si>
-  <si>
-    <t>20240725122333Test</t>
-  </si>
-  <si>
-    <t>20240725122333Auto</t>
-  </si>
-  <si>
-    <t>20240725122333@Wiley.com</t>
+    <t>900.00</t>
+  </si>
+  <si>
+    <t>Trigger Proforma Order with New Customer</t>
+  </si>
+  <si>
+    <t>Proforma</t>
+  </si>
+  <si>
+    <t>1b28a8b9-067b-4ce9-b981-e8eabe16e0a7</t>
   </si>
   <si>
     <t>Trigger Invoice Order with Existing Customer</t>
   </si>
   <si>
+    <t>20240809175918Test</t>
+  </si>
+  <si>
+    <t>20240809175918Auto</t>
+  </si>
+  <si>
+    <t>20240809175918@Wiley.com</t>
+  </si>
+  <si>
     <t>Trigger CreditCard Order with Existing Customer</t>
   </si>
   <si>
+    <t>20240809175920Test</t>
+  </si>
+  <si>
+    <t>20240809175920Auto</t>
+  </si>
+  <si>
+    <t>20240809175920@Wiley.com</t>
+  </si>
+  <si>
     <t>Trigger Alipay Order with Existing Customer</t>
   </si>
   <si>
-    <t>Trigger Proforma Order with New Customer</t>
-  </si>
-  <si>
-    <t>Proforma</t>
+    <t>20240809175921Test</t>
+  </si>
+  <si>
+    <t>20240809175921Auto</t>
+  </si>
+  <si>
+    <t>20240809175921@Wiley.com</t>
   </si>
   <si>
     <t>Trigger Proforma Order with Existing Customer</t>
+  </si>
+  <si>
+    <t>20240809181925Test</t>
+  </si>
+  <si>
+    <t>20240809181925Auto</t>
+  </si>
+  <si>
+    <t>20240809181925@Wiley.com</t>
   </si>
 </sst>
 </file>
@@ -853,7 +2596,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -902,6 +2645,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -925,7 +2674,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -949,6 +2698,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1968,10 +3718,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AI25"/>
+  <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="R13" workbookViewId="0">
+      <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1980,7 +3730,7 @@
     <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -2084,10 +3834,13 @@
         <v>170</v>
       </c>
       <c r="AI1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -2095,31 +3848,31 @@
         <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R2">
         <v>75</v>
@@ -2128,19 +3881,37 @@
         <v>5</v>
       </c>
       <c r="T2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z2" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>179</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF2" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH2" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2148,31 +3919,31 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="H3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="N3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R3">
         <v>75</v>
@@ -2181,19 +3952,37 @@
         <v>20</v>
       </c>
       <c r="T3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X3" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z3" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>189</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF3" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH3" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2201,52 +3990,70 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="H4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="N4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R4">
         <v>75</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X4" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z4" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF4" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH4" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2254,31 +4061,31 @@
         <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="E5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="H5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="N5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R5">
         <v>20</v>
@@ -2287,19 +4094,37 @@
         <v>90</v>
       </c>
       <c r="T5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X5" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y5" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z5" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF5" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH5" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2307,31 +4132,31 @@
         <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="E6" t="s">
-        <v>192</v>
+        <v>211</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="H6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R6">
         <v>10</v>
@@ -2340,19 +4165,37 @@
         <v>15.25</v>
       </c>
       <c r="T6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X6" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y6" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z6" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>214</v>
+      </c>
+      <c r="AF6" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH6" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>215</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2360,31 +4203,31 @@
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
       <c r="E7" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="H7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="N7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R7">
         <v>30</v>
@@ -2393,19 +4236,37 @@
         <v>100</v>
       </c>
       <c r="T7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X7" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z7" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF7" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH7" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>224</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2413,52 +4274,70 @@
         <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" t="s">
         <v>173</v>
       </c>
-      <c r="E8" t="s">
-        <v>172</v>
-      </c>
       <c r="F8" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R8">
         <v>75</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X8" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y8" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="Z8" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF8" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH8" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>230</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2466,34 +4345,34 @@
         <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>201</v>
+        <v>232</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="H9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="N9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -2502,28 +4381,46 @@
         <v>75</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
       <c r="X9" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y9" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
+      <c r="AD9" t="s">
+        <v>234</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AF9" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH9" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>237</v>
+      </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2531,19 +4428,19 @@
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>203</v>
+        <v>238</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>204</v>
+        <v>239</v>
       </c>
       <c r="E10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>23</v>
@@ -2552,13 +4449,13 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
@@ -2573,16 +4470,34 @@
         <v>5</v>
       </c>
       <c r="X10" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y10" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z10" t="s">
-        <v>205</v>
+        <v>240</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>241</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>242</v>
+      </c>
+      <c r="AF10" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH10" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -2590,31 +4505,31 @@
         <v>18</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>207</v>
+        <v>246</v>
       </c>
       <c r="E11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>208</v>
+        <v>247</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
@@ -2626,25 +4541,43 @@
         <v>50</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U11" s="11"/>
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
       <c r="X11" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y11" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z11" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AA11" s="11"/>
       <c r="AB11" s="11"/>
       <c r="AC11" s="11"/>
+      <c r="AD11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF11" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH11" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2652,46 +4585,46 @@
         <v>18</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>210</v>
+        <v>253</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>211</v>
+        <v>254</v>
       </c>
       <c r="E12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="H12" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="I12" t="s">
-        <v>212</v>
+        <v>255</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="R12" s="11">
         <v>75</v>
@@ -2712,25 +4645,43 @@
         <v>20</v>
       </c>
       <c r="X12" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y12" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z12" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="AA12" s="11" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="AB12" s="11" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="AC12" s="11" t="s">
-        <v>205</v>
+        <v>240</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>257</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>258</v>
+      </c>
+      <c r="AF12" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH12" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>259</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2738,61 +4689,79 @@
         <v>18</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>214</v>
+        <v>261</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>215</v>
+        <v>262</v>
       </c>
       <c r="E13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="S13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U13" s="11"/>
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
       <c r="X13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="Y13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="Z13" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AA13" s="11"/>
       <c r="AB13" s="11"/>
       <c r="AC13" s="11"/>
+      <c r="AD13" t="s">
+        <v>263</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>264</v>
+      </c>
+      <c r="AF13" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH13" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>265</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>266</v>
+      </c>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2800,93 +4769,111 @@
         <v>18</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>216</v>
+        <v>267</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>217</v>
+        <v>268</v>
       </c>
       <c r="E14" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="S14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U14" s="11"/>
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
       <c r="X14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="Y14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="Z14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AA14" s="11"/>
       <c r="AB14" s="11"/>
       <c r="AC14" s="11"/>
+      <c r="AD14" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>270</v>
+      </c>
+      <c r="AF14" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH14" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>271</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>272</v>
+      </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>218</v>
+        <v>273</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>219</v>
+        <v>274</v>
       </c>
       <c r="E15" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N15" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
@@ -2898,25 +4885,43 @@
         <v>5</v>
       </c>
       <c r="T15" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y15" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z15" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AA15" s="11"/>
       <c r="AB15" s="11"/>
       <c r="AC15" s="11"/>
+      <c r="AD15" t="s">
+        <v>275</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>276</v>
+      </c>
+      <c r="AF15" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH15" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>278</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>279</v>
+      </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2924,31 +4929,31 @@
         <v>18</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>221</v>
+        <v>281</v>
       </c>
       <c r="E16" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="H16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>222</v>
+        <v>282</v>
       </c>
       <c r="N16" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
@@ -2957,60 +4962,78 @@
         <v>75</v>
       </c>
       <c r="S16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T16" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U16" s="11"/>
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
       <c r="X16" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y16" s="11" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="Z16" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AA16" s="11"/>
       <c r="AB16" s="11"/>
       <c r="AC16" s="11"/>
+      <c r="AD16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>284</v>
+      </c>
+      <c r="AF16" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH16" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>286</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>287</v>
+      </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>223</v>
+        <v>288</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>224</v>
+        <v>289</v>
       </c>
       <c r="E17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>225</v>
+        <v>290</v>
       </c>
       <c r="N17" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
@@ -3019,98 +5042,206 @@
         <v>75</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T17" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
       <c r="X17" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y17" s="11" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="Z17" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AA17" s="11"/>
       <c r="AB17" s="11"/>
       <c r="AC17" s="11"/>
+      <c r="AD17" t="s">
+        <v>291</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>292</v>
+      </c>
+      <c r="AF17" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH17" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>293</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>294</v>
+      </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>226</v>
+        <v>295</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>227</v>
+        <v>296</v>
       </c>
       <c r="E18" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>297</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>298</v>
+      </c>
+      <c r="AF18" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH18" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>228</v>
+        <v>301</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>229</v>
+        <v>302</v>
       </c>
       <c r="E19" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF19" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH19" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>305</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>306</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>230</v>
+        <v>307</v>
       </c>
       <c r="D20" t="s">
-        <v>231</v>
+        <v>308</v>
       </c>
       <c r="E20" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>309</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>310</v>
+      </c>
+      <c r="AF20" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="AH20" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>312</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>313</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>232</v>
+        <v>314</v>
       </c>
       <c r="D21" t="s">
-        <v>233</v>
+        <v>315</v>
       </c>
       <c r="E21" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>316</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>317</v>
+      </c>
+      <c r="AF21" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="AH21" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>318</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>319</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>234</v>
+        <v>320</v>
       </c>
       <c r="D22" t="s">
-        <v>235</v>
+        <v>321</v>
       </c>
       <c r="E22" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>322</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>323</v>
+      </c>
+      <c r="AF22" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="AH22" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>324</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>325</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -3118,31 +5249,31 @@
         <v>18</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>236</v>
+        <v>326</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F23" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G23" t="s">
         <v>23</v>
       </c>
       <c r="H23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R23">
         <v>75</v>
@@ -3151,19 +5282,37 @@
         <v>5</v>
       </c>
       <c r="T23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X23" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y23" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z23" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>327</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>328</v>
+      </c>
+      <c r="AF23" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="AH23" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>330</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>331</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -3171,31 +5320,31 @@
         <v>18</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>237</v>
+        <v>332</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G24" t="s">
         <v>23</v>
       </c>
       <c r="H24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L24" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R24">
         <v>75</v>
@@ -3204,52 +5353,70 @@
         <v>5</v>
       </c>
       <c r="T24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z24" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>334</v>
+      </c>
+      <c r="AF24" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="AH24" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>336</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>337</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A25" s="13"/>
       <c r="B25" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>238</v>
+        <v>338</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>224</v>
+        <v>289</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G25" t="s">
         <v>23</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>225</v>
+        <v>290</v>
       </c>
       <c r="N25" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
@@ -3258,26 +5425,44 @@
         <v>75</v>
       </c>
       <c r="S25" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T25" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U25" s="11"/>
       <c r="V25" s="11"/>
       <c r="W25" s="11"/>
       <c r="X25" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y25" s="11" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="Z25" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AA25" s="11"/>
       <c r="AB25" s="11"/>
       <c r="AC25" s="11"/>
+      <c r="AD25" t="s">
+        <v>339</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>340</v>
+      </c>
+      <c r="AF25" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="AH25" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>342</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>343</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3286,212 +5471,439 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.81640625" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.81640625" customWidth="1"/>
+    <col min="12" max="12" width="7.7265625" customWidth="1"/>
+    <col min="13" max="14" width="21.81640625" customWidth="1"/>
+    <col min="15" max="15" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>239</v>
+        <v>344</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>240</v>
+        <v>345</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="P1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="S1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>241</v>
+      <c r="U1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>348</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>243</v>
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>349</v>
+      </c>
+      <c r="F2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>247</v>
+        <v>353</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>354</v>
       </c>
       <c r="D3" t="s">
-        <v>248</v>
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>355</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="I3" t="s">
+        <v>194</v>
+      </c>
+      <c r="J3" t="s">
+        <v>357</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>358</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>359</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>261</v>
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="I4" t="s">
+        <v>357</v>
+      </c>
+      <c r="J4" t="s">
+        <v>357</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>358</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>361</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>253</v>
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>362</v>
+      </c>
+      <c r="F5" t="s">
+        <v>363</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>257</v>
+        <v>364</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>243</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>244</v>
+        <v>349</v>
       </c>
       <c r="F6" t="s">
-        <v>245</v>
-      </c>
-      <c r="G6" t="s">
-        <v>246</v>
+        <v>173</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>365</v>
+      </c>
+      <c r="N6" t="s">
+        <v>366</v>
+      </c>
+      <c r="O6" t="s">
+        <v>367</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>258</v>
+        <v>368</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>354</v>
       </c>
       <c r="D7" t="s">
-        <v>248</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>249</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G7" t="s">
-        <v>251</v>
+        <v>355</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="I7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J7" t="s">
+        <v>357</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="M7" t="s">
+        <v>369</v>
+      </c>
+      <c r="N7" t="s">
+        <v>370</v>
+      </c>
+      <c r="O7" t="s">
+        <v>371</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>259</v>
+        <v>372</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>253</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>254</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>255</v>
-      </c>
-      <c r="G8" t="s">
-        <v>256</v>
+        <v>173</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="I8" t="s">
+        <v>357</v>
+      </c>
+      <c r="J8" t="s">
+        <v>357</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="M8" t="s">
+        <v>373</v>
+      </c>
+      <c r="N8" t="s">
+        <v>374</v>
+      </c>
+      <c r="O8" t="s">
+        <v>375</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>262</v>
+        <v>376</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>261</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>244</v>
+        <v>362</v>
       </c>
       <c r="F9" t="s">
-        <v>245</v>
-      </c>
-      <c r="G9" t="s">
-        <v>246</v>
+        <v>363</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
+        <v>377</v>
+      </c>
+      <c r="N9" t="s">
+        <v>378</v>
+      </c>
+      <c r="O9" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI Validations added V.64
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_Inputs.xlsx
+++ b/UploadExcel/TD_Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAA6064-87B2-43FF-A537-0FD291A18E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552E090F-B607-4516-BEFD-C974EBBAC1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,15 @@
     <sheet name="PriceProposal" sheetId="3" r:id="rId3"/>
     <sheet name="OrderCreationCases" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">PriceProposal!$AF$1:$AF$23</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="339">
   <si>
     <t>ExecutionEnvironment</t>
   </si>
@@ -553,15 +556,18 @@
     <t>NA</t>
   </si>
   <si>
+    <t>JCASP</t>
+  </si>
+  <si>
     <t>Research Article</t>
   </si>
   <si>
-    <t>JCASP</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
+    <t>200</t>
+  </si>
+  <si>
     <t>Create PP with Promotional discount</t>
   </si>
   <si>
@@ -574,6 +580,12 @@
     <t>PROMO50</t>
   </si>
   <si>
+    <t>29.94</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>Create PP with Institutional discount</t>
   </si>
   <si>
@@ -772,6 +784,35 @@
     <t>236.00</t>
   </si>
   <si>
+    <t>20240816190247Test</t>
+  </si>
+  <si>
+    <t>20240816190247Auto</t>
+  </si>
+  <si>
+    <t>20240816190247@Wiley.com</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f84775519</t>
+  </si>
+  <si>
+    <t>3213873</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213873 for AS order 20240816190247</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 9ca90171-81f4-4d1b-9528-8a34490d50be","Using soldTo : 9ca90171-81f4-4d1b-9528-8a34490d50be","Using billTo: 9ca90171-81f4-4d1b-9528-8a34490d50be","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213873 for AS order 20240816190247","version":"1.3.5-qa2.94","biId":"3213873"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2023-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190247 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f84775519\" title: \"Secrets of nature\" dhId: \"e0c4569c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"RRO39999\" jpcmsArticleIdentifier: \"RRO.39999.ART\" articleDOI: \"10.1111/RRO.39999\" } soldToDetails: { firstName: \"20240816190247Test\" lastName: \"20240816190247Auto\" email: \"20240816190247@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1180.00, billingAddress: { firstName: \"20240816190247Test\" lastName: \"20240816190247Auto\" streetAddress: [\"389 Nepean Hwy\"] addressLocality:\"Edison\" addressRegion: \"NJ\" countryCode: \"GB\" postalCode: \"08817\" phoneNumber: \"06667778888\" email: \"20240816190247@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-08-16 19:02:47.871</t>
+  </si>
+  <si>
     <t>Trigger CreditCard Order with New Customer</t>
   </si>
   <si>
@@ -790,12 +831,70 @@
     <t>0.00</t>
   </si>
   <si>
+    <t>20240816190249Test</t>
+  </si>
+  <si>
+    <t>20240816190249Auto</t>
+  </si>
+  <si>
+    <t>20240816190249@Wiley.com</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f82547776</t>
+  </si>
+  <si>
+    <t>3213874</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213874 for AS order 20240816190249</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP db7230bc-e352-4a3c-a64b-56d3a5bf268c","Using soldTo : db7230bc-e352-4a3c-a64b-56d3a5bf268c","Using billTo: db7230bc-e352-4a3c-a64b-56d3a5bf268c","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213874 for AS order 20240816190249","version":"1.3.5-qa2.94","biId":"3213874"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e527a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2024-08-16T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190249 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2023-01-26T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CH CC order form validation\" apc: 2300.25 appliedDiscount: 0.00 discountType: \"Institutional\" estimatedTax: 0.00 totalChargedAmount: 2300.25 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CH\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f82547776\" title: \"Secrets of volcano\" dhId: \"e0c3220c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240816190249Test\" lastName: \"20240816190249Auto\" email: \"20240816190249@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 2300.25 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2023-07-03T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240816190249Test\" lastName:\"20240816190249Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"Dufourstrasse 40a\"] addressLocality: \"St. Gallen\" addressRegion: \"SG\" countryCode: \"CH\" postalCode: \"9000\" phoneNumber: \"8299729725\" email: \"20240816190249@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e527a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-08-16 19:02:49.665</t>
+  </si>
+  <si>
     <t>Trigger Alipay Order with New Customer</t>
   </si>
   <si>
     <t>900.00</t>
   </si>
   <si>
+    <t>20240816190251Test</t>
+  </si>
+  <si>
+    <t>20240816190251Auto</t>
+  </si>
+  <si>
+    <t>20240816190251@Wiley.com</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f51045539</t>
+  </si>
+  <si>
+    <t>3213875</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213875 for AS order 20240816190251</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP c56044fa-84e5-4134-b919-d954b8524a7e","Using soldTo : c56044fa-84e5-4134-b919-d954b8524a7e","Using billTo: c56044fa-84e5-4134-b919-d954b8524a7e","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213875 for AS order 20240816190251","version":"1.3.5-qa2.94","biId":"3213875"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e873a\"eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190251 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2023-09-12T15:00:14-05\" paymentDate: \"2023-09-12T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2023-09-12T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 900.00 appliedDiscount: 0.00 estimatedTax: 0.00 totalChargedAmount: 900.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f51045539\" title: \"Secrets of nature\" dhId: \"e0c1151c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"CAM448363\" jpcmsArticleIdentifier: \"CAM4.48363.ART\" articleDOI: \"10.1111/CAM4.48363\" } soldToDetails: { firstName: \"20240816190251Test\" lastName: \"20240816190251Auto\" email: \"20240816190251@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 900.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2024-08-16 08:00:00\" } billingAddress: { firstName: \"20240816190251Test\" lastName: \"20240816190251Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"No. 1 Xikang Road\"] addressLocality: \"Harbin\" addressRegion: \"100\" countryCode: \"CN\" postalCode: \"210024\" phoneNumber: \"0703503263\" email: \"20240816190251@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e873a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-08-16 19:02:51.200</t>
+  </si>
+  <si>
     <t>Trigger Proforma Order with New Customer</t>
   </si>
   <si>
@@ -805,6 +904,35 @@
     <t>1b28a8b9-067b-4ce9-b981-e8eabe16e0a7</t>
   </si>
   <si>
+    <t>20240816190256Test</t>
+  </si>
+  <si>
+    <t>20240816190256Auto</t>
+  </si>
+  <si>
+    <t>20240816190256@Wiley.com</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f27834654</t>
+  </si>
+  <si>
+    <t>3213879</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213879 for AS order 20240816190256</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP db9caa52-3038-4d87-8158-9f847e8c63d4","Using soldTo : db9caa52-3038-4d87-8158-9f847e8c63d4","Using billTo: db9caa52-3038-4d87-8158-9f847e8c63d4","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213879 for AS order 20240816190256","version":"1.3.5-qa2.94","biId":"3213879"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e366a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190256 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-08-16\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f27834654\" title: \"Secrets of nature\" dhId: \"e0c3582c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240816190256Test\" lastName: \"20240816190256Auto\" email: \"20240816190256@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240816190256Test\" lastName: \"20240816190256Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240816190256@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e366a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-08-16 19:02:56.916</t>
+  </si>
+  <si>
     <t>Trigger Invoice Order with Existing Customer</t>
   </si>
   <si>
@@ -817,6 +945,26 @@
     <t>20240809175918@Wiley.com</t>
   </si>
   <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f62879150</t>
+  </si>
+  <si>
+    <t>3213878</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213878 for AS order 20240816190255</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 3f7431cb-eef3-49fa-bdfc-5d16128c6fd5","Using billTo: 3f7431cb-eef3-49fa-bdfc-5d16128c6fd5","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213878 for AS order 20240816190255","version":"1.3.5-qa2.94","biId":"3213878"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e572a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2023-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190255 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f62879150\" title: \"Secrets of nature\" dhId: \"e0c7856c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"RRO39999\" jpcmsArticleIdentifier: \"RRO.39999.ART\" articleDOI: \"10.1111/RRO.39999\" } soldToDetails: { firstName: \"20240809175918Test\" lastName: \"20240809175918Auto\" email: \"20240809175918@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1180.00, billingAddress: { firstName: \"20240809175918Test\" lastName: \"20240809175918Auto\" streetAddress: [\"389 Nepean Hwy\"] addressLocality:\"Edison\" addressRegion: \"NJ\" countryCode: \"GB\" postalCode: \"08817\" phoneNumber: \"06667778888\" email: \"20240809175918@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e572a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-08-16 19:02:55.481</t>
+  </si>
+  <si>
     <t>Trigger CreditCard Order with Existing Customer</t>
   </si>
   <si>
@@ -829,6 +977,26 @@
     <t>20240809175920@Wiley.com</t>
   </si>
   <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f16859253</t>
+  </si>
+  <si>
+    <t>3213877</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213877 for AS order 20240816190254</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 9be953a5-d4ea-4149-a439-801fe3371d6a","Using billTo: 9be953a5-d4ea-4149-a439-801fe3371d6a","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213877 for AS order 20240816190254","version":"1.3.5-qa2.94","biId":"3213877"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e832a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2024-08-16T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190254 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2023-01-26T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CH CC order form validation\" apc: 2300.25 appliedDiscount: 0.00 discountType: \"Institutional\" estimatedTax: 0.00 totalChargedAmount: 2300.25 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CH\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f16859253\" title: \"Secrets of volcano\" dhId: \"e0c3651c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240809175920Test\" lastName: \"20240809175920Auto\" email: \"20240809175920@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 2300.25 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2023-07-03T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240809175920Test\" lastName:\"20240809175920Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"Dufourstrasse 40a\"] addressLocality: \"St. Gallen\" addressRegion: \"SG\" countryCode: \"CH\" postalCode: \"9000\" phoneNumber: \"8299729725\" email: \"20240809175920@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e832a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-08-16 19:02:54.193</t>
+  </si>
+  <si>
     <t>Trigger Alipay Order with Existing Customer</t>
   </si>
   <si>
@@ -841,6 +1009,26 @@
     <t>20240809175921@Wiley.com</t>
   </si>
   <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f55866607</t>
+  </si>
+  <si>
+    <t>3213876</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213876 for AS order 20240816190252</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 58af0986-6542-4f02-84c5-faff2f9041c7","Using billTo: 58af0986-6542-4f02-84c5-faff2f9041c7","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213876 for AS order 20240816190252","version":"1.3.5-qa2.94","biId":"3213876"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e617a\"eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190252 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2023-09-12T15:00:14-05\" paymentDate: \"2023-09-12T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2023-09-12T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 900.00 appliedDiscount: 0.00 estimatedTax: 0.00 totalChargedAmount: 900.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f55866607\" title: \"Secrets of nature\" dhId: \"e0c4870c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"CAM448363\" jpcmsArticleIdentifier: \"CAM4.48363.ART\" articleDOI: \"10.1111/CAM4.48363\" } soldToDetails: { firstName: \"20240809175921Test\" lastName: \"20240809175921Auto\" email: \"20240809175921@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 900.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2024-08-16 08:00:00\" } billingAddress: { firstName: \"20240809175921Test\" lastName: \"20240809175921Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"No. 1 Xikang Road\"] addressLocality: \"Harbin\" addressRegion: \"100\" countryCode: \"CN\" postalCode: \"210024\" phoneNumber: \"0703503263\" email: \"20240809175921@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e617a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-08-16 19:02:52.820</t>
+  </si>
+  <si>
     <t>Trigger Proforma Order with Existing Customer</t>
   </si>
   <si>
@@ -851,6 +1039,26 @@
   </si>
   <si>
     <t>20240809181925@Wiley.com</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f51013723</t>
+  </si>
+  <si>
+    <t>3213880</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213880 for AS order 20240816190258</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 19d4ae48-402a-46e7-be58-753966fbec09","Using billTo: 19d4ae48-402a-46e7-be58-753966fbec09","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213880 for AS order 20240816190258","version":"1.3.5-qa2.94","biId":"3213880"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e705a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190258 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-08-16\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f51013723\" title: \"Secrets of nature\" dhId: \"e0c8024c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240809181925Test\" lastName: \"20240809181925Auto\" email: \"20240809181925@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240809181925Test\" lastName: \"20240809181925Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240809181925@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e705a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-08-16 19:02:58.389</t>
   </si>
 </sst>
 </file>
@@ -892,7 +1100,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -941,6 +1149,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -964,7 +1178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -981,12 +1195,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2009,14 +2225,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R18" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="79" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
@@ -2164,10 +2382,10 @@
         <v>175</v>
       </c>
       <c r="R2">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="S2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T2" t="s">
         <v>175</v>
@@ -2190,10 +2408,10 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E3" t="s">
         <v>173</v>
@@ -2202,25 +2420,25 @@
         <v>174</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H3" t="s">
         <v>175</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="N3" t="s">
         <v>175</v>
       </c>
-      <c r="R3">
-        <v>75</v>
-      </c>
-      <c r="S3">
-        <v>20</v>
+      <c r="R3" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="T3" t="s">
         <v>175</v>
@@ -2243,10 +2461,10 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E4" t="s">
         <v>173</v>
@@ -2255,25 +2473,25 @@
         <v>174</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H4" t="s">
         <v>175</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="M4" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="N4" t="s">
+        <v>175</v>
+      </c>
+      <c r="R4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S4" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="N4" t="s">
-        <v>175</v>
-      </c>
-      <c r="R4">
-        <v>75</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>175</v>
       </c>
       <c r="T4" t="s">
         <v>175</v>
@@ -2296,10 +2514,10 @@
         <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s">
         <v>173</v>
@@ -2308,16 +2526,16 @@
         <v>174</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="H5" t="s">
         <v>175</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="N5" t="s">
         <v>175</v>
@@ -2325,8 +2543,8 @@
       <c r="R5">
         <v>20</v>
       </c>
-      <c r="S5">
-        <v>90</v>
+      <c r="S5" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="T5" t="s">
         <v>175</v>
@@ -2349,25 +2567,25 @@
         <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E6" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>174</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="H6" t="s">
         <v>175</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>175</v>
@@ -2402,28 +2620,28 @@
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E7" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>174</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H7" t="s">
         <v>175</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="N7" t="s">
         <v>175</v>
@@ -2455,7 +2673,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>174</v>
@@ -2473,7 +2691,7 @@
         <v>175</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>175</v>
@@ -2481,8 +2699,8 @@
       <c r="N8" t="s">
         <v>175</v>
       </c>
-      <c r="R8">
-        <v>75</v>
+      <c r="R8" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="S8" s="11" t="s">
         <v>175</v>
@@ -2508,10 +2726,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>173</v>
@@ -2520,7 +2738,7 @@
         <v>174</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H9" t="s">
         <v>175</v>
@@ -2529,10 +2747,10 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="11" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="N9" t="s">
         <v>175</v>
@@ -2540,11 +2758,11 @@
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
-      <c r="R9" s="7">
-        <v>75</v>
-      </c>
-      <c r="S9" s="11" t="s">
-        <v>175</v>
+      <c r="R9" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="S9" s="15" t="s">
+        <v>185</v>
       </c>
       <c r="T9" t="s">
         <v>175</v>
@@ -2573,10 +2791,10 @@
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E10" t="s">
         <v>173</v>
@@ -2585,7 +2803,7 @@
         <v>174</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>23</v>
@@ -2594,25 +2812,25 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="N10" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
-      <c r="R10">
-        <v>75</v>
+      <c r="R10" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="S10">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="X10" s="11" t="s">
         <v>178</v>
@@ -2621,7 +2839,7 @@
         <v>178</v>
       </c>
       <c r="Z10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.35">
@@ -2632,16 +2850,16 @@
         <v>18</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E11" t="s">
         <v>173</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>23</v>
@@ -2650,10 +2868,10 @@
         <v>175</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="N11" s="11" t="s">
         <v>175</v>
@@ -2665,7 +2883,7 @@
         <v>50</v>
       </c>
       <c r="S11">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T11" s="11" t="s">
         <v>175</v>
@@ -2694,10 +2912,10 @@
         <v>18</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E12" t="s">
         <v>173</v>
@@ -2706,70 +2924,70 @@
         <v>174</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="H12" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="I12" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R12" s="11">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="S12">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="T12" s="11">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="U12" s="11">
         <v>50</v>
       </c>
       <c r="V12" s="11">
-        <v>5</v>
-      </c>
-      <c r="W12" s="11">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="W12" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="X12" s="11" t="s">
         <v>178</v>
       </c>
       <c r="Y12" s="11" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="Z12" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AA12" s="11" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AB12" s="11" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AC12" s="11" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.35">
@@ -2780,10 +2998,10 @@
         <v>18</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E13" t="s">
         <v>173</v>
@@ -2842,10 +3060,10 @@
         <v>18</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E14" t="s">
         <v>173</v>
@@ -2904,10 +3122,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E15" t="s">
         <v>173</v>
@@ -2924,7 +3142,7 @@
       <c r="L15" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="M15" s="12" t="s">
+      <c r="M15" s="16" t="s">
         <v>177</v>
       </c>
       <c r="N15" s="11" t="s">
@@ -2933,11 +3151,11 @@
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
-      <c r="R15">
-        <v>75</v>
+      <c r="R15" s="4">
+        <v>10</v>
       </c>
       <c r="S15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T15" s="11" t="s">
         <v>175</v>
@@ -2966,10 +3184,10 @@
         <v>18</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E16" t="s">
         <v>173</v>
@@ -2978,16 +3196,16 @@
         <v>174</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H16" t="s">
         <v>175</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="N16" s="11" t="s">
         <v>175</v>
@@ -2995,8 +3213,8 @@
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
-      <c r="R16">
-        <v>75</v>
+      <c r="R16" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="S16" t="s">
         <v>175</v>
@@ -3011,7 +3229,7 @@
         <v>178</v>
       </c>
       <c r="Y16" s="11" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="Z16" s="11" t="s">
         <v>175</v>
@@ -3025,10 +3243,10 @@
         <v>18</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E17" t="s">
         <v>173</v>
@@ -3046,10 +3264,10 @@
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="N17" s="11" t="s">
         <v>175</v>
@@ -3073,7 +3291,7 @@
         <v>178</v>
       </c>
       <c r="Y17" s="11" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="Z17" s="11" t="s">
         <v>175</v>
@@ -3087,10 +3305,10 @@
         <v>18</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E18" t="s">
         <v>173</v>
@@ -3101,10 +3319,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E19" t="s">
         <v>173</v>
@@ -3115,10 +3333,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D20" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E20" t="s">
         <v>173</v>
@@ -3129,10 +3347,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D21" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E21" t="s">
         <v>173</v>
@@ -3143,10 +3361,10 @@
         <v>18</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D22" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E22" t="s">
         <v>173</v>
@@ -3160,7 +3378,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>23</v>
@@ -3178,10 +3396,10 @@
         <v>175</v>
       </c>
       <c r="L23" t="s">
+        <v>177</v>
+      </c>
+      <c r="M23" t="s">
         <v>176</v>
-      </c>
-      <c r="M23" t="s">
-        <v>177</v>
       </c>
       <c r="N23" t="s">
         <v>175</v>
@@ -3213,7 +3431,7 @@
         <v>18</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>23</v>
@@ -3231,10 +3449,10 @@
         <v>175</v>
       </c>
       <c r="L24" t="s">
+        <v>177</v>
+      </c>
+      <c r="M24" t="s">
         <v>176</v>
-      </c>
-      <c r="M24" t="s">
-        <v>177</v>
       </c>
       <c r="N24" t="s">
         <v>175</v>
@@ -3259,17 +3477,17 @@
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="E25" s="13" t="s">
+      <c r="C25" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>173</v>
       </c>
       <c r="F25" t="s">
@@ -3285,10 +3503,10 @@
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="N25" s="11" t="s">
         <v>175</v>
@@ -3296,7 +3514,7 @@
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
-      <c r="R25" s="13">
+      <c r="R25" s="12">
         <v>75</v>
       </c>
       <c r="S25" s="11" t="s">
@@ -3312,7 +3530,7 @@
         <v>178</v>
       </c>
       <c r="Y25" s="11" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="Z25" s="11" t="s">
         <v>175</v>
@@ -3330,8 +3548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3360,10 +3578,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>11</v>
@@ -3390,7 +3608,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>48</v>
@@ -3420,7 +3638,7 @@
         <v>171</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3428,7 +3646,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -3437,16 +3655,16 @@
         <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F2" t="s">
         <v>173</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I2" t="s">
         <v>23</v>
@@ -3455,10 +3673,40 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>252</v>
+      </c>
+      <c r="N2" t="s">
+        <v>253</v>
+      </c>
+      <c r="O2" t="s">
+        <v>254</v>
+      </c>
+      <c r="P2" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>256</v>
+      </c>
+      <c r="R2" t="s">
+        <v>257</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="T2" t="s">
+        <v>258</v>
+      </c>
+      <c r="U2" t="s">
+        <v>259</v>
+      </c>
+      <c r="V2" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3466,10 +3714,10 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="C3" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -3478,25 +3726,55 @@
         <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="I3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="J3" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>254</v>
+        <v>266</v>
+      </c>
+      <c r="M3" t="s">
+        <v>267</v>
+      </c>
+      <c r="N3" t="s">
+        <v>268</v>
+      </c>
+      <c r="O3" t="s">
+        <v>269</v>
+      </c>
+      <c r="P3" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>271</v>
+      </c>
+      <c r="R3" t="s">
+        <v>272</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="T3" t="s">
+        <v>273</v>
+      </c>
+      <c r="U3" t="s">
+        <v>274</v>
+      </c>
+      <c r="V3" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
@@ -3504,7 +3782,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>276</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -3519,22 +3797,52 @@
         <v>173</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="I4" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="J4" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>254</v>
+        <v>266</v>
+      </c>
+      <c r="M4" t="s">
+        <v>278</v>
+      </c>
+      <c r="N4" t="s">
+        <v>279</v>
+      </c>
+      <c r="O4" t="s">
+        <v>280</v>
+      </c>
+      <c r="P4" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>282</v>
+      </c>
+      <c r="R4" t="s">
+        <v>283</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="T4" t="s">
+        <v>284</v>
+      </c>
+      <c r="U4" t="s">
+        <v>285</v>
+      </c>
+      <c r="V4" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3542,7 +3850,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>257</v>
+        <v>287</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -3551,16 +3859,16 @@
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>258</v>
+        <v>288</v>
       </c>
       <c r="F5" t="s">
-        <v>259</v>
+        <v>289</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I5" t="s">
         <v>23</v>
@@ -3569,10 +3877,40 @@
         <v>24</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>290</v>
+      </c>
+      <c r="N5" t="s">
+        <v>291</v>
+      </c>
+      <c r="O5" t="s">
+        <v>292</v>
+      </c>
+      <c r="P5" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>294</v>
+      </c>
+      <c r="R5" t="s">
+        <v>295</v>
+      </c>
+      <c r="S5" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="T5" t="s">
+        <v>296</v>
+      </c>
+      <c r="U5" t="s">
+        <v>297</v>
+      </c>
+      <c r="V5" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
@@ -3580,7 +3918,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
+        <v>299</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -3589,16 +3927,16 @@
         <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F6" t="s">
         <v>173</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I6" t="s">
         <v>23</v>
@@ -3607,19 +3945,40 @@
         <v>24</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="M6" t="s">
-        <v>261</v>
+        <v>300</v>
       </c>
       <c r="N6" t="s">
-        <v>262</v>
+        <v>301</v>
       </c>
       <c r="O6" t="s">
-        <v>263</v>
+        <v>302</v>
+      </c>
+      <c r="P6" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>304</v>
+      </c>
+      <c r="R6" t="s">
+        <v>305</v>
+      </c>
+      <c r="S6" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="T6" t="s">
+        <v>306</v>
+      </c>
+      <c r="U6" t="s">
+        <v>307</v>
+      </c>
+      <c r="V6" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
@@ -3627,10 +3986,10 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>264</v>
+        <v>309</v>
       </c>
       <c r="C7" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -3639,34 +3998,55 @@
         <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="I7" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="J7" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="M7" t="s">
-        <v>265</v>
+        <v>310</v>
       </c>
       <c r="N7" t="s">
-        <v>266</v>
+        <v>311</v>
       </c>
       <c r="O7" t="s">
-        <v>267</v>
+        <v>312</v>
+      </c>
+      <c r="P7" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>314</v>
+      </c>
+      <c r="R7" t="s">
+        <v>315</v>
+      </c>
+      <c r="S7" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="T7" t="s">
+        <v>316</v>
+      </c>
+      <c r="U7" t="s">
+        <v>317</v>
+      </c>
+      <c r="V7" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
@@ -3674,7 +4054,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>268</v>
+        <v>319</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -3689,31 +4069,52 @@
         <v>173</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="I8" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="J8" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="M8" t="s">
-        <v>269</v>
+        <v>320</v>
       </c>
       <c r="N8" t="s">
-        <v>270</v>
+        <v>321</v>
       </c>
       <c r="O8" t="s">
-        <v>271</v>
+        <v>322</v>
+      </c>
+      <c r="P8" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>324</v>
+      </c>
+      <c r="R8" t="s">
+        <v>325</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="T8" t="s">
+        <v>326</v>
+      </c>
+      <c r="U8" t="s">
+        <v>327</v>
+      </c>
+      <c r="V8" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
@@ -3721,7 +4122,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>272</v>
+        <v>329</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -3730,16 +4131,16 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>258</v>
+        <v>288</v>
       </c>
       <c r="F9" t="s">
-        <v>259</v>
+        <v>289</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I9" t="s">
         <v>23</v>
@@ -3748,19 +4149,40 @@
         <v>24</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="M9" t="s">
-        <v>273</v>
+        <v>330</v>
       </c>
       <c r="N9" t="s">
-        <v>274</v>
+        <v>331</v>
       </c>
       <c r="O9" t="s">
-        <v>275</v>
+        <v>332</v>
+      </c>
+      <c r="P9" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>334</v>
+      </c>
+      <c r="R9" t="s">
+        <v>335</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="T9" t="s">
+        <v>336</v>
+      </c>
+      <c r="U9" t="s">
+        <v>337</v>
+      </c>
+      <c r="V9" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI Validations added V.67
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_Inputs.xlsx
+++ b/UploadExcel/TD_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552E090F-B607-4516-BEFD-C974EBBAC1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39391CF6-2738-44D2-A8EA-10F9B40C25FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,14 @@
     <sheet name="OrderCreationCases" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">PriceProposal!$AF$1:$AF$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">PriceProposal!$AF$1:$AF$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="339">
   <si>
     <t>ExecutionEnvironment</t>
   </si>
@@ -550,78 +550,78 @@
     <t>c597beef-e45f-4cc7-b34c-0df812e2ef25</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>JCASP</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Create PP with Promotional discount</t>
+  </si>
+  <si>
+    <t>Promotional</t>
+  </si>
+  <si>
+    <t>WileyPromoCode</t>
+  </si>
+  <si>
+    <t>PROMO50</t>
+  </si>
+  <si>
+    <t>29.94</t>
+  </si>
+  <si>
+    <t>Create PP with Institutional discount</t>
+  </si>
+  <si>
+    <t>Institutional</t>
+  </si>
+  <si>
+    <t>E O Lawrence Berkeley National Laboratory</t>
+  </si>
+  <si>
+    <t>Create PP with Editorial discount</t>
+  </si>
+  <si>
+    <t>Editorial</t>
+  </si>
+  <si>
     <t>ArticleType</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>JCASP</t>
+    <t>EditorialDiscount</t>
+  </si>
+  <si>
+    <t>OPINION</t>
+  </si>
+  <si>
+    <t>CCCAM424</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Create PP with Referral discount</t>
+  </si>
+  <si>
+    <t>Referal</t>
+  </si>
+  <si>
+    <t>e1bbb7b4-5369-4c40-a53a-aa3dc55390a6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ReferralDiscount</t>
   </si>
   <si>
     <t>Research Article</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>Create PP with Promotional discount</t>
-  </si>
-  <si>
-    <t>Promotional</t>
-  </si>
-  <si>
-    <t>WileyPromoCode</t>
-  </si>
-  <si>
-    <t>PROMO50</t>
-  </si>
-  <si>
-    <t>29.94</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Create PP with Institutional discount</t>
-  </si>
-  <si>
-    <t>Institutional</t>
-  </si>
-  <si>
-    <t>E O Lawrence Berkeley National Laboratory</t>
-  </si>
-  <si>
-    <t>Create PP with Editorial discount</t>
-  </si>
-  <si>
-    <t>Editorial</t>
-  </si>
-  <si>
-    <t>EditorialDiscount</t>
-  </si>
-  <si>
-    <t>OPINION</t>
-  </si>
-  <si>
-    <t>CCCAM424</t>
-  </si>
-  <si>
-    <t>Create PP with Referral discount</t>
-  </si>
-  <si>
-    <t>Referal</t>
-  </si>
-  <si>
-    <t>e1bbb7b4-5369-4c40-a53a-aa3dc55390a6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ReferralDiscount</t>
-  </si>
-  <si>
     <t>Create PP with Geographical discount</t>
   </si>
   <si>
@@ -784,33 +784,33 @@
     <t>236.00</t>
   </si>
   <si>
-    <t>20240816190247Test</t>
-  </si>
-  <si>
-    <t>20240816190247Auto</t>
-  </si>
-  <si>
-    <t>20240816190247@Wiley.com</t>
-  </si>
-  <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f84775519</t>
-  </si>
-  <si>
-    <t>3213873</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213873 for AS order 20240816190247</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 9ca90171-81f4-4d1b-9528-8a34490d50be","Using soldTo : 9ca90171-81f4-4d1b-9528-8a34490d50be","Using billTo: 9ca90171-81f4-4d1b-9528-8a34490d50be","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213873 for AS order 20240816190247","version":"1.3.5-qa2.94","biId":"3213873"}}'}}}</t>
+    <t>20241004134254Test</t>
+  </si>
+  <si>
+    <t>20241004134254Auto</t>
+  </si>
+  <si>
+    <t>20241004134254@Wiley.com</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f25573132</t>
+  </si>
+  <si>
+    <t>3215589</t>
+  </si>
+  <si>
+    <t>Created Viax order 3215589 for AS order 20241004134254</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 20c3edf6-0eee-4dcd-8385-6f2b6d0c7e13","Using soldTo : 20c3edf6-0eee-4dcd-8385-6f2b6d0c7e13","Using billTo: 20c3edf6-0eee-4dcd-8385-6f2b6d0c7e13","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3215589 for AS order 20241004134254","version":"1.3.6-qa2.106","biId":"3215589"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2023-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190247 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f84775519\" title: \"Secrets of nature\" dhId: \"e0c4569c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"RRO39999\" jpcmsArticleIdentifier: \"RRO.39999.ART\" articleDOI: \"10.1111/RRO.39999\" } soldToDetails: { firstName: \"20240816190247Test\" lastName: \"20240816190247Auto\" email: \"20240816190247@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1180.00, billingAddress: { firstName: \"20240816190247Test\" lastName: \"20240816190247Auto\" streetAddress: [\"389 Nepean Hwy\"] addressLocality:\"Edison\" addressRegion: \"NJ\" countryCode: \"GB\" postalCode: \"08817\" phoneNumber: \"06667778888\" email: \"20240816190247@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e970a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2023-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20241004134254 submittedDate: \"2024-10-04T15:00:14-05\" createdDate: \"2024-10-04T15:00:14-05\" cancelDate: \"2024-10-04T15:00:14-05\" paymentDate: \"2024-10-04T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-10-04T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f25573132\" title: \"Secrets of nature\" dhId: \"e0c2798c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"RRO39999\" jpcmsArticleIdentifier: \"RRO.39999.ART\" articleDOI: \"10.1111/RRO.39999\" } soldToDetails: { firstName: \"20241004134254Test\" lastName: \"20241004134254Auto\" email: \"20241004134254@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1180.00, billingAddress: { firstName: \"20241004134254Test\" lastName: \"20241004134254Auto\" streetAddress: [\"389 Nepean Hwy\"] addressLocality:\"Edison\" addressRegion: \"NJ\" countryCode: \"GB\" postalCode: \"08817\" phoneNumber: \"06667778888\" email: \"20241004134254@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e970a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-08-16 19:02:47.871</t>
+    <t>2024-10-04 13:42:54.336</t>
   </si>
   <si>
     <t>Trigger CreditCard Order with New Customer</t>
@@ -831,33 +831,33 @@
     <t>0.00</t>
   </si>
   <si>
-    <t>20240816190249Test</t>
-  </si>
-  <si>
-    <t>20240816190249Auto</t>
-  </si>
-  <si>
-    <t>20240816190249@Wiley.com</t>
-  </si>
-  <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f82547776</t>
-  </si>
-  <si>
-    <t>3213874</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213874 for AS order 20240816190249</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP db7230bc-e352-4a3c-a64b-56d3a5bf268c","Using soldTo : db7230bc-e352-4a3c-a64b-56d3a5bf268c","Using billTo: db7230bc-e352-4a3c-a64b-56d3a5bf268c","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213874 for AS order 20240816190249","version":"1.3.5-qa2.94","biId":"3213874"}}'}}}</t>
+    <t>20241004134255Test</t>
+  </si>
+  <si>
+    <t>20241004134255Auto</t>
+  </si>
+  <si>
+    <t>20241004134255@Wiley.com</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f97612983</t>
+  </si>
+  <si>
+    <t>3215590</t>
+  </si>
+  <si>
+    <t>Created Viax order 3215590 for AS order 20241004134256</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 636b66bb-9d51-4013-9e00-175e39c018a2","Using soldTo : 636b66bb-9d51-4013-9e00-175e39c018a2","Using billTo: 636b66bb-9d51-4013-9e00-175e39c018a2","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3215590 for AS order 20241004134256","version":"1.3.6-qa2.106","biId":"3215590"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e527a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2024-08-16T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190249 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2023-01-26T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CH CC order form validation\" apc: 2300.25 appliedDiscount: 0.00 discountType: \"Institutional\" estimatedTax: 0.00 totalChargedAmount: 2300.25 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CH\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f82547776\" title: \"Secrets of volcano\" dhId: \"e0c3220c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240816190249Test\" lastName: \"20240816190249Auto\" email: \"20240816190249@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 2300.25 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2023-07-03T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240816190249Test\" lastName:\"20240816190249Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"Dufourstrasse 40a\"] addressLocality: \"St. Gallen\" addressRegion: \"SG\" countryCode: \"CH\" postalCode: \"9000\" phoneNumber: \"8299729725\" email: \"20240816190249@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e527a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e897a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2024-10-04T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20241004134256 submittedDate: \"2024-10-04T15:00:14-05\" createdDate: \"2024-10-04T15:00:14-05\" cancelDate: \"2024-10-04T15:00:14-05\" paymentDate: \"2024-10-04T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2023-01-26T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CH CC order form validation\" apc: 2300.25 appliedDiscount: 0.00 discountType: \"Institutional\" estimatedTax: 0.00 totalChargedAmount: 2300.25 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CH\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f97612983\" title: \"Secrets of volcano\" dhId: \"e0c7784c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20241004134255Test\" lastName: \"20241004134255Auto\" email: \"20241004134255@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 2300.25 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2023-07-03T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20241004134255Test\" lastName:\"20241004134255Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"Dufourstrasse 40a\"] addressLocality: \"St. Gallen\" addressRegion: \"SG\" countryCode: \"CH\" postalCode: \"9000\" phoneNumber: \"8299729725\" email: \"20241004134255@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e897a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-08-16 19:02:49.665</t>
+    <t>2024-10-04 13:42:55.969</t>
   </si>
   <si>
     <t>Trigger Alipay Order with New Customer</t>
@@ -866,33 +866,33 @@
     <t>900.00</t>
   </si>
   <si>
-    <t>20240816190251Test</t>
-  </si>
-  <si>
-    <t>20240816190251Auto</t>
-  </si>
-  <si>
-    <t>20240816190251@Wiley.com</t>
-  </si>
-  <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f51045539</t>
-  </si>
-  <si>
-    <t>3213875</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213875 for AS order 20240816190251</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP c56044fa-84e5-4134-b919-d954b8524a7e","Using soldTo : c56044fa-84e5-4134-b919-d954b8524a7e","Using billTo: c56044fa-84e5-4134-b919-d954b8524a7e","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213875 for AS order 20240816190251","version":"1.3.5-qa2.94","biId":"3213875"}}'}}}</t>
+    <t>20241004134257Test</t>
+  </si>
+  <si>
+    <t>20241004134257Auto</t>
+  </si>
+  <si>
+    <t>20241004134257@Wiley.com</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f62655957</t>
+  </si>
+  <si>
+    <t>3215591</t>
+  </si>
+  <si>
+    <t>Created Viax order 3215591 for AS order 20241004134257</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP e7b62cc9-7e19-40b3-a0ef-d32af218c321","Using soldTo : e7b62cc9-7e19-40b3-a0ef-d32af218c321","Using billTo: e7b62cc9-7e19-40b3-a0ef-d32af218c321","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3215591 for AS order 20241004134257","version":"1.3.6-qa2.106","biId":"3215591"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e873a\"eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190251 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2023-09-12T15:00:14-05\" paymentDate: \"2023-09-12T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2023-09-12T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 900.00 appliedDiscount: 0.00 estimatedTax: 0.00 totalChargedAmount: 900.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f51045539\" title: \"Secrets of nature\" dhId: \"e0c1151c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"CAM448363\" jpcmsArticleIdentifier: \"CAM4.48363.ART\" articleDOI: \"10.1111/CAM4.48363\" } soldToDetails: { firstName: \"20240816190251Test\" lastName: \"20240816190251Auto\" email: \"20240816190251@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 900.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2024-08-16 08:00:00\" } billingAddress: { firstName: \"20240816190251Test\" lastName: \"20240816190251Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"No. 1 Xikang Road\"] addressLocality: \"Harbin\" addressRegion: \"100\" countryCode: \"CN\" postalCode: \"210024\" phoneNumber: \"0703503263\" email: \"20240816190251@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e873a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e601a\"eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20241004134257 submittedDate: \"2024-10-04T15:00:14-05\" createdDate: \"2024-10-04T15:00:14-05\" cancelDate: \"2023-09-12T15:00:14-05\" paymentDate: \"2023-09-12T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2023-09-12T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 900.00 appliedDiscount: 0.00 estimatedTax: 0.00 totalChargedAmount: 900.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f62655957\" title: \"Secrets of nature\" dhId: \"e0c3945c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"CAM448363\" jpcmsArticleIdentifier: \"CAM4.48363.ART\" articleDOI: \"10.1111/CAM4.48363\" } soldToDetails: { firstName: \"20241004134257Test\" lastName: \"20241004134257Auto\" email: \"20241004134257@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 900.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2024-10-04 08:00:00\" } billingAddress: { firstName: \"20241004134257Test\" lastName: \"20241004134257Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"No. 1 Xikang Road\"] addressLocality: \"Harbin\" addressRegion: \"100\" countryCode: \"CN\" postalCode: \"210024\" phoneNumber: \"0703503263\" email: \"20241004134257@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e601a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-08-16 19:02:51.200</t>
+    <t>2024-10-04 13:42:57.449</t>
   </si>
   <si>
     <t>Trigger Proforma Order with New Customer</t>
@@ -904,33 +904,33 @@
     <t>1b28a8b9-067b-4ce9-b981-e8eabe16e0a7</t>
   </si>
   <si>
-    <t>20240816190256Test</t>
-  </si>
-  <si>
-    <t>20240816190256Auto</t>
-  </si>
-  <si>
-    <t>20240816190256@Wiley.com</t>
-  </si>
-  <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f27834654</t>
-  </si>
-  <si>
-    <t>3213879</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213879 for AS order 20240816190256</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP db9caa52-3038-4d87-8158-9f847e8c63d4","Using soldTo : db9caa52-3038-4d87-8158-9f847e8c63d4","Using billTo: db9caa52-3038-4d87-8158-9f847e8c63d4","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213879 for AS order 20240816190256","version":"1.3.5-qa2.94","biId":"3213879"}}'}}}</t>
+    <t>20241004134302Test</t>
+  </si>
+  <si>
+    <t>20241004134302Auto</t>
+  </si>
+  <si>
+    <t>20241004134302@Wiley.com</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f99608686</t>
+  </si>
+  <si>
+    <t>3215595</t>
+  </si>
+  <si>
+    <t>Created Viax order 3215595 for AS order 20241004134302</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP f7e40e60-f196-4b7f-b24c-671a66e0a7fe","Using soldTo : f7e40e60-f196-4b7f-b24c-671a66e0a7fe","Using billTo: f7e40e60-f196-4b7f-b24c-671a66e0a7fe","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3215595 for AS order 20241004134302","version":"1.3.6-qa2.106","biId":"3215595"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e366a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190256 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-08-16\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f27834654\" title: \"Secrets of nature\" dhId: \"e0c3582c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240816190256Test\" lastName: \"20240816190256Auto\" email: \"20240816190256@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240816190256Test\" lastName: \"20240816190256Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240816190256@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e366a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e855a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20241004134302 submittedDate: \"2024-10-04T15:00:14-05\" createdDate: \"2024-10-04T15:00:14-05\" cancelDate: \"2024-10-04T15:00:14-05\" paymentDate: \"2024-10-04T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-10-04T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-04\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f99608686\" title: \"Secrets of nature\" dhId: \"e0c6600c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20241004134302Test\" lastName: \"20241004134302Auto\" email: \"20241004134302@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20241004134302Test\" lastName: \"20241004134302Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20241004134302@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e855a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-08-16 19:02:56.916</t>
+    <t>2024-10-04 13:43:02.824</t>
   </si>
   <si>
     <t>Trigger Invoice Order with Existing Customer</t>
@@ -945,24 +945,24 @@
     <t>20240809175918@Wiley.com</t>
   </si>
   <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f62879150</t>
-  </si>
-  <si>
-    <t>3213878</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213878 for AS order 20240816190255</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 3f7431cb-eef3-49fa-bdfc-5d16128c6fd5","Using billTo: 3f7431cb-eef3-49fa-bdfc-5d16128c6fd5","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213878 for AS order 20240816190255","version":"1.3.5-qa2.94","biId":"3213878"}}'}}}</t>
+    <t>11ca99f1-8a00-4cb3-123e-222f88182685</t>
+  </si>
+  <si>
+    <t>3215594</t>
+  </si>
+  <si>
+    <t>Created Viax order 3215594 for AS order 20241004134301</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 3f7431cb-eef3-49fa-bdfc-5d16128c6fd5","Using billTo: 3f7431cb-eef3-49fa-bdfc-5d16128c6fd5","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3215594 for AS order 20241004134301","version":"1.3.6-qa2.106","biId":"3215594"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e572a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2023-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190255 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f62879150\" title: \"Secrets of nature\" dhId: \"e0c7856c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"RRO39999\" jpcmsArticleIdentifier: \"RRO.39999.ART\" articleDOI: \"10.1111/RRO.39999\" } soldToDetails: { firstName: \"20240809175918Test\" lastName: \"20240809175918Auto\" email: \"20240809175918@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1180.00, billingAddress: { firstName: \"20240809175918Test\" lastName: \"20240809175918Auto\" streetAddress: [\"389 Nepean Hwy\"] addressLocality:\"Edison\" addressRegion: \"NJ\" countryCode: \"GB\" postalCode: \"08817\" phoneNumber: \"06667778888\" email: \"20240809175918@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e572a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e832a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2023-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20241004134301 submittedDate: \"2024-10-04T15:00:14-05\" createdDate: \"2024-10-04T15:00:14-05\" cancelDate: \"2024-10-04T15:00:14-05\" paymentDate: \"2024-10-04T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-10-04T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f88182685\" title: \"Secrets of nature\" dhId: \"e0c5773c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"RRO39999\" jpcmsArticleIdentifier: \"RRO.39999.ART\" articleDOI: \"10.1111/RRO.39999\" } soldToDetails: { firstName: \"20240809175918Test\" lastName: \"20240809175918Auto\" email: \"20240809175918@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1180.00, billingAddress: { firstName: \"20240809175918Test\" lastName: \"20240809175918Auto\" streetAddress: [\"389 Nepean Hwy\"] addressLocality:\"Edison\" addressRegion: \"NJ\" countryCode: \"GB\" postalCode: \"08817\" phoneNumber: \"06667778888\" email: \"20240809175918@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e832a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-08-16 19:02:55.481</t>
+    <t>2024-10-04 13:43:01.561</t>
   </si>
   <si>
     <t>Trigger CreditCard Order with Existing Customer</t>
@@ -977,24 +977,24 @@
     <t>20240809175920@Wiley.com</t>
   </si>
   <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f16859253</t>
-  </si>
-  <si>
-    <t>3213877</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213877 for AS order 20240816190254</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 9be953a5-d4ea-4149-a439-801fe3371d6a","Using billTo: 9be953a5-d4ea-4149-a439-801fe3371d6a","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213877 for AS order 20240816190254","version":"1.3.5-qa2.94","biId":"3213877"}}'}}}</t>
+    <t>11ca99f1-8a00-4cb3-123e-222f65242131</t>
+  </si>
+  <si>
+    <t>3215593</t>
+  </si>
+  <si>
+    <t>Created Viax order 3215593 for AS order 20241004134300</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 9be953a5-d4ea-4149-a439-801fe3371d6a","Using billTo: 9be953a5-d4ea-4149-a439-801fe3371d6a","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3215593 for AS order 20241004134300","version":"1.3.6-qa2.106","biId":"3215593"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e832a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2024-08-16T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190254 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2023-01-26T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CH CC order form validation\" apc: 2300.25 appliedDiscount: 0.00 discountType: \"Institutional\" estimatedTax: 0.00 totalChargedAmount: 2300.25 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CH\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f16859253\" title: \"Secrets of volcano\" dhId: \"e0c3651c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240809175920Test\" lastName: \"20240809175920Auto\" email: \"20240809175920@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 2300.25 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2023-07-03T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240809175920Test\" lastName:\"20240809175920Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"Dufourstrasse 40a\"] addressLocality: \"St. Gallen\" addressRegion: \"SG\" countryCode: \"CH\" postalCode: \"9000\" phoneNumber: \"8299729725\" email: \"20240809175920@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e832a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e599a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2024-10-04T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20241004134300 submittedDate: \"2024-10-04T15:00:14-05\" createdDate: \"2024-10-04T15:00:14-05\" cancelDate: \"2024-10-04T15:00:14-05\" paymentDate: \"2024-10-04T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2023-01-26T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CH CC order form validation\" apc: 2300.25 appliedDiscount: 0.00 discountType: \"Institutional\" estimatedTax: 0.00 totalChargedAmount: 2300.25 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CH\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f65242131\" title: \"Secrets of volcano\" dhId: \"e0c8543c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240809175920Test\" lastName: \"20240809175920Auto\" email: \"20240809175920@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 2300.25 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2023-07-03T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240809175920Test\" lastName:\"20240809175920Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"Dufourstrasse 40a\"] addressLocality: \"St. Gallen\" addressRegion: \"SG\" countryCode: \"CH\" postalCode: \"9000\" phoneNumber: \"8299729725\" email: \"20240809175920@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e599a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-08-16 19:02:54.193</t>
+    <t>2024-10-04 13:43:00.180</t>
   </si>
   <si>
     <t>Trigger Alipay Order with Existing Customer</t>
@@ -1009,24 +1009,24 @@
     <t>20240809175921@Wiley.com</t>
   </si>
   <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f55866607</t>
-  </si>
-  <si>
-    <t>3213876</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213876 for AS order 20240816190252</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 58af0986-6542-4f02-84c5-faff2f9041c7","Using billTo: 58af0986-6542-4f02-84c5-faff2f9041c7","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213876 for AS order 20240816190252","version":"1.3.5-qa2.94","biId":"3213876"}}'}}}</t>
+    <t>11ca99f1-8a00-4cb3-123e-222f19770451</t>
+  </si>
+  <si>
+    <t>3215592</t>
+  </si>
+  <si>
+    <t>Created Viax order 3215592 for AS order 20241004134258</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 58af0986-6542-4f02-84c5-faff2f9041c7","Using billTo: 58af0986-6542-4f02-84c5-faff2f9041c7","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3215592 for AS order 20241004134258","version":"1.3.6-qa2.106","biId":"3215592"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e617a\"eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190252 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2023-09-12T15:00:14-05\" paymentDate: \"2023-09-12T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2023-09-12T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 900.00 appliedDiscount: 0.00 estimatedTax: 0.00 totalChargedAmount: 900.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f55866607\" title: \"Secrets of nature\" dhId: \"e0c4870c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"CAM448363\" jpcmsArticleIdentifier: \"CAM4.48363.ART\" articleDOI: \"10.1111/CAM4.48363\" } soldToDetails: { firstName: \"20240809175921Test\" lastName: \"20240809175921Auto\" email: \"20240809175921@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 900.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2024-08-16 08:00:00\" } billingAddress: { firstName: \"20240809175921Test\" lastName: \"20240809175921Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"No. 1 Xikang Road\"] addressLocality: \"Harbin\" addressRegion: \"100\" countryCode: \"CN\" postalCode: \"210024\" phoneNumber: \"0703503263\" email: \"20240809175921@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e617a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e719a\"eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20241004134258 submittedDate: \"2024-10-04T15:00:14-05\" createdDate: \"2024-10-04T15:00:14-05\" cancelDate: \"2023-09-12T15:00:14-05\" paymentDate: \"2023-09-12T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2023-09-12T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 900.00 appliedDiscount: 0.00 estimatedTax: 0.00 totalChargedAmount: 900.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f19770451\" title: \"Secrets of nature\" dhId: \"e0c6187c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"CAM448363\" jpcmsArticleIdentifier: \"CAM4.48363.ART\" articleDOI: \"10.1111/CAM4.48363\" } soldToDetails: { firstName: \"20240809175921Test\" lastName: \"20240809175921Auto\" email: \"20240809175921@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 900.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2024-10-04 08:00:00\" } billingAddress: { firstName: \"20240809175921Test\" lastName: \"20240809175921Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"No. 1 Xikang Road\"] addressLocality: \"Harbin\" addressRegion: \"100\" countryCode: \"CN\" postalCode: \"210024\" phoneNumber: \"0703503263\" email: \"20240809175921@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e719a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-08-16 19:02:52.820</t>
+    <t>2024-10-04 13:42:58.874</t>
   </si>
   <si>
     <t>Trigger Proforma Order with Existing Customer</t>
@@ -1041,31 +1041,31 @@
     <t>20240809181925@Wiley.com</t>
   </si>
   <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f51013723</t>
-  </si>
-  <si>
-    <t>3213880</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213880 for AS order 20240816190258</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 19d4ae48-402a-46e7-be58-753966fbec09","Using billTo: 19d4ae48-402a-46e7-be58-753966fbec09","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213880 for AS order 20240816190258","version":"1.3.5-qa2.94","biId":"3213880"}}'}}}</t>
+    <t>11ca99f1-8a00-4cb3-123e-222f27789398</t>
+  </si>
+  <si>
+    <t>3215596</t>
+  </si>
+  <si>
+    <t>Created Viax order 3215596 for AS order 20241004134304</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 19d4ae48-402a-46e7-be58-753966fbec09","Using billTo: 19d4ae48-402a-46e7-be58-753966fbec09","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3215596 for AS order 20241004134304","version":"1.3.6-qa2.106","biId":"3215596"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e705a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190258 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-08-16\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f51013723\" title: \"Secrets of nature\" dhId: \"e0c8024c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240809181925Test\" lastName: \"20240809181925Auto\" email: \"20240809181925@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240809181925Test\" lastName: \"20240809181925Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240809181925@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e705a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e240a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20241004134304 submittedDate: \"2024-10-04T15:00:14-05\" createdDate: \"2024-10-04T15:00:14-05\" cancelDate: \"2024-10-04T15:00:14-05\" paymentDate: \"2024-10-04T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-10-04T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-04\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f27789398\" title: \"Secrets of nature\" dhId: \"e0c5259c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240809181925Test\" lastName: \"20240809181925Auto\" email: \"20240809181925@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240809181925Test\" lastName: \"20240809181925Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240809181925@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e240a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-08-16 19:02:58.389</t>
+    <t>2024-10-04 13:43:04.208</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1097,6 +1097,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1178,7 +1183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1199,11 +1204,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2225,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AF11" sqref="AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2235,6 +2244,7 @@
     <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.1796875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
@@ -2364,40 +2374,38 @@
         <v>173</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G2" s="11" t="s">
         <v>23</v>
       </c>
+      <c r="G2" s="11"/>
       <c r="H2" t="s">
+        <v>174</v>
+      </c>
+      <c r="L2" t="s">
         <v>175</v>
       </c>
-      <c r="L2" t="s">
-        <v>176</v>
-      </c>
       <c r="M2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R2">
         <v>10</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
@@ -2408,49 +2416,45 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
         <v>173</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" t="s">
+        <v>174</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="H3" t="s">
-        <v>175</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="N3" t="s">
-        <v>175</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="S3" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="T3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X3" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
@@ -2461,49 +2465,45 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E4" t="s">
         <v>173</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>187</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="G4" s="11"/>
       <c r="H4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>177</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="M4" s="11"/>
       <c r="N4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R4" t="s">
-        <v>175</v>
-      </c>
-      <c r="S4" s="15" t="s">
-        <v>185</v>
+        <v>174</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>174</v>
       </c>
       <c r="T4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X4" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
@@ -2514,49 +2514,49 @@
         <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E5" t="s">
         <v>173</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="G5" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="M5" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="H5" t="s">
-        <v>175</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>193</v>
-      </c>
       <c r="N5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R5">
         <v>20</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="T5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X5" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y5" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">
@@ -2567,31 +2567,31 @@
         <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" t="s">
         <v>195</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" t="s">
+        <v>174</v>
+      </c>
+      <c r="L6" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="H6" t="s">
-        <v>175</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>177</v>
-      </c>
       <c r="M6" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R6">
         <v>10</v>
@@ -2600,16 +2600,16 @@
         <v>15.25</v>
       </c>
       <c r="T6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X6" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y6" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.35">
@@ -2629,22 +2629,22 @@
         <v>200</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>201</v>
       </c>
       <c r="H7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="M7" s="11" t="s">
         <v>202</v>
       </c>
       <c r="N7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R7">
         <v>30</v>
@@ -2653,16 +2653,16 @@
         <v>100</v>
       </c>
       <c r="T7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X7" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.35">
@@ -2676,169 +2676,165 @@
         <v>203</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E8" t="s">
         <v>173</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>204</v>
       </c>
       <c r="M8" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="N8" t="s">
+        <v>174</v>
+      </c>
+      <c r="R8" s="4">
+        <v>75</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="T8" t="s">
+        <v>174</v>
+      </c>
+      <c r="X8" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y8" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="M9" s="18"/>
+      <c r="N9" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="S9" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="T9" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y9" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z9" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+    </row>
+    <row r="10" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="M10" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N10" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="R8" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="S8" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="T8" t="s">
-        <v>175</v>
-      </c>
-      <c r="X8" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y8" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="H9" t="s">
-        <v>175</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="N9" t="s">
-        <v>175</v>
-      </c>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="S9" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="T9" t="s">
-        <v>175</v>
-      </c>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y9" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>175</v>
-      </c>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="E10" t="s">
-        <v>173</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G10" s="11" t="s">
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="N10" s="11" t="s">
+      <c r="S10" s="20">
+        <v>10</v>
+      </c>
+      <c r="T10" s="17">
+        <v>10</v>
+      </c>
+      <c r="X10" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>10</v>
-      </c>
-      <c r="X10" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y10" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="Z10" t="s">
+      <c r="Y10" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z10" s="17" t="s">
         <v>209</v>
       </c>
     </row>
@@ -2865,7 +2861,7 @@
         <v>23</v>
       </c>
       <c r="H11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L11" s="11" t="s">
         <v>212</v>
@@ -2874,7 +2870,7 @@
         <v>213</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
@@ -2886,107 +2882,105 @@
         <v>20</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U11" s="11"/>
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
       <c r="X11" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y11" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z11" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AA11" s="11"/>
       <c r="AB11" s="11"/>
       <c r="AC11" s="11"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G12" s="11" t="s">
+      <c r="F12" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="M12" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="H12" t="s">
-        <v>201</v>
-      </c>
-      <c r="I12" t="s">
-        <v>216</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="11" t="s">
+      <c r="N12" s="18"/>
+      <c r="P12" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q12" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="R12" s="18">
+        <v>50</v>
+      </c>
+      <c r="S12" s="17">
+        <v>0</v>
+      </c>
+      <c r="T12" s="18">
+        <v>50</v>
+      </c>
+      <c r="U12" s="18">
+        <v>10</v>
+      </c>
+      <c r="V12" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="L12" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="P12" s="11" t="s">
+      <c r="W12" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="X12" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="Q12" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="R12" s="11">
-        <v>50</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12" s="11">
-        <v>0</v>
-      </c>
-      <c r="U12" s="11">
-        <v>50</v>
-      </c>
-      <c r="V12" s="11">
-        <v>10</v>
-      </c>
-      <c r="W12" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="X12" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y12" s="11" t="s">
+      <c r="Y12" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="Z12" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="AA12" s="11" t="s">
+      <c r="AA12" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="AB12" s="11" t="s">
+      <c r="AB12" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="AC12" s="11" t="s">
+      <c r="AC12" s="18" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3007,46 +3001,46 @@
         <v>173</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U13" s="11"/>
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
       <c r="X13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Z13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AA13" s="11"/>
       <c r="AB13" s="11"/>
@@ -3069,49 +3063,49 @@
         <v>173</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U14" s="11"/>
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
       <c r="X14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Z14" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AA14" s="11"/>
       <c r="AB14" s="11"/>
@@ -3131,22 +3125,22 @@
         <v>173</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>174</v>
+        <v>23</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H15" t="s">
+        <v>174</v>
+      </c>
+      <c r="L15" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="L15" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="M15" s="16" t="s">
-        <v>177</v>
+      <c r="M15" s="15" t="s">
+        <v>175</v>
       </c>
       <c r="N15" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
@@ -3158,85 +3152,85 @@
         <v>0</v>
       </c>
       <c r="T15" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y15" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z15" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AA15" s="11"/>
       <c r="AB15" s="11"/>
       <c r="AC15" s="11"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="16" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="H16" t="s">
-        <v>175</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="M16" s="11" t="s">
+      <c r="F16" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L16" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="N16" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="S16" t="s">
-        <v>175</v>
-      </c>
-      <c r="T16" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y16" s="11" t="s">
+      <c r="M16" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="N16" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="S16" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="T16" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y16" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="Z16" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
+      <c r="Z16" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
@@ -3252,25 +3246,25 @@
         <v>173</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="M17" s="11" t="s">
         <v>229</v>
       </c>
       <c r="N17" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
@@ -3279,22 +3273,22 @@
         <v>75</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T17" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
       <c r="X17" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y17" s="11" t="s">
         <v>209</v>
       </c>
       <c r="Z17" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AA17" s="11"/>
       <c r="AB17" s="11"/>
@@ -3387,22 +3381,22 @@
         <v>173</v>
       </c>
       <c r="F23" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="G23" t="s">
         <v>23</v>
       </c>
       <c r="H23" t="s">
+        <v>174</v>
+      </c>
+      <c r="L23" t="s">
+        <v>197</v>
+      </c>
+      <c r="M23" t="s">
         <v>175</v>
       </c>
-      <c r="L23" t="s">
-        <v>177</v>
-      </c>
-      <c r="M23" t="s">
-        <v>176</v>
-      </c>
       <c r="N23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R23">
         <v>75</v>
@@ -3411,16 +3405,16 @@
         <v>5</v>
       </c>
       <c r="T23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.35">
@@ -3440,22 +3434,22 @@
         <v>173</v>
       </c>
       <c r="F24" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="G24" t="s">
         <v>23</v>
       </c>
       <c r="H24" t="s">
+        <v>174</v>
+      </c>
+      <c r="L24" t="s">
+        <v>197</v>
+      </c>
+      <c r="M24" t="s">
         <v>175</v>
       </c>
-      <c r="L24" t="s">
-        <v>177</v>
-      </c>
-      <c r="M24" t="s">
-        <v>176</v>
-      </c>
       <c r="N24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R24">
         <v>75</v>
@@ -3464,16 +3458,16 @@
         <v>5</v>
       </c>
       <c r="T24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Z24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.35">
@@ -3491,25 +3485,25 @@
         <v>173</v>
       </c>
       <c r="F25" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="G25" t="s">
         <v>23</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="M25" s="11" t="s">
         <v>229</v>
       </c>
       <c r="N25" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
@@ -3518,28 +3512,29 @@
         <v>75</v>
       </c>
       <c r="S25" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T25" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U25" s="11"/>
       <c r="V25" s="11"/>
       <c r="W25" s="11"/>
       <c r="X25" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y25" s="11" t="s">
         <v>209</v>
       </c>
       <c r="Z25" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AA25" s="11"/>
       <c r="AB25" s="11"/>
       <c r="AC25" s="11"/>
     </row>
   </sheetData>
+  <autoFilter ref="AF1:AF25" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3696,8 +3691,8 @@
       <c r="R2" t="s">
         <v>257</v>
       </c>
-      <c r="S2" s="14" t="s">
-        <v>179</v>
+      <c r="S2" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="T2" t="s">
         <v>258</v>
@@ -3735,7 +3730,7 @@
         <v>264</v>
       </c>
       <c r="I3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J3" t="s">
         <v>265</v>
@@ -3764,8 +3759,8 @@
       <c r="R3" t="s">
         <v>272</v>
       </c>
-      <c r="S3" s="14" t="s">
-        <v>179</v>
+      <c r="S3" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="T3" t="s">
         <v>273</v>
@@ -3832,8 +3827,8 @@
       <c r="R4" t="s">
         <v>283</v>
       </c>
-      <c r="S4" s="14" t="s">
-        <v>179</v>
+      <c r="S4" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="T4" t="s">
         <v>284</v>
@@ -3900,8 +3895,8 @@
       <c r="R5" t="s">
         <v>295</v>
       </c>
-      <c r="S5" s="14" t="s">
-        <v>179</v>
+      <c r="S5" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="T5" t="s">
         <v>296</v>
@@ -3968,8 +3963,8 @@
       <c r="R6" t="s">
         <v>305</v>
       </c>
-      <c r="S6" s="14" t="s">
-        <v>179</v>
+      <c r="S6" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="T6" t="s">
         <v>306</v>
@@ -4007,7 +4002,7 @@
         <v>264</v>
       </c>
       <c r="I7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J7" t="s">
         <v>265</v>
@@ -4036,8 +4031,8 @@
       <c r="R7" t="s">
         <v>315</v>
       </c>
-      <c r="S7" s="14" t="s">
-        <v>179</v>
+      <c r="S7" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="T7" t="s">
         <v>316</v>
@@ -4104,8 +4099,8 @@
       <c r="R8" t="s">
         <v>325</v>
       </c>
-      <c r="S8" s="14" t="s">
-        <v>179</v>
+      <c r="S8" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="T8" t="s">
         <v>326</v>
@@ -4172,8 +4167,8 @@
       <c r="R9" t="s">
         <v>335</v>
       </c>
-      <c r="S9" s="14" t="s">
-        <v>179</v>
+      <c r="S9" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="T9" t="s">
         <v>336</v>

</xml_diff>

<commit_message>
UI Validations added V.72
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_Inputs.xlsx
+++ b/UploadExcel/TD_Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39391CF6-2738-44D2-A8EA-10F9B40C25FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425670FE-3FB3-4A8B-A40C-09ED62BEA831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -604,9 +604,6 @@
     <t>CCCAM424</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>Create PP with Referral discount</t>
   </si>
   <si>
@@ -1059,6 +1056,9 @@
   </si>
   <si>
     <t>2024-10-04 13:43:04.208</t>
+  </si>
+  <si>
+    <t>90</t>
   </si>
 </sst>
 </file>
@@ -2234,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AF11" sqref="AF11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2544,7 +2544,7 @@
         <v>20</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>192</v>
+        <v>338</v>
       </c>
       <c r="T5" t="s">
         <v>174</v>
@@ -2567,25 +2567,25 @@
         <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" t="s">
         <v>194</v>
-      </c>
-      <c r="E6" t="s">
-        <v>195</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>188</v>
       </c>
       <c r="G6" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="H6" t="s">
+        <v>174</v>
+      </c>
+      <c r="L6" s="11" t="s">
         <v>196</v>
-      </c>
-      <c r="H6" t="s">
-        <v>174</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>197</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>174</v>
@@ -2620,28 +2620,28 @@
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" t="s">
         <v>199</v>
-      </c>
-      <c r="E7" t="s">
-        <v>200</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>188</v>
       </c>
       <c r="G7" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="H7" t="s">
+        <v>174</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="M7" s="11" t="s">
         <v>201</v>
-      </c>
-      <c r="H7" t="s">
-        <v>174</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>202</v>
       </c>
       <c r="N7" t="s">
         <v>174</v>
@@ -2673,7 +2673,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>188</v>
@@ -2691,7 +2691,7 @@
         <v>174</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>174</v>
@@ -2726,10 +2726,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>173</v>
@@ -2787,10 +2787,10 @@
         <v>18</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>208</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>173</v>
@@ -2835,7 +2835,7 @@
         <v>176</v>
       </c>
       <c r="Z10" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.35">
@@ -2846,16 +2846,16 @@
         <v>18</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="E11" t="s">
         <v>173</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>23</v>
@@ -2864,10 +2864,10 @@
         <v>174</v>
       </c>
       <c r="L11" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="M11" s="11" t="s">
         <v>212</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>213</v>
       </c>
       <c r="N11" s="11" t="s">
         <v>174</v>
@@ -2908,25 +2908,25 @@
         <v>18</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>173</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G12" s="18" t="s">
         <v>189</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>23</v>
@@ -2935,10 +2935,10 @@
         <v>180</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="N12" s="18"/>
       <c r="P12" s="18" t="s">
@@ -2948,10 +2948,10 @@
         <v>181</v>
       </c>
       <c r="R12" s="18">
+        <v>90</v>
+      </c>
+      <c r="S12" s="17">
         <v>50</v>
-      </c>
-      <c r="S12" s="17">
-        <v>0</v>
       </c>
       <c r="T12" s="18">
         <v>50</v>
@@ -2969,19 +2969,19 @@
         <v>176</v>
       </c>
       <c r="Y12" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z12" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AA12" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB12" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AC12" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.35">
@@ -2992,10 +2992,10 @@
         <v>18</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>219</v>
       </c>
       <c r="E13" t="s">
         <v>173</v>
@@ -3054,10 +3054,10 @@
         <v>18</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="E14" t="s">
         <v>173</v>
@@ -3116,10 +3116,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>223</v>
       </c>
       <c r="E15" t="s">
         <v>173</v>
@@ -3178,10 +3178,10 @@
         <v>18</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>225</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>173</v>
@@ -3196,10 +3196,10 @@
         <v>174</v>
       </c>
       <c r="L16" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M16" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N16" s="18" t="s">
         <v>174</v>
@@ -3223,7 +3223,7 @@
         <v>176</v>
       </c>
       <c r="Y16" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z16" s="18" t="s">
         <v>174</v>
@@ -3237,10 +3237,10 @@
         <v>18</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>227</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>228</v>
       </c>
       <c r="E17" t="s">
         <v>173</v>
@@ -3258,10 +3258,10 @@
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N17" s="11" t="s">
         <v>174</v>
@@ -3285,7 +3285,7 @@
         <v>176</v>
       </c>
       <c r="Y17" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z17" s="11" t="s">
         <v>174</v>
@@ -3299,10 +3299,10 @@
         <v>18</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="E18" t="s">
         <v>173</v>
@@ -3313,10 +3313,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
+        <v>231</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>233</v>
       </c>
       <c r="E19" t="s">
         <v>173</v>
@@ -3327,10 +3327,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D20" t="s">
         <v>234</v>
-      </c>
-      <c r="D20" t="s">
-        <v>235</v>
       </c>
       <c r="E20" t="s">
         <v>173</v>
@@ -3341,10 +3341,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D21" t="s">
         <v>236</v>
-      </c>
-      <c r="D21" t="s">
-        <v>237</v>
       </c>
       <c r="E21" t="s">
         <v>173</v>
@@ -3355,10 +3355,10 @@
         <v>18</v>
       </c>
       <c r="C22" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D22" t="s">
         <v>238</v>
-      </c>
-      <c r="D22" t="s">
-        <v>239</v>
       </c>
       <c r="E22" t="s">
         <v>173</v>
@@ -3372,7 +3372,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>23</v>
@@ -3390,7 +3390,7 @@
         <v>174</v>
       </c>
       <c r="L23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M23" t="s">
         <v>175</v>
@@ -3425,7 +3425,7 @@
         <v>18</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>23</v>
@@ -3443,7 +3443,7 @@
         <v>174</v>
       </c>
       <c r="L24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M24" t="s">
         <v>175</v>
@@ -3476,10 +3476,10 @@
         <v>18</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>173</v>
@@ -3497,10 +3497,10 @@
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N25" s="11" t="s">
         <v>174</v>
@@ -3524,7 +3524,7 @@
         <v>176</v>
       </c>
       <c r="Y25" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z25" s="11" t="s">
         <v>174</v>
@@ -3573,10 +3573,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>244</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>11</v>
@@ -3603,7 +3603,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>48</v>
@@ -3633,7 +3633,7 @@
         <v>171</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3641,7 +3641,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -3650,16 +3650,16 @@
         <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F2" t="s">
         <v>173</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="I2" t="s">
         <v>23</v>
@@ -3668,40 +3668,40 @@
         <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="M2" t="s">
+        <v>251</v>
+      </c>
+      <c r="N2" t="s">
         <v>252</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>253</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>254</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>255</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>256</v>
-      </c>
-      <c r="R2" t="s">
-        <v>257</v>
       </c>
       <c r="S2" s="16" t="s">
         <v>177</v>
       </c>
       <c r="T2" t="s">
+        <v>257</v>
+      </c>
+      <c r="U2" t="s">
         <v>258</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>259</v>
-      </c>
-      <c r="V2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3709,10 +3709,10 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" t="s">
         <v>261</v>
-      </c>
-      <c r="C3" t="s">
-        <v>262</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -3721,55 +3721,55 @@
         <v>35</v>
       </c>
       <c r="F3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>264</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I3" t="s">
         <v>184</v>
       </c>
       <c r="J3" t="s">
+        <v>264</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="M3" t="s">
         <v>266</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>267</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>268</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>269</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>270</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>271</v>
-      </c>
-      <c r="R3" t="s">
-        <v>272</v>
       </c>
       <c r="S3" s="16" t="s">
         <v>177</v>
       </c>
       <c r="T3" t="s">
+        <v>272</v>
+      </c>
+      <c r="U3" t="s">
         <v>273</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>274</v>
-      </c>
-      <c r="V3" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
@@ -3777,7 +3777,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -3792,52 +3792,52 @@
         <v>173</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="I4" t="s">
+        <v>264</v>
+      </c>
+      <c r="J4" t="s">
+        <v>264</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="M4" t="s">
         <v>277</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="I4" t="s">
-        <v>265</v>
-      </c>
-      <c r="J4" t="s">
-        <v>265</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>278</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>279</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>280</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>281</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>282</v>
-      </c>
-      <c r="R4" t="s">
-        <v>283</v>
       </c>
       <c r="S4" s="16" t="s">
         <v>177</v>
       </c>
       <c r="T4" t="s">
+        <v>283</v>
+      </c>
+      <c r="U4" t="s">
         <v>284</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>285</v>
-      </c>
-      <c r="V4" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3845,7 +3845,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -3854,16 +3854,16 @@
         <v>27</v>
       </c>
       <c r="E5" t="s">
+        <v>287</v>
+      </c>
+      <c r="F5" t="s">
         <v>288</v>
       </c>
-      <c r="F5" t="s">
-        <v>289</v>
-      </c>
       <c r="G5" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="I5" t="s">
         <v>23</v>
@@ -3872,40 +3872,40 @@
         <v>24</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="M5" t="s">
+        <v>289</v>
+      </c>
+      <c r="N5" t="s">
         <v>290</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>291</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>292</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>293</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>294</v>
-      </c>
-      <c r="R5" t="s">
-        <v>295</v>
       </c>
       <c r="S5" s="16" t="s">
         <v>177</v>
       </c>
       <c r="T5" t="s">
+        <v>295</v>
+      </c>
+      <c r="U5" t="s">
         <v>296</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>297</v>
-      </c>
-      <c r="V5" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
@@ -3913,7 +3913,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -3922,16 +3922,16 @@
         <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F6" t="s">
         <v>173</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="I6" t="s">
         <v>23</v>
@@ -3940,40 +3940,40 @@
         <v>24</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="M6" t="s">
+        <v>299</v>
+      </c>
+      <c r="N6" t="s">
         <v>300</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>301</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>302</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>303</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>304</v>
-      </c>
-      <c r="R6" t="s">
-        <v>305</v>
       </c>
       <c r="S6" s="16" t="s">
         <v>177</v>
       </c>
       <c r="T6" t="s">
+        <v>305</v>
+      </c>
+      <c r="U6" t="s">
         <v>306</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>307</v>
-      </c>
-      <c r="V6" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
@@ -3981,10 +3981,10 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -3993,55 +3993,55 @@
         <v>35</v>
       </c>
       <c r="F7" t="s">
+        <v>262</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>264</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I7" t="s">
         <v>184</v>
       </c>
       <c r="J7" t="s">
+        <v>264</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>266</v>
-      </c>
       <c r="L7" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M7" t="s">
+        <v>309</v>
+      </c>
+      <c r="N7" t="s">
         <v>310</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>311</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>312</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>313</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>314</v>
-      </c>
-      <c r="R7" t="s">
-        <v>315</v>
       </c>
       <c r="S7" s="16" t="s">
         <v>177</v>
       </c>
       <c r="T7" t="s">
+        <v>315</v>
+      </c>
+      <c r="U7" t="s">
         <v>316</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>317</v>
-      </c>
-      <c r="V7" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
@@ -4049,7 +4049,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -4064,52 +4064,52 @@
         <v>173</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I8" t="s">
+        <v>264</v>
+      </c>
+      <c r="J8" t="s">
+        <v>264</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>266</v>
-      </c>
       <c r="M8" t="s">
+        <v>319</v>
+      </c>
+      <c r="N8" t="s">
         <v>320</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>321</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>322</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>323</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>324</v>
-      </c>
-      <c r="R8" t="s">
-        <v>325</v>
       </c>
       <c r="S8" s="16" t="s">
         <v>177</v>
       </c>
       <c r="T8" t="s">
+        <v>325</v>
+      </c>
+      <c r="U8" t="s">
         <v>326</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>327</v>
-      </c>
-      <c r="V8" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
@@ -4117,7 +4117,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -4126,16 +4126,16 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
+        <v>287</v>
+      </c>
+      <c r="F9" t="s">
         <v>288</v>
       </c>
-      <c r="F9" t="s">
-        <v>289</v>
-      </c>
       <c r="G9" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="I9" t="s">
         <v>23</v>
@@ -4144,40 +4144,40 @@
         <v>24</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="M9" t="s">
+        <v>329</v>
+      </c>
+      <c r="N9" t="s">
         <v>330</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>331</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>332</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>333</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>334</v>
-      </c>
-      <c r="R9" t="s">
-        <v>335</v>
       </c>
       <c r="S9" s="16" t="s">
         <v>177</v>
       </c>
       <c r="T9" t="s">
+        <v>335</v>
+      </c>
+      <c r="U9" t="s">
         <v>336</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>337</v>
-      </c>
-      <c r="V9" t="s">
-        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>